<commit_message>
Kreole Map Work, Added a Few Weapons
</commit_message>
<xml_diff>
--- a/Weapons and Armor.xlsx
+++ b/Weapons and Armor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="12435" windowHeight="7740" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="12435" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="118">
   <si>
     <t>Reminiscence Weapons and Armor</t>
   </si>
@@ -353,6 +353,32 @@
   </si>
   <si>
     <t>Increases TP regeneration rate by +4</t>
+  </si>
+  <si>
+    <t>Basics of Attack</t>
+  </si>
+  <si>
+    <t>Beginner's Defense</t>
+  </si>
+  <si>
+    <t>Strategy over Brawn</t>
+  </si>
+  <si>
+    <t>Sometimes Luck Helps</t>
+  </si>
+  <si>
+    <t>Staff of Lightning</t>
+  </si>
+  <si>
+    <t>Thunder Element
+Enables "Thunder of the Gods" skill</t>
+  </si>
+  <si>
+    <t>Staff of Ice</t>
+  </si>
+  <si>
+    <t>Ice Element
+Enables "Eternal Winter" skill</t>
   </si>
 </sst>
 </file>
@@ -840,7 +866,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -866,11 +892,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1208,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV68"/>
+  <dimension ref="A1:AV116"/>
   <sheetViews>
-    <sheetView topLeftCell="AE2" workbookViewId="0">
-      <selection activeCell="AT16" sqref="AT16"/>
+    <sheetView tabSelected="1" topLeftCell="S38" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AI66" sqref="AI66:AL68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,13 +1250,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:48" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
@@ -1242,17 +1268,17 @@
       <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="82"/>
+      <c r="B4" s="81"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
     </row>
     <row r="5" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -2355,10 +2381,10 @@
       </c>
     </row>
     <row r="16" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="81"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -2518,37 +2544,37 @@
       <c r="AV17" s="71"/>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="J18" s="81"/>
+      <c r="J18" s="72"/>
       <c r="K18" s="73"/>
       <c r="L18" s="73"/>
       <c r="M18" s="74"/>
-      <c r="O18" s="81"/>
+      <c r="O18" s="72"/>
       <c r="P18" s="73"/>
       <c r="Q18" s="73"/>
       <c r="R18" s="74"/>
-      <c r="T18" s="81"/>
+      <c r="T18" s="72"/>
       <c r="U18" s="73"/>
       <c r="V18" s="73"/>
       <c r="W18" s="74"/>
-      <c r="Y18" s="81"/>
+      <c r="Y18" s="72"/>
       <c r="Z18" s="73"/>
       <c r="AA18" s="73"/>
       <c r="AB18" s="74"/>
-      <c r="AD18" s="81"/>
+      <c r="AD18" s="72"/>
       <c r="AE18" s="73"/>
       <c r="AF18" s="73"/>
       <c r="AG18" s="74"/>
-      <c r="AI18" s="81"/>
+      <c r="AI18" s="72"/>
       <c r="AJ18" s="73"/>
       <c r="AK18" s="73"/>
       <c r="AL18" s="74"/>
-      <c r="AN18" s="72" t="s">
+      <c r="AN18" s="82" t="s">
         <v>105</v>
       </c>
       <c r="AO18" s="73"/>
       <c r="AP18" s="73"/>
       <c r="AQ18" s="74"/>
-      <c r="AS18" s="81"/>
+      <c r="AS18" s="72"/>
       <c r="AT18" s="73"/>
       <c r="AU18" s="73"/>
       <c r="AV18" s="74"/>
@@ -2561,7 +2587,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="13">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="J19" s="75"/>
       <c r="K19" s="76"/>
@@ -2605,7 +2631,7 @@
       </c>
       <c r="C20" s="53">
         <f t="shared" ref="C20:C27" si="0">C7+($C$19-1)*(D7-C7)/98</f>
-        <v>7000</v>
+        <v>565</v>
       </c>
       <c r="J20" s="78"/>
       <c r="K20" s="79"/>
@@ -2649,7 +2675,7 @@
       </c>
       <c r="C21" s="53">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>121.07142857142857</v>
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.25">
@@ -2661,7 +2687,7 @@
       </c>
       <c r="C22" s="4">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>35.357142857142861</v>
       </c>
       <c r="J22" s="70" t="s">
         <v>52</v>
@@ -2709,7 +2735,7 @@
       </c>
       <c r="C23" s="4">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>35.357142857142861</v>
       </c>
       <c r="J23" s="54" t="s">
         <v>22</v>
@@ -2769,7 +2795,7 @@
       </c>
       <c r="C24" s="53">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>35.357142857142861</v>
       </c>
       <c r="J24" s="54" t="s">
         <v>32</v>
@@ -2829,7 +2855,7 @@
       </c>
       <c r="C25" s="53">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>35.357142857142861</v>
       </c>
       <c r="J25" s="54" t="s">
         <v>47</v>
@@ -2919,7 +2945,7 @@
       </c>
       <c r="C26" s="4">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>47.142857142857139</v>
       </c>
       <c r="J26" s="54" t="s">
         <v>48</v>
@@ -3009,7 +3035,7 @@
       </c>
       <c r="C27" s="4">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>47.142857142857139</v>
       </c>
       <c r="J27" s="54" t="s">
         <v>41</v>
@@ -3529,31 +3555,31 @@
       <c r="AL33" s="71"/>
     </row>
     <row r="34" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J34" s="72" t="s">
+      <c r="J34" s="82" t="s">
         <v>53</v>
       </c>
       <c r="K34" s="73"/>
       <c r="L34" s="73"/>
       <c r="M34" s="74"/>
-      <c r="O34" s="81"/>
+      <c r="O34" s="72"/>
       <c r="P34" s="73"/>
       <c r="Q34" s="73"/>
       <c r="R34" s="74"/>
-      <c r="T34" s="81" t="s">
+      <c r="T34" s="72" t="s">
         <v>63</v>
       </c>
       <c r="U34" s="73"/>
       <c r="V34" s="73"/>
       <c r="W34" s="74"/>
-      <c r="Y34" s="81"/>
+      <c r="Y34" s="72"/>
       <c r="Z34" s="73"/>
       <c r="AA34" s="73"/>
       <c r="AB34" s="74"/>
-      <c r="AD34" s="81"/>
+      <c r="AD34" s="72"/>
       <c r="AE34" s="73"/>
       <c r="AF34" s="73"/>
       <c r="AG34" s="74"/>
-      <c r="AI34" s="81"/>
+      <c r="AI34" s="72"/>
       <c r="AJ34" s="73"/>
       <c r="AK34" s="73"/>
       <c r="AL34" s="74"/>
@@ -3623,6 +3649,12 @@
       <c r="U38" s="70"/>
       <c r="V38" s="70"/>
       <c r="W38" s="70"/>
+      <c r="AI38" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ38" s="70"/>
+      <c r="AK38" s="70"/>
+      <c r="AL38" s="70"/>
     </row>
     <row r="39" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O39" s="54" t="s">
@@ -3641,6 +3673,14 @@
       </c>
       <c r="V39" s="55"/>
       <c r="W39" s="55"/>
+      <c r="AI39" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ39" s="62">
+        <v>10</v>
+      </c>
+      <c r="AK39" s="55"/>
+      <c r="AL39" s="55"/>
     </row>
     <row r="40" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O40" s="54" t="s">
@@ -3659,6 +3699,14 @@
       </c>
       <c r="V40" s="55"/>
       <c r="W40" s="55"/>
+      <c r="AI40" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ40" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK40" s="55"/>
+      <c r="AL40" s="55"/>
     </row>
     <row r="41" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O41" s="54" t="s">
@@ -3687,6 +3735,19 @@
         <f>ROUND(U41*($C$7+(U39-1)*($D$7-$C$7)/98),0)</f>
         <v>0</v>
       </c>
+      <c r="AI41" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ41" s="63">
+        <v>0</v>
+      </c>
+      <c r="AK41" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL41" s="65">
+        <f>ROUND(AJ41*($C$7+(AJ39-1)*($D$7-$C$7)/98),0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O42" s="54" t="s">
@@ -3715,6 +3776,19 @@
         <f>ROUND(U42*($C$8+(U39-1)*($D$8-$C$8)/98),0)</f>
         <v>0</v>
       </c>
+      <c r="AI42" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ42" s="63">
+        <v>0</v>
+      </c>
+      <c r="AK42" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL42" s="65">
+        <f>ROUND(AJ42*($C$8+(AJ39-1)*($D$8-$C$8)/98),0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O43" s="54" t="s">
@@ -3743,6 +3817,19 @@
         <f>ROUND(U43*($C$9+(U39-1)*($D$9-$C$9)/98),0)</f>
         <v>13</v>
       </c>
+      <c r="AI43" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ43" s="63">
+        <v>0.35</v>
+      </c>
+      <c r="AK43" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL43" s="65">
+        <f>ROUND(AJ43*($C$9+(AJ39-1)*($D$9-$C$9)/98),0)</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="44" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O44" s="54" t="s">
@@ -3771,6 +3858,19 @@
         <f>ROUND(U44*($C$10+(U39-1)*($D$10-$C$10)/98),0)</f>
         <v>0</v>
       </c>
+      <c r="AI44" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ44" s="63">
+        <v>0</v>
+      </c>
+      <c r="AK44" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL44" s="65">
+        <f>ROUND(AJ44*($C$10+(AJ39-1)*($D$10-$C$10)/98),0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O45" s="54" t="s">
@@ -3799,6 +3899,19 @@
         <f>ROUND(U45*($C$11+(U39-1)*($D$11-$C$11)/98),0)</f>
         <v>3</v>
       </c>
+      <c r="AI45" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ45" s="63">
+        <v>0.7</v>
+      </c>
+      <c r="AK45" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL45" s="65">
+        <f>ROUND(AJ45*($C$11+(AJ39-1)*($D$11-$C$11)/98),0)</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="46" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O46" s="54" t="s">
@@ -3827,6 +3940,19 @@
         <f>ROUND(U46*($C$12+(U39-1)*($D$12-$C$12)/98),0)</f>
         <v>0</v>
       </c>
+      <c r="AI46" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ46" s="63">
+        <v>0</v>
+      </c>
+      <c r="AK46" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL46" s="65">
+        <f>ROUND(AJ46*($C$12+(AJ39-1)*($D$12-$C$12)/98),0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O47" s="54" t="s">
@@ -3855,6 +3981,19 @@
         <f>ROUND(U47*($C$13+(U39-1)*($D$13-$C$13)/98),0)</f>
         <v>0</v>
       </c>
+      <c r="AI47" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ47" s="63">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL47" s="65">
+        <f>ROUND(AJ47*($C$13+(AJ39-1)*($D$13-$C$13)/98),0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O48" s="56" t="s">
@@ -3883,8 +4022,21 @@
         <f>ROUND(U48*($C$14+(U39-1)*($D$14-$C$14)/98),0)</f>
         <v>-3</v>
       </c>
-    </row>
-    <row r="49" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="AI48" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ48" s="64">
+        <v>0</v>
+      </c>
+      <c r="AK48" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL48" s="65">
+        <f>ROUND(AJ48*($C$14+(AJ39-1)*($D$14-$C$14)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O49" s="71" t="s">
         <v>51</v>
       </c>
@@ -3897,20 +4049,32 @@
       <c r="U49" s="71"/>
       <c r="V49" s="71"/>
       <c r="W49" s="71"/>
-    </row>
-    <row r="50" spans="15:23" x14ac:dyDescent="0.25">
-      <c r="O50" s="81"/>
+      <c r="AI49" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ49" s="71"/>
+      <c r="AK49" s="71"/>
+      <c r="AL49" s="71"/>
+    </row>
+    <row r="50" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="O50" s="72"/>
       <c r="P50" s="73"/>
       <c r="Q50" s="73"/>
       <c r="R50" s="74"/>
-      <c r="T50" s="81" t="s">
+      <c r="T50" s="72" t="s">
         <v>63</v>
       </c>
       <c r="U50" s="73"/>
       <c r="V50" s="73"/>
       <c r="W50" s="74"/>
-    </row>
-    <row r="51" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="AI50" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ50" s="73"/>
+      <c r="AK50" s="73"/>
+      <c r="AL50" s="74"/>
+    </row>
+    <row r="51" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O51" s="75"/>
       <c r="P51" s="76"/>
       <c r="Q51" s="76"/>
@@ -3919,8 +4083,12 @@
       <c r="U51" s="76"/>
       <c r="V51" s="76"/>
       <c r="W51" s="77"/>
-    </row>
-    <row r="52" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="AI51" s="75"/>
+      <c r="AJ51" s="76"/>
+      <c r="AK51" s="76"/>
+      <c r="AL51" s="77"/>
+    </row>
+    <row r="52" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O52" s="78"/>
       <c r="P52" s="79"/>
       <c r="Q52" s="79"/>
@@ -3929,16 +4097,32 @@
       <c r="U52" s="79"/>
       <c r="V52" s="79"/>
       <c r="W52" s="80"/>
-    </row>
-    <row r="54" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="AI52" s="78"/>
+      <c r="AJ52" s="79"/>
+      <c r="AK52" s="79"/>
+      <c r="AL52" s="80"/>
+    </row>
+    <row r="54" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O54" s="70" t="s">
         <v>59</v>
       </c>
       <c r="P54" s="70"/>
       <c r="Q54" s="70"/>
       <c r="R54" s="70"/>
-    </row>
-    <row r="55" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="T54" s="70" t="s">
+        <v>110</v>
+      </c>
+      <c r="U54" s="70"/>
+      <c r="V54" s="70"/>
+      <c r="W54" s="70"/>
+      <c r="AI54" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ54" s="70"/>
+      <c r="AK54" s="70"/>
+      <c r="AL54" s="70"/>
+    </row>
+    <row r="55" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O55" s="54" t="s">
         <v>22</v>
       </c>
@@ -3947,8 +4131,24 @@
       </c>
       <c r="Q55" s="55"/>
       <c r="R55" s="55"/>
-    </row>
-    <row r="56" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="T55" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="U55" s="62">
+        <v>8</v>
+      </c>
+      <c r="V55" s="55"/>
+      <c r="W55" s="55"/>
+      <c r="AI55" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ55" s="62">
+        <v>10</v>
+      </c>
+      <c r="AK55" s="55"/>
+      <c r="AL55" s="55"/>
+    </row>
+    <row r="56" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O56" s="54" t="s">
         <v>32</v>
       </c>
@@ -3957,8 +4157,24 @@
       </c>
       <c r="Q56" s="55"/>
       <c r="R56" s="55"/>
-    </row>
-    <row r="57" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="T56" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="U56" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="V56" s="55"/>
+      <c r="W56" s="55"/>
+      <c r="AI56" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ56" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK56" s="55"/>
+      <c r="AL56" s="55"/>
+    </row>
+    <row r="57" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O57" s="54" t="s">
         <v>47</v>
       </c>
@@ -3972,8 +4188,34 @@
         <f>ROUND(P57*($C$7+(P55-1)*($D$7-$C$7)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="T57" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="U57" s="63">
+        <v>0</v>
+      </c>
+      <c r="V57" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="W57" s="65">
+        <f>ROUND(U57*($C$7+(U55-1)*($D$7-$C$7)/98),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI57" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ57" s="63">
+        <v>0</v>
+      </c>
+      <c r="AK57" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL57" s="65">
+        <f>ROUND(AJ57*($C$7+(AJ55-1)*($D$7-$C$7)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O58" s="54" t="s">
         <v>48</v>
       </c>
@@ -3987,8 +4229,34 @@
         <f>ROUND(P58*($C$8+(P55-1)*($D$8-$C$8)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="T58" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="U58" s="63">
+        <v>0</v>
+      </c>
+      <c r="V58" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="W58" s="65">
+        <f>ROUND(U58*($C$8+(U55-1)*($D$8-$C$8)/98),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI58" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ58" s="63">
+        <v>0</v>
+      </c>
+      <c r="AK58" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL58" s="65">
+        <f>ROUND(AJ58*($C$8+(AJ55-1)*($D$8-$C$8)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O59" s="54" t="s">
         <v>41</v>
       </c>
@@ -4002,8 +4270,34 @@
         <f>ROUND(P59*($C$9+(P55-1)*($D$9-$C$9)/98),0)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="60" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="T59" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="U59" s="63">
+        <v>0.6</v>
+      </c>
+      <c r="V59" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="W59" s="65">
+        <f>ROUND(U59*($C$9+(U55-1)*($D$9-$C$9)/98),0)</f>
+        <v>21</v>
+      </c>
+      <c r="AI59" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ59" s="63">
+        <v>0.36</v>
+      </c>
+      <c r="AK59" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL59" s="65">
+        <f>ROUND(AJ59*($C$9+(AJ55-1)*($D$9-$C$9)/98),0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O60" s="54" t="s">
         <v>42</v>
       </c>
@@ -4017,8 +4311,34 @@
         <f>ROUND(P60*($C$10+(P55-1)*($D$10-$C$10)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="T60" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="U60" s="63">
+        <v>-0.2</v>
+      </c>
+      <c r="V60" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="W60" s="65">
+        <f>ROUND(U60*($C$10+(U55-1)*($D$10-$C$10)/98),0)</f>
+        <v>-7</v>
+      </c>
+      <c r="AI60" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ60" s="63">
+        <v>0.1</v>
+      </c>
+      <c r="AK60" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL60" s="65">
+        <f>ROUND(AJ60*($C$10+(AJ55-1)*($D$10-$C$10)/98),0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O61" s="54" t="s">
         <v>43</v>
       </c>
@@ -4032,8 +4352,34 @@
         <f>ROUND(P61*($C$11+(P55-1)*($D$11-$C$11)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="T61" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="U61" s="63">
+        <v>0</v>
+      </c>
+      <c r="V61" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="W61" s="65">
+        <f>ROUND(U61*($C$11+(U55-1)*($D$11-$C$11)/98),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI61" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ61" s="63">
+        <v>0.6</v>
+      </c>
+      <c r="AK61" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL61" s="65">
+        <f>ROUND(AJ61*($C$11+(AJ55-1)*($D$11-$C$11)/98),0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O62" s="54" t="s">
         <v>44</v>
       </c>
@@ -4047,8 +4393,34 @@
         <f>ROUND(P62*($C$12+(P55-1)*($D$12-$C$12)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="T62" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="U62" s="63">
+        <v>0</v>
+      </c>
+      <c r="V62" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="W62" s="65">
+        <f>ROUND(U62*($C$12+(U55-1)*($D$12-$C$12)/98),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI62" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ62" s="63">
+        <v>0</v>
+      </c>
+      <c r="AK62" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL62" s="65">
+        <f>ROUND(AJ62*($C$12+(AJ55-1)*($D$12-$C$12)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O63" s="54" t="s">
         <v>45</v>
       </c>
@@ -4062,8 +4434,34 @@
         <f>ROUND(P63*($C$13+(P55-1)*($D$13-$C$13)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="T63" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="U63" s="63">
+        <v>0</v>
+      </c>
+      <c r="V63" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="W63" s="65">
+        <f>ROUND(U63*($C$13+(U55-1)*($D$13-$C$13)/98),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI63" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ63" s="63">
+        <v>0</v>
+      </c>
+      <c r="AK63" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL63" s="65">
+        <f>ROUND(AJ63*($C$13+(AJ55-1)*($D$13-$C$13)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O64" s="56" t="s">
         <v>46</v>
       </c>
@@ -4077,37 +4475,678 @@
         <f>ROUND(P64*($C$14+(P55-1)*($D$14-$C$14)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="T64" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="U64" s="64">
+        <v>0</v>
+      </c>
+      <c r="V64" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="W64" s="65">
+        <f>ROUND(U64*($C$14+(U55-1)*($D$14-$C$14)/98),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI64" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ64" s="64">
+        <v>0</v>
+      </c>
+      <c r="AK64" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL64" s="65">
+        <f>ROUND(AJ64*($C$14+(AJ55-1)*($D$14-$C$14)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O65" s="71" t="s">
         <v>51</v>
       </c>
       <c r="P65" s="71"/>
       <c r="Q65" s="71"/>
       <c r="R65" s="71"/>
-    </row>
-    <row r="66" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O66" s="72" t="s">
+      <c r="T65" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="U65" s="71"/>
+      <c r="V65" s="71"/>
+      <c r="W65" s="71"/>
+      <c r="AI65" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ65" s="71"/>
+      <c r="AK65" s="71"/>
+      <c r="AL65" s="71"/>
+    </row>
+    <row r="66" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="O66" s="82" t="s">
         <v>89</v>
       </c>
       <c r="P66" s="73"/>
       <c r="Q66" s="73"/>
       <c r="R66" s="74"/>
-    </row>
-    <row r="67" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="T66" s="72"/>
+      <c r="U66" s="73"/>
+      <c r="V66" s="73"/>
+      <c r="W66" s="74"/>
+      <c r="AI66" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ66" s="73"/>
+      <c r="AK66" s="73"/>
+      <c r="AL66" s="74"/>
+    </row>
+    <row r="67" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O67" s="75"/>
       <c r="P67" s="76"/>
       <c r="Q67" s="76"/>
       <c r="R67" s="77"/>
-    </row>
-    <row r="68" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="T67" s="75"/>
+      <c r="U67" s="76"/>
+      <c r="V67" s="76"/>
+      <c r="W67" s="77"/>
+      <c r="AI67" s="75"/>
+      <c r="AJ67" s="76"/>
+      <c r="AK67" s="76"/>
+      <c r="AL67" s="77"/>
+    </row>
+    <row r="68" spans="15:38" x14ac:dyDescent="0.25">
       <c r="O68" s="78"/>
       <c r="P68" s="79"/>
       <c r="Q68" s="79"/>
       <c r="R68" s="80"/>
+      <c r="T68" s="78"/>
+      <c r="U68" s="79"/>
+      <c r="V68" s="79"/>
+      <c r="W68" s="80"/>
+      <c r="AI68" s="78"/>
+      <c r="AJ68" s="79"/>
+      <c r="AK68" s="79"/>
+      <c r="AL68" s="80"/>
+    </row>
+    <row r="70" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T70" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="U70" s="70"/>
+      <c r="V70" s="70"/>
+      <c r="W70" s="70"/>
+    </row>
+    <row r="71" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T71" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="U71" s="62">
+        <v>8</v>
+      </c>
+      <c r="V71" s="55"/>
+      <c r="W71" s="55"/>
+    </row>
+    <row r="72" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T72" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="U72" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="V72" s="55"/>
+      <c r="W72" s="55"/>
+    </row>
+    <row r="73" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T73" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="U73" s="63">
+        <v>0</v>
+      </c>
+      <c r="V73" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="W73" s="65">
+        <f>ROUND(U73*($C$7+(U71-1)*($D$7-$C$7)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T74" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="U74" s="63">
+        <v>0</v>
+      </c>
+      <c r="V74" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="W74" s="65">
+        <f>ROUND(U74*($C$8+(U71-1)*($D$8-$C$8)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T75" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="U75" s="63">
+        <v>-0.2</v>
+      </c>
+      <c r="V75" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="W75" s="65">
+        <f>ROUND(U75*($C$9+(U71-1)*($D$9-$C$9)/98),0)</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="76" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T76" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="U76" s="63">
+        <v>0.6</v>
+      </c>
+      <c r="V76" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="W76" s="65">
+        <f>ROUND(U76*($C$10+(U71-1)*($D$10-$C$10)/98),0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T77" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="U77" s="63">
+        <v>-0.2</v>
+      </c>
+      <c r="V77" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="W77" s="65">
+        <f>ROUND(U77*($C$11+(U71-1)*($D$11-$C$11)/98),0)</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="78" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T78" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="U78" s="63">
+        <v>0.6</v>
+      </c>
+      <c r="V78" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="W78" s="65">
+        <f>ROUND(U78*($C$12+(U71-1)*($D$12-$C$12)/98),0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T79" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="U79" s="63">
+        <v>0</v>
+      </c>
+      <c r="V79" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="W79" s="65">
+        <f>ROUND(U79*($C$13+(U71-1)*($D$13-$C$13)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="15:38" x14ac:dyDescent="0.25">
+      <c r="T80" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="U80" s="64">
+        <v>0</v>
+      </c>
+      <c r="V80" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="W80" s="65">
+        <f>ROUND(U80*($C$14+(U71-1)*($D$14-$C$14)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T81" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="U81" s="71"/>
+      <c r="V81" s="71"/>
+      <c r="W81" s="71"/>
+    </row>
+    <row r="82" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T82" s="72"/>
+      <c r="U82" s="73"/>
+      <c r="V82" s="73"/>
+      <c r="W82" s="74"/>
+    </row>
+    <row r="83" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T83" s="75"/>
+      <c r="U83" s="76"/>
+      <c r="V83" s="76"/>
+      <c r="W83" s="77"/>
+    </row>
+    <row r="84" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T84" s="78"/>
+      <c r="U84" s="79"/>
+      <c r="V84" s="79"/>
+      <c r="W84" s="80"/>
+    </row>
+    <row r="86" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T86" s="70" t="s">
+        <v>112</v>
+      </c>
+      <c r="U86" s="70"/>
+      <c r="V86" s="70"/>
+      <c r="W86" s="70"/>
+    </row>
+    <row r="87" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T87" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="U87" s="62">
+        <v>8</v>
+      </c>
+      <c r="V87" s="55"/>
+      <c r="W87" s="55"/>
+    </row>
+    <row r="88" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T88" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="U88" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="V88" s="55"/>
+      <c r="W88" s="55"/>
+    </row>
+    <row r="89" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T89" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="U89" s="63"/>
+      <c r="V89" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="W89" s="65">
+        <f>ROUND(U89*($C$7+(U87-1)*($D$7-$C$7)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T90" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="U90" s="63">
+        <v>0.15</v>
+      </c>
+      <c r="V90" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="W90" s="65">
+        <f>ROUND(U90*($C$8+(U87-1)*($D$8-$C$8)/98),0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T91" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="U91" s="63">
+        <v>-0.17</v>
+      </c>
+      <c r="V91" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="W91" s="65">
+        <f>ROUND(U91*($C$9+(U87-1)*($D$9-$C$9)/98),0)</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="92" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T92" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="U92" s="63">
+        <v>-0.1</v>
+      </c>
+      <c r="V92" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="W92" s="65">
+        <f>ROUND(U92*($C$10+(U87-1)*($D$10-$C$10)/98),0)</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="93" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T93" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="U93" s="63">
+        <v>0.2</v>
+      </c>
+      <c r="V93" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="W93" s="65">
+        <f>ROUND(U93*($C$11+(U87-1)*($D$11-$C$11)/98),0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T94" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="U94" s="63">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="V94" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="W94" s="65">
+        <f>ROUND(U94*($C$12+(U87-1)*($D$12-$C$12)/98),0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T95" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="U95" s="63">
+        <v>0</v>
+      </c>
+      <c r="V95" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="W95" s="65">
+        <f>ROUND(U95*($C$13+(U87-1)*($D$13-$C$13)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T96" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="U96" s="64">
+        <v>0</v>
+      </c>
+      <c r="V96" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="W96" s="65">
+        <f>ROUND(U96*($C$14+(U87-1)*($D$14-$C$14)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T97" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="U97" s="71"/>
+      <c r="V97" s="71"/>
+      <c r="W97" s="71"/>
+    </row>
+    <row r="98" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T98" s="72"/>
+      <c r="U98" s="73"/>
+      <c r="V98" s="73"/>
+      <c r="W98" s="74"/>
+    </row>
+    <row r="99" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T99" s="75"/>
+      <c r="U99" s="76"/>
+      <c r="V99" s="76"/>
+      <c r="W99" s="77"/>
+    </row>
+    <row r="100" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T100" s="78"/>
+      <c r="U100" s="79"/>
+      <c r="V100" s="79"/>
+      <c r="W100" s="80"/>
+    </row>
+    <row r="102" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T102" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="U102" s="70"/>
+      <c r="V102" s="70"/>
+      <c r="W102" s="70"/>
+    </row>
+    <row r="103" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T103" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="U103" s="62">
+        <v>8</v>
+      </c>
+      <c r="V103" s="55"/>
+      <c r="W103" s="55"/>
+    </row>
+    <row r="104" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T104" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="U104" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="V104" s="55"/>
+      <c r="W104" s="55"/>
+    </row>
+    <row r="105" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T105" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="U105" s="63">
+        <v>-0.15</v>
+      </c>
+      <c r="V105" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="W105" s="65">
+        <f>ROUND(U105*($C$7+(U103-1)*($D$7-$C$7)/98),0)</f>
+        <v>-85</v>
+      </c>
+    </row>
+    <row r="106" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T106" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="U106" s="63">
+        <v>-0.15</v>
+      </c>
+      <c r="V106" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="W106" s="65">
+        <f>ROUND(U106*($C$8+(U103-1)*($D$8-$C$8)/98),0)</f>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="107" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T107" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="U107" s="63">
+        <v>-0.15</v>
+      </c>
+      <c r="V107" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="W107" s="65">
+        <f>ROUND(U107*($C$9+(U103-1)*($D$9-$C$9)/98),0)</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="108" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T108" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="U108" s="63">
+        <v>-0.15</v>
+      </c>
+      <c r="V108" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="W108" s="65">
+        <f>ROUND(U108*($C$10+(U103-1)*($D$10-$C$10)/98),0)</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="109" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T109" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="U109" s="63">
+        <v>-0.15</v>
+      </c>
+      <c r="V109" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="W109" s="65">
+        <f>ROUND(U109*($C$11+(U103-1)*($D$11-$C$11)/98),0)</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="110" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T110" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="U110" s="63">
+        <v>-0.15</v>
+      </c>
+      <c r="V110" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="W110" s="65">
+        <f>ROUND(U110*($C$12+(U103-1)*($D$12-$C$12)/98),0)</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="111" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T111" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="U111" s="63">
+        <v>-0.15</v>
+      </c>
+      <c r="V111" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="W111" s="65">
+        <f>ROUND(U111*($C$13+(U103-1)*($D$13-$C$13)/98),0)</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="112" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T112" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="U112" s="64">
+        <v>2</v>
+      </c>
+      <c r="V112" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="W112" s="65">
+        <f>ROUND(U112*($C$14+(U103-1)*($D$14-$C$14)/98),0)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="113" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T113" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="U113" s="71"/>
+      <c r="V113" s="71"/>
+      <c r="W113" s="71"/>
+    </row>
+    <row r="114" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T114" s="72"/>
+      <c r="U114" s="73"/>
+      <c r="V114" s="73"/>
+      <c r="W114" s="74"/>
+    </row>
+    <row r="115" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T115" s="75"/>
+      <c r="U115" s="76"/>
+      <c r="V115" s="76"/>
+      <c r="W115" s="77"/>
+    </row>
+    <row r="116" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T116" s="78"/>
+      <c r="U116" s="79"/>
+      <c r="V116" s="79"/>
+      <c r="W116" s="80"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="73">
+    <mergeCell ref="T114:W116"/>
+    <mergeCell ref="AI38:AL38"/>
+    <mergeCell ref="AI49:AL49"/>
+    <mergeCell ref="AI50:AL52"/>
+    <mergeCell ref="AI54:AL54"/>
+    <mergeCell ref="AI65:AL65"/>
+    <mergeCell ref="AI66:AL68"/>
+    <mergeCell ref="T86:W86"/>
+    <mergeCell ref="T97:W97"/>
+    <mergeCell ref="T98:W100"/>
+    <mergeCell ref="T102:W102"/>
+    <mergeCell ref="T113:W113"/>
+    <mergeCell ref="T65:W65"/>
+    <mergeCell ref="T66:W68"/>
+    <mergeCell ref="T70:W70"/>
+    <mergeCell ref="T81:W81"/>
+    <mergeCell ref="T82:W84"/>
+    <mergeCell ref="AN17:AQ17"/>
+    <mergeCell ref="AN18:AQ20"/>
+    <mergeCell ref="O66:R68"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="T17:W17"/>
+    <mergeCell ref="T18:W20"/>
+    <mergeCell ref="T22:W22"/>
+    <mergeCell ref="T33:W33"/>
+    <mergeCell ref="T34:W36"/>
+    <mergeCell ref="T38:W38"/>
+    <mergeCell ref="T49:W49"/>
+    <mergeCell ref="T50:W52"/>
+    <mergeCell ref="O38:R38"/>
+    <mergeCell ref="O49:R49"/>
+    <mergeCell ref="O50:R52"/>
+    <mergeCell ref="T54:W54"/>
+    <mergeCell ref="O54:R54"/>
+    <mergeCell ref="O65:R65"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M36"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="O18:R20"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="O33:R33"/>
+    <mergeCell ref="O34:R36"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J18:M20"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="Y17:AB17"/>
+    <mergeCell ref="Y18:AB20"/>
+    <mergeCell ref="Y22:AB22"/>
+    <mergeCell ref="Y33:AB33"/>
+    <mergeCell ref="Y34:AB36"/>
     <mergeCell ref="AS6:AV6"/>
     <mergeCell ref="AS17:AV17"/>
     <mergeCell ref="AS18:AV20"/>
@@ -4123,46 +5162,7 @@
     <mergeCell ref="AD18:AG20"/>
     <mergeCell ref="AD22:AG22"/>
     <mergeCell ref="AD33:AG33"/>
-    <mergeCell ref="Y17:AB17"/>
-    <mergeCell ref="Y18:AB20"/>
-    <mergeCell ref="Y22:AB22"/>
-    <mergeCell ref="Y33:AB33"/>
-    <mergeCell ref="Y34:AB36"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="Y6:AB6"/>
-    <mergeCell ref="O54:R54"/>
-    <mergeCell ref="O65:R65"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M36"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O17:R17"/>
-    <mergeCell ref="O18:R20"/>
-    <mergeCell ref="O22:R22"/>
-    <mergeCell ref="O33:R33"/>
-    <mergeCell ref="O34:R36"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="J18:M20"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J22:M22"/>
     <mergeCell ref="AN6:AQ6"/>
-    <mergeCell ref="AN17:AQ17"/>
-    <mergeCell ref="AN18:AQ20"/>
-    <mergeCell ref="O66:R68"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="T17:W17"/>
-    <mergeCell ref="T18:W20"/>
-    <mergeCell ref="T22:W22"/>
-    <mergeCell ref="T33:W33"/>
-    <mergeCell ref="T34:W36"/>
-    <mergeCell ref="T38:W38"/>
-    <mergeCell ref="T49:W49"/>
-    <mergeCell ref="T50:W52"/>
-    <mergeCell ref="O38:R38"/>
-    <mergeCell ref="O49:R49"/>
-    <mergeCell ref="O50:R52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4190,13 +5190,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
@@ -4208,15 +5208,15 @@
       <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="F4" s="82" t="s">
+      <c r="B4" s="81"/>
+      <c r="F4" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -4525,10 +5525,10 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="81"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -4555,7 +5555,7 @@
       <c r="M17" s="71"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="81"/>
+      <c r="J18" s="72"/>
       <c r="K18" s="73"/>
       <c r="L18" s="73"/>
       <c r="M18" s="74"/>
@@ -4820,7 +5820,7 @@
       <c r="M33" s="71"/>
     </row>
     <row r="34" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J34" s="81"/>
+      <c r="J34" s="72"/>
       <c r="K34" s="73"/>
       <c r="L34" s="73"/>
       <c r="M34" s="74"/>
@@ -4994,7 +5994,7 @@
       <c r="M49" s="71"/>
     </row>
     <row r="50" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J50" s="81"/>
+      <c r="J50" s="72"/>
       <c r="K50" s="73"/>
       <c r="L50" s="73"/>
       <c r="M50" s="74"/>
@@ -5013,6 +6013,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
     <mergeCell ref="J38:M38"/>
     <mergeCell ref="J49:M49"/>
     <mergeCell ref="J50:M52"/>
@@ -5020,12 +6026,6 @@
     <mergeCell ref="J22:M22"/>
     <mergeCell ref="J33:M33"/>
     <mergeCell ref="J34:M36"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5052,13 +6052,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -5070,15 +6070,15 @@
       <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="F4" s="82" t="s">
+      <c r="B4" s="81"/>
+      <c r="F4" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -5613,10 +6613,10 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="81"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -5681,15 +6681,15 @@
       <c r="W17" s="71"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J18" s="81"/>
+      <c r="J18" s="72"/>
       <c r="K18" s="73"/>
       <c r="L18" s="73"/>
       <c r="M18" s="74"/>
-      <c r="O18" s="81"/>
+      <c r="O18" s="72"/>
       <c r="P18" s="73"/>
       <c r="Q18" s="73"/>
       <c r="R18" s="74"/>
-      <c r="T18" s="81"/>
+      <c r="T18" s="72"/>
       <c r="U18" s="73"/>
       <c r="V18" s="73"/>
       <c r="W18" s="74"/>
@@ -6102,11 +7102,11 @@
       <c r="R33" s="71"/>
     </row>
     <row r="34" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J34" s="81"/>
+      <c r="J34" s="72"/>
       <c r="K34" s="73"/>
       <c r="L34" s="73"/>
       <c r="M34" s="74"/>
-      <c r="O34" s="81"/>
+      <c r="O34" s="72"/>
       <c r="P34" s="73"/>
       <c r="Q34" s="73"/>
       <c r="R34" s="74"/>
@@ -6288,7 +7288,7 @@
       <c r="R49" s="71"/>
     </row>
     <row r="50" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O50" s="81"/>
+      <c r="O50" s="72"/>
       <c r="P50" s="73"/>
       <c r="Q50" s="73"/>
       <c r="R50" s="74"/>
@@ -6307,11 +7307,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="O38:R38"/>
+    <mergeCell ref="O49:R49"/>
+    <mergeCell ref="O50:R52"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="T17:W17"/>
+    <mergeCell ref="T18:W20"/>
     <mergeCell ref="J18:M20"/>
     <mergeCell ref="J22:M22"/>
     <mergeCell ref="J33:M33"/>
@@ -6323,12 +7324,11 @@
     <mergeCell ref="O33:R33"/>
     <mergeCell ref="O34:R36"/>
     <mergeCell ref="J17:M17"/>
-    <mergeCell ref="O38:R38"/>
-    <mergeCell ref="O49:R49"/>
-    <mergeCell ref="O50:R52"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="T17:W17"/>
-    <mergeCell ref="T18:W20"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6353,13 +7353,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
@@ -6371,15 +7371,15 @@
       <c r="E2" s="17"/>
     </row>
     <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="F4" s="82" t="s">
+      <c r="B4" s="81"/>
+      <c r="F4" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -6801,10 +7801,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="81"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -6850,11 +7850,11 @@
       <c r="R17" s="71"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J18" s="81"/>
+      <c r="J18" s="72"/>
       <c r="K18" s="73"/>
       <c r="L18" s="73"/>
       <c r="M18" s="74"/>
-      <c r="O18" s="81"/>
+      <c r="O18" s="72"/>
       <c r="P18" s="73"/>
       <c r="Q18" s="73"/>
       <c r="R18" s="74"/>
@@ -7259,11 +8259,11 @@
       <c r="R33" s="71"/>
     </row>
     <row r="34" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J34" s="81"/>
+      <c r="J34" s="72"/>
       <c r="K34" s="73"/>
       <c r="L34" s="73"/>
       <c r="M34" s="74"/>
-      <c r="O34" s="81"/>
+      <c r="O34" s="72"/>
       <c r="P34" s="73"/>
       <c r="Q34" s="73"/>
       <c r="R34" s="74"/>
@@ -7445,7 +8445,7 @@
       <c r="M49" s="71"/>
     </row>
     <row r="50" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J50" s="81"/>
+      <c r="J50" s="72"/>
       <c r="K50" s="73"/>
       <c r="L50" s="73"/>
       <c r="M50" s="74"/>
@@ -7464,11 +8464,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J50:M52"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="O33:R33"/>
+    <mergeCell ref="O34:R36"/>
     <mergeCell ref="J18:M20"/>
     <mergeCell ref="J22:M22"/>
     <mergeCell ref="J33:M33"/>
@@ -7477,12 +8478,11 @@
     <mergeCell ref="O17:R17"/>
     <mergeCell ref="O18:R20"/>
     <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="J50:M52"/>
-    <mergeCell ref="O22:R22"/>
-    <mergeCell ref="O33:R33"/>
-    <mergeCell ref="O34:R36"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7492,7 +8492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -7507,13 +8507,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -7521,15 +8521,15 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="F4" s="82" t="s">
+      <c r="B4" s="81"/>
+      <c r="F4" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -7963,10 +8963,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="82"/>
+      <c r="B16" s="81"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -8012,13 +9012,13 @@
       <c r="R17" s="71"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J18" s="72" t="s">
+      <c r="J18" s="82" t="s">
         <v>76</v>
       </c>
       <c r="K18" s="83"/>
       <c r="L18" s="83"/>
       <c r="M18" s="84"/>
-      <c r="O18" s="72" t="s">
+      <c r="O18" s="82" t="s">
         <v>100</v>
       </c>
       <c r="P18" s="83"/>
@@ -8293,7 +9293,7 @@
       <c r="M33" s="71"/>
     </row>
     <row r="34" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J34" s="72" t="s">
+      <c r="J34" s="82" t="s">
         <v>80</v>
       </c>
       <c r="K34" s="83"/>
@@ -8469,7 +9469,7 @@
       <c r="M49" s="71"/>
     </row>
     <row r="50" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J50" s="72" t="s">
+      <c r="J50" s="82" t="s">
         <v>87</v>
       </c>
       <c r="K50" s="83"/>
@@ -8645,7 +9645,7 @@
       <c r="M65" s="71"/>
     </row>
     <row r="66" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J66" s="72" t="s">
+      <c r="J66" s="82" t="s">
         <v>102</v>
       </c>
       <c r="K66" s="83"/>
@@ -8821,7 +9821,7 @@
       <c r="M81" s="71"/>
     </row>
     <row r="82" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J82" s="72" t="s">
+      <c r="J82" s="82" t="s">
         <v>109</v>
       </c>
       <c r="K82" s="83"/>
@@ -8842,6 +9842,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="J18:M20"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="O18:R20"/>
     <mergeCell ref="J34:M36"/>
     <mergeCell ref="J70:M70"/>
     <mergeCell ref="J81:M81"/>
@@ -8852,18 +9864,6 @@
     <mergeCell ref="J38:M38"/>
     <mergeCell ref="J49:M49"/>
     <mergeCell ref="J50:M52"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O17:R17"/>
-    <mergeCell ref="J18:M20"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="O18:R20"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Kreole work / mine work
</commit_message>
<xml_diff>
--- a/Weapons and Armor.xlsx
+++ b/Weapons and Armor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="12435" windowHeight="7740" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="12435" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="141">
   <si>
     <t>Reminiscence Weapons and Armor</t>
   </si>
@@ -443,6 +443,9 @@
   </si>
   <si>
     <t>Aaglon Pass</t>
+  </si>
+  <si>
+    <t>Mine B1</t>
   </si>
 </sst>
 </file>
@@ -947,21 +950,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -989,6 +977,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -997,12 +1006,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1342,7 +1345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV123"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="O69" sqref="O69:R69"/>
     </sheetView>
   </sheetViews>
@@ -1356,13 +1359,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:48" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
@@ -1374,17 +1377,17 @@
       <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="87"/>
+      <c r="B4" s="85"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -1407,54 +1410,54 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="O6" s="73" t="s">
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="O6" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-      <c r="T6" s="73" t="s">
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="T6" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="U6" s="73"/>
-      <c r="V6" s="73"/>
-      <c r="W6" s="73"/>
-      <c r="Y6" s="73" t="s">
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="Y6" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="Z6" s="73"/>
-      <c r="AA6" s="73"/>
-      <c r="AB6" s="73"/>
-      <c r="AD6" s="73" t="s">
+      <c r="Z6" s="79"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="79"/>
+      <c r="AD6" s="79" t="s">
         <v>91</v>
       </c>
-      <c r="AE6" s="73"/>
-      <c r="AF6" s="73"/>
-      <c r="AG6" s="73"/>
-      <c r="AI6" s="73" t="s">
+      <c r="AE6" s="79"/>
+      <c r="AF6" s="79"/>
+      <c r="AG6" s="79"/>
+      <c r="AI6" s="79" t="s">
         <v>95</v>
       </c>
-      <c r="AJ6" s="73"/>
-      <c r="AK6" s="73"/>
-      <c r="AL6" s="73"/>
-      <c r="AN6" s="73" t="s">
+      <c r="AJ6" s="79"/>
+      <c r="AK6" s="79"/>
+      <c r="AL6" s="79"/>
+      <c r="AN6" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="AO6" s="73"/>
-      <c r="AP6" s="73"/>
-      <c r="AQ6" s="73"/>
-      <c r="AS6" s="73" t="s">
+      <c r="AO6" s="79"/>
+      <c r="AP6" s="79"/>
+      <c r="AQ6" s="79"/>
+      <c r="AS6" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="AT6" s="73"/>
-      <c r="AU6" s="73"/>
-      <c r="AV6" s="73"/>
+      <c r="AT6" s="79"/>
+      <c r="AU6" s="79"/>
+      <c r="AV6" s="79"/>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -2487,10 +2490,10 @@
       </c>
     </row>
     <row r="16" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="87"/>
+      <c r="B16" s="85"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -2603,117 +2606,117 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="70" t="s">
+      <c r="K17" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="L17" s="71"/>
-      <c r="M17" s="72"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="84"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="70" t="s">
+      <c r="P17" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="72"/>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="84"/>
       <c r="T17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U17" s="70" t="s">
+      <c r="U17" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="V17" s="71"/>
-      <c r="W17" s="72"/>
+      <c r="V17" s="83"/>
+      <c r="W17" s="84"/>
       <c r="Y17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Z17" s="70" t="s">
+      <c r="Z17" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="AA17" s="71"/>
-      <c r="AB17" s="72"/>
+      <c r="AA17" s="83"/>
+      <c r="AB17" s="84"/>
       <c r="AD17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE17" s="70" t="s">
+      <c r="AE17" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="AF17" s="71"/>
-      <c r="AG17" s="72"/>
+      <c r="AF17" s="83"/>
+      <c r="AG17" s="84"/>
       <c r="AI17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ17" s="70" t="s">
+      <c r="AJ17" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="AK17" s="71"/>
-      <c r="AL17" s="72"/>
+      <c r="AK17" s="83"/>
+      <c r="AL17" s="84"/>
       <c r="AN17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AO17" s="70" t="s">
+      <c r="AO17" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="AP17" s="71"/>
-      <c r="AQ17" s="72"/>
+      <c r="AP17" s="83"/>
+      <c r="AQ17" s="84"/>
       <c r="AS17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AT17" s="70" t="s">
+      <c r="AT17" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="AU17" s="71"/>
-      <c r="AV17" s="72"/>
+      <c r="AU17" s="83"/>
+      <c r="AV17" s="84"/>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="J18" s="74" t="s">
+      <c r="J18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
-      <c r="O18" s="74" t="s">
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
+      <c r="O18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
-      <c r="T18" s="74" t="s">
+      <c r="P18" s="80"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="80"/>
+      <c r="T18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="U18" s="74"/>
-      <c r="V18" s="74"/>
-      <c r="W18" s="74"/>
-      <c r="Y18" s="74" t="s">
+      <c r="U18" s="80"/>
+      <c r="V18" s="80"/>
+      <c r="W18" s="80"/>
+      <c r="Y18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="Z18" s="74"/>
-      <c r="AA18" s="74"/>
-      <c r="AB18" s="74"/>
-      <c r="AD18" s="74" t="s">
+      <c r="Z18" s="80"/>
+      <c r="AA18" s="80"/>
+      <c r="AB18" s="80"/>
+      <c r="AD18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AE18" s="74"/>
-      <c r="AF18" s="74"/>
-      <c r="AG18" s="74"/>
-      <c r="AI18" s="74" t="s">
+      <c r="AE18" s="80"/>
+      <c r="AF18" s="80"/>
+      <c r="AG18" s="80"/>
+      <c r="AI18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AJ18" s="74"/>
-      <c r="AK18" s="74"/>
-      <c r="AL18" s="74"/>
-      <c r="AN18" s="74" t="s">
+      <c r="AJ18" s="80"/>
+      <c r="AK18" s="80"/>
+      <c r="AL18" s="80"/>
+      <c r="AN18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AO18" s="74"/>
-      <c r="AP18" s="74"/>
-      <c r="AQ18" s="74"/>
-      <c r="AS18" s="74" t="s">
+      <c r="AO18" s="80"/>
+      <c r="AP18" s="80"/>
+      <c r="AQ18" s="80"/>
+      <c r="AS18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AT18" s="74"/>
-      <c r="AU18" s="74"/>
-      <c r="AV18" s="74"/>
+      <c r="AT18" s="80"/>
+      <c r="AU18" s="80"/>
+      <c r="AV18" s="80"/>
     </row>
     <row r="19" spans="1:48" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -2725,42 +2728,42 @@
       <c r="C19" s="13">
         <v>8</v>
       </c>
-      <c r="J19" s="75"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="77"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="76"/>
-      <c r="R19" s="77"/>
-      <c r="T19" s="75"/>
-      <c r="U19" s="76"/>
-      <c r="V19" s="76"/>
-      <c r="W19" s="77"/>
-      <c r="Y19" s="75"/>
-      <c r="Z19" s="76"/>
-      <c r="AA19" s="76"/>
-      <c r="AB19" s="77"/>
-      <c r="AD19" s="75" t="s">
+      <c r="J19" s="70"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="72"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="71"/>
+      <c r="Q19" s="71"/>
+      <c r="R19" s="72"/>
+      <c r="T19" s="70"/>
+      <c r="U19" s="71"/>
+      <c r="V19" s="71"/>
+      <c r="W19" s="72"/>
+      <c r="Y19" s="70"/>
+      <c r="Z19" s="71"/>
+      <c r="AA19" s="71"/>
+      <c r="AB19" s="72"/>
+      <c r="AD19" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="AE19" s="76"/>
-      <c r="AF19" s="76"/>
-      <c r="AG19" s="77"/>
-      <c r="AI19" s="75"/>
-      <c r="AJ19" s="76"/>
-      <c r="AK19" s="76"/>
-      <c r="AL19" s="77"/>
-      <c r="AN19" s="88" t="s">
+      <c r="AE19" s="71"/>
+      <c r="AF19" s="71"/>
+      <c r="AG19" s="72"/>
+      <c r="AI19" s="70"/>
+      <c r="AJ19" s="71"/>
+      <c r="AK19" s="71"/>
+      <c r="AL19" s="72"/>
+      <c r="AN19" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="AO19" s="76"/>
-      <c r="AP19" s="76"/>
-      <c r="AQ19" s="77"/>
-      <c r="AS19" s="75"/>
-      <c r="AT19" s="76"/>
-      <c r="AU19" s="76"/>
-      <c r="AV19" s="77"/>
+      <c r="AO19" s="71"/>
+      <c r="AP19" s="71"/>
+      <c r="AQ19" s="72"/>
+      <c r="AS19" s="70"/>
+      <c r="AT19" s="71"/>
+      <c r="AU19" s="71"/>
+      <c r="AV19" s="72"/>
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
@@ -2773,38 +2776,38 @@
         <f t="shared" ref="C20:C27" si="0">C7+($C$19-1)*(D7-C7)/98</f>
         <v>565</v>
       </c>
-      <c r="J20" s="78"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="80"/>
-      <c r="O20" s="78"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="80"/>
-      <c r="T20" s="78"/>
-      <c r="U20" s="79"/>
-      <c r="V20" s="79"/>
-      <c r="W20" s="80"/>
-      <c r="Y20" s="78"/>
-      <c r="Z20" s="79"/>
-      <c r="AA20" s="79"/>
-      <c r="AB20" s="80"/>
-      <c r="AD20" s="78"/>
-      <c r="AE20" s="79"/>
-      <c r="AF20" s="79"/>
-      <c r="AG20" s="80"/>
-      <c r="AI20" s="78"/>
-      <c r="AJ20" s="79"/>
-      <c r="AK20" s="79"/>
-      <c r="AL20" s="80"/>
-      <c r="AN20" s="78"/>
-      <c r="AO20" s="79"/>
-      <c r="AP20" s="79"/>
-      <c r="AQ20" s="80"/>
-      <c r="AS20" s="78"/>
-      <c r="AT20" s="79"/>
-      <c r="AU20" s="79"/>
-      <c r="AV20" s="80"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="75"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="74"/>
+      <c r="Q20" s="74"/>
+      <c r="R20" s="75"/>
+      <c r="T20" s="73"/>
+      <c r="U20" s="74"/>
+      <c r="V20" s="74"/>
+      <c r="W20" s="75"/>
+      <c r="Y20" s="73"/>
+      <c r="Z20" s="74"/>
+      <c r="AA20" s="74"/>
+      <c r="AB20" s="75"/>
+      <c r="AD20" s="73"/>
+      <c r="AE20" s="74"/>
+      <c r="AF20" s="74"/>
+      <c r="AG20" s="75"/>
+      <c r="AI20" s="73"/>
+      <c r="AJ20" s="74"/>
+      <c r="AK20" s="74"/>
+      <c r="AL20" s="75"/>
+      <c r="AN20" s="73"/>
+      <c r="AO20" s="74"/>
+      <c r="AP20" s="74"/>
+      <c r="AQ20" s="75"/>
+      <c r="AS20" s="73"/>
+      <c r="AT20" s="74"/>
+      <c r="AU20" s="74"/>
+      <c r="AV20" s="75"/>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
@@ -2817,38 +2820,38 @@
         <f t="shared" si="0"/>
         <v>121.07142857142857</v>
       </c>
-      <c r="J21" s="81"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="82"/>
-      <c r="M21" s="83"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="82"/>
-      <c r="Q21" s="82"/>
-      <c r="R21" s="83"/>
-      <c r="T21" s="81"/>
-      <c r="U21" s="82"/>
-      <c r="V21" s="82"/>
-      <c r="W21" s="83"/>
-      <c r="Y21" s="81"/>
-      <c r="Z21" s="82"/>
-      <c r="AA21" s="82"/>
-      <c r="AB21" s="83"/>
-      <c r="AD21" s="81"/>
-      <c r="AE21" s="82"/>
-      <c r="AF21" s="82"/>
-      <c r="AG21" s="83"/>
-      <c r="AI21" s="81"/>
-      <c r="AJ21" s="82"/>
-      <c r="AK21" s="82"/>
-      <c r="AL21" s="83"/>
-      <c r="AN21" s="81"/>
-      <c r="AO21" s="82"/>
-      <c r="AP21" s="82"/>
-      <c r="AQ21" s="83"/>
-      <c r="AS21" s="81"/>
-      <c r="AT21" s="82"/>
-      <c r="AU21" s="82"/>
-      <c r="AV21" s="83"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="78"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="77"/>
+      <c r="Q21" s="77"/>
+      <c r="R21" s="78"/>
+      <c r="T21" s="76"/>
+      <c r="U21" s="77"/>
+      <c r="V21" s="77"/>
+      <c r="W21" s="78"/>
+      <c r="Y21" s="76"/>
+      <c r="Z21" s="77"/>
+      <c r="AA21" s="77"/>
+      <c r="AB21" s="78"/>
+      <c r="AD21" s="76"/>
+      <c r="AE21" s="77"/>
+      <c r="AF21" s="77"/>
+      <c r="AG21" s="78"/>
+      <c r="AI21" s="76"/>
+      <c r="AJ21" s="77"/>
+      <c r="AK21" s="77"/>
+      <c r="AL21" s="78"/>
+      <c r="AN21" s="76"/>
+      <c r="AO21" s="77"/>
+      <c r="AP21" s="77"/>
+      <c r="AQ21" s="78"/>
+      <c r="AS21" s="76"/>
+      <c r="AT21" s="77"/>
+      <c r="AU21" s="77"/>
+      <c r="AV21" s="78"/>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -2873,42 +2876,42 @@
         <f t="shared" si="0"/>
         <v>35.357142857142861</v>
       </c>
-      <c r="J23" s="73" t="s">
+      <c r="J23" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="73"/>
-      <c r="O23" s="73" t="s">
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="O23" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="P23" s="73"/>
-      <c r="Q23" s="73"/>
-      <c r="R23" s="73"/>
-      <c r="T23" s="73" t="s">
+      <c r="P23" s="79"/>
+      <c r="Q23" s="79"/>
+      <c r="R23" s="79"/>
+      <c r="T23" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="U23" s="73"/>
-      <c r="V23" s="73"/>
-      <c r="W23" s="73"/>
-      <c r="Y23" s="73" t="s">
+      <c r="U23" s="79"/>
+      <c r="V23" s="79"/>
+      <c r="W23" s="79"/>
+      <c r="Y23" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="Z23" s="73"/>
-      <c r="AA23" s="73"/>
-      <c r="AB23" s="73"/>
-      <c r="AD23" s="73" t="s">
+      <c r="Z23" s="79"/>
+      <c r="AA23" s="79"/>
+      <c r="AB23" s="79"/>
+      <c r="AD23" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="AE23" s="73"/>
-      <c r="AF23" s="73"/>
-      <c r="AG23" s="73"/>
-      <c r="AI23" s="73" t="s">
+      <c r="AE23" s="79"/>
+      <c r="AF23" s="79"/>
+      <c r="AG23" s="79"/>
+      <c r="AI23" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="AJ23" s="73"/>
-      <c r="AK23" s="73"/>
-      <c r="AL23" s="73"/>
+      <c r="AJ23" s="79"/>
+      <c r="AK23" s="79"/>
+      <c r="AL23" s="79"/>
     </row>
     <row r="24" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
@@ -3694,209 +3697,209 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="70" t="s">
+      <c r="K34" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="L34" s="71"/>
-      <c r="M34" s="72"/>
+      <c r="L34" s="83"/>
+      <c r="M34" s="84"/>
       <c r="O34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P34" s="70" t="s">
+      <c r="P34" s="82" t="s">
         <v>130</v>
       </c>
-      <c r="Q34" s="71"/>
-      <c r="R34" s="72"/>
+      <c r="Q34" s="83"/>
+      <c r="R34" s="84"/>
       <c r="T34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U34" s="70" t="s">
+      <c r="U34" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="V34" s="71"/>
-      <c r="W34" s="72"/>
+      <c r="V34" s="83"/>
+      <c r="W34" s="84"/>
       <c r="Y34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Z34" s="70" t="s">
+      <c r="Z34" s="82" t="s">
         <v>133</v>
       </c>
-      <c r="AA34" s="71"/>
-      <c r="AB34" s="72"/>
+      <c r="AA34" s="83"/>
+      <c r="AB34" s="84"/>
       <c r="AD34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE34" s="70" t="s">
+      <c r="AE34" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="AF34" s="71"/>
-      <c r="AG34" s="72"/>
+      <c r="AF34" s="83"/>
+      <c r="AG34" s="84"/>
       <c r="AI34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ34" s="70" t="s">
+      <c r="AJ34" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="AK34" s="71"/>
-      <c r="AL34" s="72"/>
+      <c r="AK34" s="83"/>
+      <c r="AL34" s="84"/>
     </row>
     <row r="35" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J35" s="74" t="s">
+      <c r="J35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="74"/>
-      <c r="O35" s="74" t="s">
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
+      <c r="O35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="P35" s="74"/>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="74"/>
-      <c r="T35" s="74" t="s">
+      <c r="P35" s="80"/>
+      <c r="Q35" s="80"/>
+      <c r="R35" s="80"/>
+      <c r="T35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="U35" s="74"/>
-      <c r="V35" s="74"/>
-      <c r="W35" s="74"/>
-      <c r="Y35" s="74" t="s">
+      <c r="U35" s="80"/>
+      <c r="V35" s="80"/>
+      <c r="W35" s="80"/>
+      <c r="Y35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="Z35" s="74"/>
-      <c r="AA35" s="74"/>
-      <c r="AB35" s="74"/>
-      <c r="AD35" s="74" t="s">
+      <c r="Z35" s="80"/>
+      <c r="AA35" s="80"/>
+      <c r="AB35" s="80"/>
+      <c r="AD35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AE35" s="74"/>
-      <c r="AF35" s="74"/>
-      <c r="AG35" s="74"/>
-      <c r="AI35" s="84" t="s">
+      <c r="AE35" s="80"/>
+      <c r="AF35" s="80"/>
+      <c r="AG35" s="80"/>
+      <c r="AI35" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="AJ35" s="85"/>
-      <c r="AK35" s="85"/>
-      <c r="AL35" s="86"/>
+      <c r="AJ35" s="87"/>
+      <c r="AK35" s="87"/>
+      <c r="AL35" s="88"/>
     </row>
     <row r="36" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J36" s="88" t="s">
+      <c r="J36" s="81" t="s">
         <v>119</v>
       </c>
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="77"/>
-      <c r="O36" s="75"/>
-      <c r="P36" s="76"/>
-      <c r="Q36" s="76"/>
-      <c r="R36" s="77"/>
-      <c r="T36" s="75" t="s">
+      <c r="K36" s="71"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="72"/>
+      <c r="O36" s="70"/>
+      <c r="P36" s="71"/>
+      <c r="Q36" s="71"/>
+      <c r="R36" s="72"/>
+      <c r="T36" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="U36" s="76"/>
-      <c r="V36" s="76"/>
-      <c r="W36" s="77"/>
-      <c r="Y36" s="75"/>
-      <c r="Z36" s="76"/>
-      <c r="AA36" s="76"/>
-      <c r="AB36" s="77"/>
-      <c r="AD36" s="75"/>
-      <c r="AE36" s="76"/>
-      <c r="AF36" s="76"/>
-      <c r="AG36" s="77"/>
-      <c r="AI36" s="75"/>
-      <c r="AJ36" s="76"/>
-      <c r="AK36" s="76"/>
-      <c r="AL36" s="77"/>
+      <c r="U36" s="71"/>
+      <c r="V36" s="71"/>
+      <c r="W36" s="72"/>
+      <c r="Y36" s="70"/>
+      <c r="Z36" s="71"/>
+      <c r="AA36" s="71"/>
+      <c r="AB36" s="72"/>
+      <c r="AD36" s="70"/>
+      <c r="AE36" s="71"/>
+      <c r="AF36" s="71"/>
+      <c r="AG36" s="72"/>
+      <c r="AI36" s="70"/>
+      <c r="AJ36" s="71"/>
+      <c r="AK36" s="71"/>
+      <c r="AL36" s="72"/>
     </row>
     <row r="37" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J37" s="78"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="80"/>
-      <c r="O37" s="78"/>
-      <c r="P37" s="79"/>
-      <c r="Q37" s="79"/>
-      <c r="R37" s="80"/>
-      <c r="T37" s="78"/>
-      <c r="U37" s="79"/>
-      <c r="V37" s="79"/>
-      <c r="W37" s="80"/>
-      <c r="Y37" s="78"/>
-      <c r="Z37" s="79"/>
-      <c r="AA37" s="79"/>
-      <c r="AB37" s="80"/>
-      <c r="AD37" s="78"/>
-      <c r="AE37" s="79"/>
-      <c r="AF37" s="79"/>
-      <c r="AG37" s="80"/>
-      <c r="AI37" s="78"/>
-      <c r="AJ37" s="79"/>
-      <c r="AK37" s="79"/>
-      <c r="AL37" s="80"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="74"/>
+      <c r="L37" s="74"/>
+      <c r="M37" s="75"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="74"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="75"/>
+      <c r="T37" s="73"/>
+      <c r="U37" s="74"/>
+      <c r="V37" s="74"/>
+      <c r="W37" s="75"/>
+      <c r="Y37" s="73"/>
+      <c r="Z37" s="74"/>
+      <c r="AA37" s="74"/>
+      <c r="AB37" s="75"/>
+      <c r="AD37" s="73"/>
+      <c r="AE37" s="74"/>
+      <c r="AF37" s="74"/>
+      <c r="AG37" s="75"/>
+      <c r="AI37" s="73"/>
+      <c r="AJ37" s="74"/>
+      <c r="AK37" s="74"/>
+      <c r="AL37" s="75"/>
     </row>
     <row r="38" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J38" s="81"/>
-      <c r="K38" s="82"/>
-      <c r="L38" s="82"/>
-      <c r="M38" s="83"/>
-      <c r="O38" s="81"/>
-      <c r="P38" s="82"/>
-      <c r="Q38" s="82"/>
-      <c r="R38" s="83"/>
-      <c r="T38" s="81"/>
-      <c r="U38" s="82"/>
-      <c r="V38" s="82"/>
-      <c r="W38" s="83"/>
-      <c r="Y38" s="81"/>
-      <c r="Z38" s="82"/>
-      <c r="AA38" s="82"/>
-      <c r="AB38" s="83"/>
-      <c r="AD38" s="81"/>
-      <c r="AE38" s="82"/>
-      <c r="AF38" s="82"/>
-      <c r="AG38" s="83"/>
-      <c r="AI38" s="81"/>
-      <c r="AJ38" s="82"/>
-      <c r="AK38" s="82"/>
-      <c r="AL38" s="83"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="77"/>
+      <c r="L38" s="77"/>
+      <c r="M38" s="78"/>
+      <c r="O38" s="76"/>
+      <c r="P38" s="77"/>
+      <c r="Q38" s="77"/>
+      <c r="R38" s="78"/>
+      <c r="T38" s="76"/>
+      <c r="U38" s="77"/>
+      <c r="V38" s="77"/>
+      <c r="W38" s="78"/>
+      <c r="Y38" s="76"/>
+      <c r="Z38" s="77"/>
+      <c r="AA38" s="77"/>
+      <c r="AB38" s="78"/>
+      <c r="AD38" s="76"/>
+      <c r="AE38" s="77"/>
+      <c r="AF38" s="77"/>
+      <c r="AG38" s="78"/>
+      <c r="AI38" s="76"/>
+      <c r="AJ38" s="77"/>
+      <c r="AK38" s="77"/>
+      <c r="AL38" s="78"/>
     </row>
     <row r="40" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J40" s="73" t="s">
+      <c r="J40" s="79" t="s">
         <v>122</v>
       </c>
-      <c r="K40" s="73"/>
-      <c r="L40" s="73"/>
-      <c r="M40" s="73"/>
-      <c r="O40" s="73" t="s">
+      <c r="K40" s="79"/>
+      <c r="L40" s="79"/>
+      <c r="M40" s="79"/>
+      <c r="O40" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="P40" s="73"/>
-      <c r="Q40" s="73"/>
-      <c r="R40" s="73"/>
-      <c r="T40" s="73" t="s">
+      <c r="P40" s="79"/>
+      <c r="Q40" s="79"/>
+      <c r="R40" s="79"/>
+      <c r="T40" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="U40" s="73"/>
-      <c r="V40" s="73"/>
-      <c r="W40" s="73"/>
-      <c r="Y40" s="73" t="s">
+      <c r="U40" s="79"/>
+      <c r="V40" s="79"/>
+      <c r="W40" s="79"/>
+      <c r="Y40" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="Z40" s="73"/>
-      <c r="AA40" s="73"/>
-      <c r="AB40" s="73"/>
-      <c r="AD40" s="73" t="s">
+      <c r="Z40" s="79"/>
+      <c r="AA40" s="79"/>
+      <c r="AB40" s="79"/>
+      <c r="AD40" s="79" t="s">
         <v>117</v>
       </c>
-      <c r="AE40" s="73"/>
-      <c r="AF40" s="73"/>
-      <c r="AG40" s="73"/>
-      <c r="AI40" s="73" t="s">
+      <c r="AE40" s="79"/>
+      <c r="AF40" s="79"/>
+      <c r="AG40" s="79"/>
+      <c r="AI40" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="AJ40" s="73"/>
-      <c r="AK40" s="73"/>
-      <c r="AL40" s="73"/>
+      <c r="AJ40" s="79"/>
+      <c r="AK40" s="79"/>
+      <c r="AL40" s="79"/>
     </row>
     <row r="41" spans="10:38" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -4642,193 +4645,193 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="70"/>
-      <c r="L51" s="71"/>
-      <c r="M51" s="72"/>
+      <c r="K51" s="82"/>
+      <c r="L51" s="83"/>
+      <c r="M51" s="84"/>
       <c r="O51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P51" s="70" t="s">
+      <c r="P51" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="Q51" s="71"/>
-      <c r="R51" s="72"/>
+      <c r="Q51" s="83"/>
+      <c r="R51" s="84"/>
       <c r="T51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U51" s="70" t="s">
+      <c r="U51" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="V51" s="71"/>
-      <c r="W51" s="72"/>
+      <c r="V51" s="83"/>
+      <c r="W51" s="84"/>
       <c r="Y51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Z51" s="70"/>
-      <c r="AA51" s="71"/>
-      <c r="AB51" s="72"/>
+      <c r="Z51" s="82"/>
+      <c r="AA51" s="83"/>
+      <c r="AB51" s="84"/>
       <c r="AD51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE51" s="70" t="s">
+      <c r="AE51" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="AF51" s="71"/>
-      <c r="AG51" s="72"/>
+      <c r="AF51" s="83"/>
+      <c r="AG51" s="84"/>
       <c r="AI51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ51" s="70" t="s">
+      <c r="AJ51" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="AK51" s="71"/>
-      <c r="AL51" s="72"/>
+      <c r="AK51" s="83"/>
+      <c r="AL51" s="84"/>
     </row>
     <row r="52" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J52" s="74" t="s">
+      <c r="J52" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="74"/>
-      <c r="L52" s="74"/>
-      <c r="M52" s="74"/>
-      <c r="O52" s="74" t="s">
+      <c r="K52" s="80"/>
+      <c r="L52" s="80"/>
+      <c r="M52" s="80"/>
+      <c r="O52" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="P52" s="74"/>
-      <c r="Q52" s="74"/>
-      <c r="R52" s="74"/>
-      <c r="T52" s="74" t="s">
+      <c r="P52" s="80"/>
+      <c r="Q52" s="80"/>
+      <c r="R52" s="80"/>
+      <c r="T52" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="U52" s="74"/>
-      <c r="V52" s="74"/>
-      <c r="W52" s="74"/>
-      <c r="Y52" s="74" t="s">
+      <c r="U52" s="80"/>
+      <c r="V52" s="80"/>
+      <c r="W52" s="80"/>
+      <c r="Y52" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="Z52" s="74"/>
-      <c r="AA52" s="74"/>
-      <c r="AB52" s="74"/>
-      <c r="AD52" s="74" t="s">
+      <c r="Z52" s="80"/>
+      <c r="AA52" s="80"/>
+      <c r="AB52" s="80"/>
+      <c r="AD52" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AE52" s="74"/>
-      <c r="AF52" s="74"/>
-      <c r="AG52" s="74"/>
-      <c r="AI52" s="74" t="s">
+      <c r="AE52" s="80"/>
+      <c r="AF52" s="80"/>
+      <c r="AG52" s="80"/>
+      <c r="AI52" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AJ52" s="74"/>
-      <c r="AK52" s="74"/>
-      <c r="AL52" s="74"/>
+      <c r="AJ52" s="80"/>
+      <c r="AK52" s="80"/>
+      <c r="AL52" s="80"/>
     </row>
     <row r="53" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J53" s="88"/>
-      <c r="K53" s="76"/>
-      <c r="L53" s="76"/>
-      <c r="M53" s="77"/>
-      <c r="O53" s="75"/>
-      <c r="P53" s="76"/>
-      <c r="Q53" s="76"/>
-      <c r="R53" s="77"/>
-      <c r="T53" s="75" t="s">
+      <c r="J53" s="81"/>
+      <c r="K53" s="71"/>
+      <c r="L53" s="71"/>
+      <c r="M53" s="72"/>
+      <c r="O53" s="70"/>
+      <c r="P53" s="71"/>
+      <c r="Q53" s="71"/>
+      <c r="R53" s="72"/>
+      <c r="T53" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="U53" s="76"/>
-      <c r="V53" s="76"/>
-      <c r="W53" s="77"/>
-      <c r="Y53" s="75"/>
-      <c r="Z53" s="76"/>
-      <c r="AA53" s="76"/>
-      <c r="AB53" s="77"/>
-      <c r="AD53" s="75"/>
-      <c r="AE53" s="76"/>
-      <c r="AF53" s="76"/>
-      <c r="AG53" s="77"/>
-      <c r="AI53" s="88" t="s">
+      <c r="U53" s="71"/>
+      <c r="V53" s="71"/>
+      <c r="W53" s="72"/>
+      <c r="Y53" s="70"/>
+      <c r="Z53" s="71"/>
+      <c r="AA53" s="71"/>
+      <c r="AB53" s="72"/>
+      <c r="AD53" s="70"/>
+      <c r="AE53" s="71"/>
+      <c r="AF53" s="71"/>
+      <c r="AG53" s="72"/>
+      <c r="AI53" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="AJ53" s="76"/>
-      <c r="AK53" s="76"/>
-      <c r="AL53" s="77"/>
+      <c r="AJ53" s="71"/>
+      <c r="AK53" s="71"/>
+      <c r="AL53" s="72"/>
     </row>
     <row r="54" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J54" s="78"/>
-      <c r="K54" s="79"/>
-      <c r="L54" s="79"/>
-      <c r="M54" s="80"/>
-      <c r="O54" s="78"/>
-      <c r="P54" s="79"/>
-      <c r="Q54" s="79"/>
-      <c r="R54" s="80"/>
-      <c r="T54" s="78"/>
-      <c r="U54" s="79"/>
-      <c r="V54" s="79"/>
-      <c r="W54" s="80"/>
-      <c r="Y54" s="78"/>
-      <c r="Z54" s="79"/>
-      <c r="AA54" s="79"/>
-      <c r="AB54" s="80"/>
-      <c r="AD54" s="78"/>
-      <c r="AE54" s="79"/>
-      <c r="AF54" s="79"/>
-      <c r="AG54" s="80"/>
-      <c r="AI54" s="78"/>
-      <c r="AJ54" s="79"/>
-      <c r="AK54" s="79"/>
-      <c r="AL54" s="80"/>
+      <c r="J54" s="73"/>
+      <c r="K54" s="74"/>
+      <c r="L54" s="74"/>
+      <c r="M54" s="75"/>
+      <c r="O54" s="73"/>
+      <c r="P54" s="74"/>
+      <c r="Q54" s="74"/>
+      <c r="R54" s="75"/>
+      <c r="T54" s="73"/>
+      <c r="U54" s="74"/>
+      <c r="V54" s="74"/>
+      <c r="W54" s="75"/>
+      <c r="Y54" s="73"/>
+      <c r="Z54" s="74"/>
+      <c r="AA54" s="74"/>
+      <c r="AB54" s="75"/>
+      <c r="AD54" s="73"/>
+      <c r="AE54" s="74"/>
+      <c r="AF54" s="74"/>
+      <c r="AG54" s="75"/>
+      <c r="AI54" s="73"/>
+      <c r="AJ54" s="74"/>
+      <c r="AK54" s="74"/>
+      <c r="AL54" s="75"/>
     </row>
     <row r="55" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J55" s="81"/>
-      <c r="K55" s="82"/>
-      <c r="L55" s="82"/>
-      <c r="M55" s="83"/>
-      <c r="O55" s="81"/>
-      <c r="P55" s="82"/>
-      <c r="Q55" s="82"/>
-      <c r="R55" s="83"/>
-      <c r="T55" s="81"/>
-      <c r="U55" s="82"/>
-      <c r="V55" s="82"/>
-      <c r="W55" s="83"/>
-      <c r="Y55" s="81"/>
-      <c r="Z55" s="82"/>
-      <c r="AA55" s="82"/>
-      <c r="AB55" s="83"/>
-      <c r="AD55" s="81"/>
-      <c r="AE55" s="82"/>
-      <c r="AF55" s="82"/>
-      <c r="AG55" s="83"/>
-      <c r="AI55" s="81"/>
-      <c r="AJ55" s="82"/>
-      <c r="AK55" s="82"/>
-      <c r="AL55" s="83"/>
+      <c r="J55" s="76"/>
+      <c r="K55" s="77"/>
+      <c r="L55" s="77"/>
+      <c r="M55" s="78"/>
+      <c r="O55" s="76"/>
+      <c r="P55" s="77"/>
+      <c r="Q55" s="77"/>
+      <c r="R55" s="78"/>
+      <c r="T55" s="76"/>
+      <c r="U55" s="77"/>
+      <c r="V55" s="77"/>
+      <c r="W55" s="78"/>
+      <c r="Y55" s="76"/>
+      <c r="Z55" s="77"/>
+      <c r="AA55" s="77"/>
+      <c r="AB55" s="78"/>
+      <c r="AD55" s="76"/>
+      <c r="AE55" s="77"/>
+      <c r="AF55" s="77"/>
+      <c r="AG55" s="78"/>
+      <c r="AI55" s="76"/>
+      <c r="AJ55" s="77"/>
+      <c r="AK55" s="77"/>
+      <c r="AL55" s="78"/>
     </row>
     <row r="57" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="O57" s="73" t="s">
+      <c r="O57" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="P57" s="73"/>
-      <c r="Q57" s="73"/>
-      <c r="R57" s="73"/>
-      <c r="T57" s="73" t="s">
+      <c r="P57" s="79"/>
+      <c r="Q57" s="79"/>
+      <c r="R57" s="79"/>
+      <c r="T57" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="U57" s="73"/>
-      <c r="V57" s="73"/>
-      <c r="W57" s="73"/>
-      <c r="AD57" s="73" t="s">
+      <c r="U57" s="79"/>
+      <c r="V57" s="79"/>
+      <c r="W57" s="79"/>
+      <c r="AD57" s="79" t="s">
         <v>118</v>
       </c>
-      <c r="AE57" s="73"/>
-      <c r="AF57" s="73"/>
-      <c r="AG57" s="73"/>
-      <c r="AI57" s="73" t="s">
+      <c r="AE57" s="79"/>
+      <c r="AF57" s="79"/>
+      <c r="AG57" s="79"/>
+      <c r="AI57" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="AJ57" s="73"/>
-      <c r="AK57" s="73"/>
-      <c r="AL57" s="73"/>
+      <c r="AJ57" s="79"/>
+      <c r="AK57" s="79"/>
+      <c r="AL57" s="79"/>
     </row>
     <row r="58" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O58" s="54" t="s">
@@ -5334,135 +5337,135 @@
       <c r="O68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P68" s="70" t="s">
+      <c r="P68" s="82" t="s">
         <v>137</v>
       </c>
-      <c r="Q68" s="71"/>
-      <c r="R68" s="72"/>
+      <c r="Q68" s="83"/>
+      <c r="R68" s="84"/>
       <c r="T68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U68" s="70" t="s">
+      <c r="U68" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="V68" s="71"/>
-      <c r="W68" s="72"/>
+      <c r="V68" s="83"/>
+      <c r="W68" s="84"/>
       <c r="AD68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE68" s="70" t="s">
+      <c r="AE68" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="AF68" s="71"/>
-      <c r="AG68" s="72"/>
+      <c r="AF68" s="83"/>
+      <c r="AG68" s="84"/>
       <c r="AI68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ68" s="70" t="s">
+      <c r="AJ68" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="AK68" s="71"/>
-      <c r="AL68" s="72"/>
+      <c r="AK68" s="83"/>
+      <c r="AL68" s="84"/>
     </row>
     <row r="69" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="O69" s="74" t="s">
+      <c r="O69" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="P69" s="74"/>
-      <c r="Q69" s="74"/>
-      <c r="R69" s="74"/>
-      <c r="T69" s="74" t="s">
+      <c r="P69" s="80"/>
+      <c r="Q69" s="80"/>
+      <c r="R69" s="80"/>
+      <c r="T69" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="U69" s="74"/>
-      <c r="V69" s="74"/>
-      <c r="W69" s="74"/>
-      <c r="AD69" s="74" t="s">
+      <c r="U69" s="80"/>
+      <c r="V69" s="80"/>
+      <c r="W69" s="80"/>
+      <c r="AD69" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AE69" s="74"/>
-      <c r="AF69" s="74"/>
-      <c r="AG69" s="74"/>
-      <c r="AI69" s="74" t="s">
+      <c r="AE69" s="80"/>
+      <c r="AF69" s="80"/>
+      <c r="AG69" s="80"/>
+      <c r="AI69" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AJ69" s="74"/>
-      <c r="AK69" s="74"/>
-      <c r="AL69" s="74"/>
+      <c r="AJ69" s="80"/>
+      <c r="AK69" s="80"/>
+      <c r="AL69" s="80"/>
     </row>
     <row r="70" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="O70" s="88" t="s">
+      <c r="O70" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="P70" s="76"/>
-      <c r="Q70" s="76"/>
-      <c r="R70" s="77"/>
-      <c r="T70" s="75"/>
-      <c r="U70" s="76"/>
-      <c r="V70" s="76"/>
-      <c r="W70" s="77"/>
-      <c r="AD70" s="75" t="s">
+      <c r="P70" s="71"/>
+      <c r="Q70" s="71"/>
+      <c r="R70" s="72"/>
+      <c r="T70" s="70"/>
+      <c r="U70" s="71"/>
+      <c r="V70" s="71"/>
+      <c r="W70" s="72"/>
+      <c r="AD70" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="AE70" s="76"/>
-      <c r="AF70" s="76"/>
-      <c r="AG70" s="77"/>
-      <c r="AI70" s="88" t="s">
+      <c r="AE70" s="71"/>
+      <c r="AF70" s="71"/>
+      <c r="AG70" s="72"/>
+      <c r="AI70" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="AJ70" s="76"/>
-      <c r="AK70" s="76"/>
-      <c r="AL70" s="77"/>
+      <c r="AJ70" s="71"/>
+      <c r="AK70" s="71"/>
+      <c r="AL70" s="72"/>
     </row>
     <row r="71" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="O71" s="78"/>
-      <c r="P71" s="79"/>
-      <c r="Q71" s="79"/>
-      <c r="R71" s="80"/>
-      <c r="T71" s="78"/>
-      <c r="U71" s="79"/>
-      <c r="V71" s="79"/>
-      <c r="W71" s="80"/>
-      <c r="AD71" s="78"/>
-      <c r="AE71" s="79"/>
-      <c r="AF71" s="79"/>
-      <c r="AG71" s="80"/>
-      <c r="AI71" s="78"/>
-      <c r="AJ71" s="79"/>
-      <c r="AK71" s="79"/>
-      <c r="AL71" s="80"/>
+      <c r="O71" s="73"/>
+      <c r="P71" s="74"/>
+      <c r="Q71" s="74"/>
+      <c r="R71" s="75"/>
+      <c r="T71" s="73"/>
+      <c r="U71" s="74"/>
+      <c r="V71" s="74"/>
+      <c r="W71" s="75"/>
+      <c r="AD71" s="73"/>
+      <c r="AE71" s="74"/>
+      <c r="AF71" s="74"/>
+      <c r="AG71" s="75"/>
+      <c r="AI71" s="73"/>
+      <c r="AJ71" s="74"/>
+      <c r="AK71" s="74"/>
+      <c r="AL71" s="75"/>
     </row>
     <row r="72" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="O72" s="81"/>
-      <c r="P72" s="82"/>
-      <c r="Q72" s="82"/>
-      <c r="R72" s="83"/>
-      <c r="T72" s="81"/>
-      <c r="U72" s="82"/>
-      <c r="V72" s="82"/>
-      <c r="W72" s="83"/>
-      <c r="AD72" s="81"/>
-      <c r="AE72" s="82"/>
-      <c r="AF72" s="82"/>
-      <c r="AG72" s="83"/>
-      <c r="AI72" s="81"/>
-      <c r="AJ72" s="82"/>
-      <c r="AK72" s="82"/>
-      <c r="AL72" s="83"/>
+      <c r="O72" s="76"/>
+      <c r="P72" s="77"/>
+      <c r="Q72" s="77"/>
+      <c r="R72" s="78"/>
+      <c r="T72" s="76"/>
+      <c r="U72" s="77"/>
+      <c r="V72" s="77"/>
+      <c r="W72" s="78"/>
+      <c r="AD72" s="76"/>
+      <c r="AE72" s="77"/>
+      <c r="AF72" s="77"/>
+      <c r="AG72" s="78"/>
+      <c r="AI72" s="76"/>
+      <c r="AJ72" s="77"/>
+      <c r="AK72" s="77"/>
+      <c r="AL72" s="78"/>
     </row>
     <row r="74" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="T74" s="73" t="s">
+      <c r="T74" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="U74" s="73"/>
-      <c r="V74" s="73"/>
-      <c r="W74" s="73"/>
-      <c r="AI74" s="73" t="s">
+      <c r="U74" s="79"/>
+      <c r="V74" s="79"/>
+      <c r="W74" s="79"/>
+      <c r="AI74" s="79" t="s">
         <v>121</v>
       </c>
-      <c r="AJ74" s="73"/>
-      <c r="AK74" s="73"/>
-      <c r="AL74" s="73"/>
+      <c r="AJ74" s="79"/>
+      <c r="AK74" s="79"/>
+      <c r="AL74" s="79"/>
     </row>
     <row r="75" spans="15:38" x14ac:dyDescent="0.25">
       <c r="T75" s="54" t="s">
@@ -5728,71 +5731,71 @@
       <c r="T85" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U85" s="70" t="s">
+      <c r="U85" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="V85" s="71"/>
-      <c r="W85" s="72"/>
+      <c r="V85" s="83"/>
+      <c r="W85" s="84"/>
       <c r="AI85" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ85" s="70" t="s">
+      <c r="AJ85" s="82" t="s">
         <v>134</v>
       </c>
-      <c r="AK85" s="71"/>
-      <c r="AL85" s="72"/>
+      <c r="AK85" s="83"/>
+      <c r="AL85" s="84"/>
     </row>
     <row r="86" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T86" s="74" t="s">
+      <c r="T86" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="U86" s="74"/>
-      <c r="V86" s="74"/>
-      <c r="W86" s="74"/>
-      <c r="AI86" s="74" t="s">
+      <c r="U86" s="80"/>
+      <c r="V86" s="80"/>
+      <c r="W86" s="80"/>
+      <c r="AI86" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="AJ86" s="74"/>
-      <c r="AK86" s="74"/>
-      <c r="AL86" s="74"/>
+      <c r="AJ86" s="80"/>
+      <c r="AK86" s="80"/>
+      <c r="AL86" s="80"/>
     </row>
     <row r="87" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T87" s="75"/>
-      <c r="U87" s="76"/>
-      <c r="V87" s="76"/>
-      <c r="W87" s="77"/>
-      <c r="AI87" s="75"/>
-      <c r="AJ87" s="76"/>
-      <c r="AK87" s="76"/>
-      <c r="AL87" s="77"/>
+      <c r="T87" s="70"/>
+      <c r="U87" s="71"/>
+      <c r="V87" s="71"/>
+      <c r="W87" s="72"/>
+      <c r="AI87" s="70"/>
+      <c r="AJ87" s="71"/>
+      <c r="AK87" s="71"/>
+      <c r="AL87" s="72"/>
     </row>
     <row r="88" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T88" s="78"/>
-      <c r="U88" s="79"/>
-      <c r="V88" s="79"/>
-      <c r="W88" s="80"/>
-      <c r="AI88" s="78"/>
-      <c r="AJ88" s="79"/>
-      <c r="AK88" s="79"/>
-      <c r="AL88" s="80"/>
+      <c r="T88" s="73"/>
+      <c r="U88" s="74"/>
+      <c r="V88" s="74"/>
+      <c r="W88" s="75"/>
+      <c r="AI88" s="73"/>
+      <c r="AJ88" s="74"/>
+      <c r="AK88" s="74"/>
+      <c r="AL88" s="75"/>
     </row>
     <row r="89" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T89" s="81"/>
-      <c r="U89" s="82"/>
-      <c r="V89" s="82"/>
-      <c r="W89" s="83"/>
-      <c r="AI89" s="81"/>
-      <c r="AJ89" s="82"/>
-      <c r="AK89" s="82"/>
-      <c r="AL89" s="83"/>
+      <c r="T89" s="76"/>
+      <c r="U89" s="77"/>
+      <c r="V89" s="77"/>
+      <c r="W89" s="78"/>
+      <c r="AI89" s="76"/>
+      <c r="AJ89" s="77"/>
+      <c r="AK89" s="77"/>
+      <c r="AL89" s="78"/>
     </row>
     <row r="91" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T91" s="73" t="s">
+      <c r="T91" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="U91" s="73"/>
-      <c r="V91" s="73"/>
-      <c r="W91" s="73"/>
+      <c r="U91" s="79"/>
+      <c r="V91" s="79"/>
+      <c r="W91" s="79"/>
     </row>
     <row r="92" spans="20:38" x14ac:dyDescent="0.25">
       <c r="T92" s="54" t="s">
@@ -5936,45 +5939,45 @@
       <c r="T102" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U102" s="70" t="s">
+      <c r="U102" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="V102" s="71"/>
-      <c r="W102" s="72"/>
+      <c r="V102" s="83"/>
+      <c r="W102" s="84"/>
     </row>
     <row r="103" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T103" s="74" t="s">
+      <c r="T103" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="U103" s="74"/>
-      <c r="V103" s="74"/>
-      <c r="W103" s="74"/>
+      <c r="U103" s="80"/>
+      <c r="V103" s="80"/>
+      <c r="W103" s="80"/>
     </row>
     <row r="104" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T104" s="75"/>
-      <c r="U104" s="76"/>
-      <c r="V104" s="76"/>
-      <c r="W104" s="77"/>
+      <c r="T104" s="70"/>
+      <c r="U104" s="71"/>
+      <c r="V104" s="71"/>
+      <c r="W104" s="72"/>
     </row>
     <row r="105" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T105" s="78"/>
-      <c r="U105" s="79"/>
-      <c r="V105" s="79"/>
-      <c r="W105" s="80"/>
+      <c r="T105" s="73"/>
+      <c r="U105" s="74"/>
+      <c r="V105" s="74"/>
+      <c r="W105" s="75"/>
     </row>
     <row r="106" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T106" s="81"/>
-      <c r="U106" s="82"/>
-      <c r="V106" s="82"/>
-      <c r="W106" s="83"/>
+      <c r="T106" s="76"/>
+      <c r="U106" s="77"/>
+      <c r="V106" s="77"/>
+      <c r="W106" s="78"/>
     </row>
     <row r="108" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T108" s="73" t="s">
+      <c r="T108" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="U108" s="73"/>
-      <c r="V108" s="73"/>
-      <c r="W108" s="73"/>
+      <c r="U108" s="79"/>
+      <c r="V108" s="79"/>
+      <c r="W108" s="79"/>
     </row>
     <row r="109" spans="20:23" x14ac:dyDescent="0.25">
       <c r="T109" s="54" t="s">
@@ -6120,134 +6123,40 @@
       <c r="T119" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U119" s="70" t="s">
+      <c r="U119" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="V119" s="71"/>
-      <c r="W119" s="72"/>
+      <c r="V119" s="83"/>
+      <c r="W119" s="84"/>
     </row>
     <row r="120" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T120" s="74" t="s">
+      <c r="T120" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="U120" s="74"/>
-      <c r="V120" s="74"/>
-      <c r="W120" s="74"/>
+      <c r="U120" s="80"/>
+      <c r="V120" s="80"/>
+      <c r="W120" s="80"/>
     </row>
     <row r="121" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T121" s="75"/>
-      <c r="U121" s="76"/>
-      <c r="V121" s="76"/>
-      <c r="W121" s="77"/>
+      <c r="T121" s="70"/>
+      <c r="U121" s="71"/>
+      <c r="V121" s="71"/>
+      <c r="W121" s="72"/>
     </row>
     <row r="122" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T122" s="78"/>
-      <c r="U122" s="79"/>
-      <c r="V122" s="79"/>
-      <c r="W122" s="80"/>
+      <c r="T122" s="73"/>
+      <c r="U122" s="74"/>
+      <c r="V122" s="74"/>
+      <c r="W122" s="75"/>
     </row>
     <row r="123" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T123" s="81"/>
-      <c r="U123" s="82"/>
-      <c r="V123" s="82"/>
-      <c r="W123" s="83"/>
+      <c r="T123" s="76"/>
+      <c r="U123" s="77"/>
+      <c r="V123" s="77"/>
+      <c r="W123" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="116">
-    <mergeCell ref="T121:W123"/>
-    <mergeCell ref="AI40:AL40"/>
-    <mergeCell ref="AI52:AL52"/>
-    <mergeCell ref="AI53:AL55"/>
-    <mergeCell ref="AI57:AL57"/>
-    <mergeCell ref="AI69:AL69"/>
-    <mergeCell ref="AI70:AL72"/>
-    <mergeCell ref="T91:W91"/>
-    <mergeCell ref="T103:W103"/>
-    <mergeCell ref="T104:W106"/>
-    <mergeCell ref="T108:W108"/>
-    <mergeCell ref="T120:W120"/>
-    <mergeCell ref="T69:W69"/>
-    <mergeCell ref="T70:W72"/>
-    <mergeCell ref="T74:W74"/>
-    <mergeCell ref="T86:W86"/>
-    <mergeCell ref="O70:R72"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="T18:W18"/>
-    <mergeCell ref="T19:W21"/>
-    <mergeCell ref="T23:W23"/>
-    <mergeCell ref="T35:W35"/>
-    <mergeCell ref="T36:W38"/>
-    <mergeCell ref="T40:W40"/>
-    <mergeCell ref="T52:W52"/>
-    <mergeCell ref="T53:W55"/>
-    <mergeCell ref="O40:R40"/>
-    <mergeCell ref="O52:R52"/>
-    <mergeCell ref="O53:R55"/>
-    <mergeCell ref="O57:R57"/>
-    <mergeCell ref="O69:R69"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J36:M38"/>
-    <mergeCell ref="O36:R38"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M55"/>
-    <mergeCell ref="P68:R68"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="O19:R21"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="O35:R35"/>
-    <mergeCell ref="Y6:AB6"/>
-    <mergeCell ref="Y18:AB18"/>
-    <mergeCell ref="Y19:AB21"/>
-    <mergeCell ref="Y23:AB23"/>
-    <mergeCell ref="Y35:AB35"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="J19:M21"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="AS6:AV6"/>
-    <mergeCell ref="AS18:AV18"/>
-    <mergeCell ref="AS19:AV21"/>
-    <mergeCell ref="AD36:AG38"/>
-    <mergeCell ref="AI6:AL6"/>
-    <mergeCell ref="AI18:AL18"/>
-    <mergeCell ref="AI19:AL21"/>
-    <mergeCell ref="AI23:AL23"/>
-    <mergeCell ref="AI35:AL35"/>
-    <mergeCell ref="AI36:AL38"/>
-    <mergeCell ref="AD6:AG6"/>
-    <mergeCell ref="AD18:AG18"/>
-    <mergeCell ref="AD19:AG21"/>
-    <mergeCell ref="AD23:AG23"/>
-    <mergeCell ref="AD35:AG35"/>
-    <mergeCell ref="AN18:AQ18"/>
-    <mergeCell ref="AN19:AQ21"/>
-    <mergeCell ref="AN6:AQ6"/>
-    <mergeCell ref="AD40:AG40"/>
-    <mergeCell ref="AD52:AG52"/>
-    <mergeCell ref="AD53:AG55"/>
-    <mergeCell ref="AD57:AG57"/>
-    <mergeCell ref="AE17:AG17"/>
-    <mergeCell ref="AJ17:AL17"/>
-    <mergeCell ref="AO17:AQ17"/>
-    <mergeCell ref="AE51:AG51"/>
-    <mergeCell ref="AJ51:AL51"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="Z17:AB17"/>
-    <mergeCell ref="U34:W34"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="Z51:AB51"/>
-    <mergeCell ref="U51:W51"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="K51:M51"/>
     <mergeCell ref="Y36:AB38"/>
     <mergeCell ref="U119:W119"/>
     <mergeCell ref="AE68:AG68"/>
@@ -6270,6 +6179,100 @@
     <mergeCell ref="T57:W57"/>
     <mergeCell ref="U68:W68"/>
     <mergeCell ref="T87:W89"/>
+    <mergeCell ref="AS6:AV6"/>
+    <mergeCell ref="AS18:AV18"/>
+    <mergeCell ref="AS19:AV21"/>
+    <mergeCell ref="AD36:AG38"/>
+    <mergeCell ref="AI6:AL6"/>
+    <mergeCell ref="AI18:AL18"/>
+    <mergeCell ref="AI19:AL21"/>
+    <mergeCell ref="AI23:AL23"/>
+    <mergeCell ref="AI35:AL35"/>
+    <mergeCell ref="AI36:AL38"/>
+    <mergeCell ref="AD6:AG6"/>
+    <mergeCell ref="AD18:AG18"/>
+    <mergeCell ref="AD19:AG21"/>
+    <mergeCell ref="AD23:AG23"/>
+    <mergeCell ref="AD35:AG35"/>
+    <mergeCell ref="AN18:AQ18"/>
+    <mergeCell ref="AN19:AQ21"/>
+    <mergeCell ref="AN6:AQ6"/>
+    <mergeCell ref="AE17:AG17"/>
+    <mergeCell ref="AJ17:AL17"/>
+    <mergeCell ref="AO17:AQ17"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="Y18:AB18"/>
+    <mergeCell ref="Y19:AB21"/>
+    <mergeCell ref="Y23:AB23"/>
+    <mergeCell ref="Y35:AB35"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J19:M21"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="Z17:AB17"/>
+    <mergeCell ref="U34:W34"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J36:M38"/>
+    <mergeCell ref="O36:R38"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M55"/>
+    <mergeCell ref="P68:R68"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="O19:R21"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O35:R35"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="O70:R72"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="T19:W21"/>
+    <mergeCell ref="T23:W23"/>
+    <mergeCell ref="T35:W35"/>
+    <mergeCell ref="T36:W38"/>
+    <mergeCell ref="T40:W40"/>
+    <mergeCell ref="T52:W52"/>
+    <mergeCell ref="T53:W55"/>
+    <mergeCell ref="O40:R40"/>
+    <mergeCell ref="O52:R52"/>
+    <mergeCell ref="O53:R55"/>
+    <mergeCell ref="O57:R57"/>
+    <mergeCell ref="O69:R69"/>
+    <mergeCell ref="U51:W51"/>
+    <mergeCell ref="T121:W123"/>
+    <mergeCell ref="AI40:AL40"/>
+    <mergeCell ref="AI52:AL52"/>
+    <mergeCell ref="AI53:AL55"/>
+    <mergeCell ref="AI57:AL57"/>
+    <mergeCell ref="AI69:AL69"/>
+    <mergeCell ref="AI70:AL72"/>
+    <mergeCell ref="T91:W91"/>
+    <mergeCell ref="T103:W103"/>
+    <mergeCell ref="T104:W106"/>
+    <mergeCell ref="T108:W108"/>
+    <mergeCell ref="T120:W120"/>
+    <mergeCell ref="T69:W69"/>
+    <mergeCell ref="T70:W72"/>
+    <mergeCell ref="T74:W74"/>
+    <mergeCell ref="T86:W86"/>
+    <mergeCell ref="AD40:AG40"/>
+    <mergeCell ref="AD52:AG52"/>
+    <mergeCell ref="AD53:AG55"/>
+    <mergeCell ref="AD57:AG57"/>
+    <mergeCell ref="AE51:AG51"/>
+    <mergeCell ref="AJ51:AL51"/>
+    <mergeCell ref="Z51:AB51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6280,7 +6283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
@@ -6297,13 +6300,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
@@ -6315,15 +6318,15 @@
       <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="F4" s="87" t="s">
+      <c r="B4" s="85"/>
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -6343,12 +6346,12 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
@@ -6632,10 +6635,10 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="87"/>
+      <c r="B16" s="85"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -6657,19 +6660,19 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="70" t="s">
+      <c r="K17" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="L17" s="71"/>
-      <c r="M17" s="72"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="84"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="74" t="s">
+      <c r="J18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -6681,10 +6684,10 @@
       <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="75"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="77"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="72"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
@@ -6697,10 +6700,10 @@
         <f t="shared" ref="C20:C27" si="0">C7+($C$19-1)*(D7-C7)/98</f>
         <v>70</v>
       </c>
-      <c r="J20" s="78"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="80"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="75"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
@@ -6713,10 +6716,10 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J21" s="81"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="82"/>
-      <c r="M21" s="83"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="78"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -6741,12 +6744,12 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J23" s="73" t="s">
+      <c r="J23" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="73"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
@@ -6932,45 +6935,45 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="70" t="s">
+      <c r="K34" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="71"/>
-      <c r="M34" s="72"/>
+      <c r="L34" s="83"/>
+      <c r="M34" s="84"/>
     </row>
     <row r="35" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J35" s="74" t="s">
+      <c r="J35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="74"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
     </row>
     <row r="36" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J36" s="75"/>
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="77"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="72"/>
     </row>
     <row r="37" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J37" s="78"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="80"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="74"/>
+      <c r="L37" s="74"/>
+      <c r="M37" s="75"/>
     </row>
     <row r="38" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J38" s="81"/>
-      <c r="K38" s="82"/>
-      <c r="L38" s="82"/>
-      <c r="M38" s="83"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="77"/>
+      <c r="L38" s="77"/>
+      <c r="M38" s="78"/>
     </row>
     <row r="40" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J40" s="73" t="s">
+      <c r="J40" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="K40" s="73"/>
-      <c r="L40" s="73"/>
-      <c r="M40" s="73"/>
+      <c r="K40" s="79"/>
+      <c r="L40" s="79"/>
+      <c r="M40" s="79"/>
     </row>
     <row r="41" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -7116,47 +7119,40 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="70" t="s">
+      <c r="K51" s="82" t="s">
         <v>139</v>
       </c>
-      <c r="L51" s="71"/>
-      <c r="M51" s="72"/>
+      <c r="L51" s="83"/>
+      <c r="M51" s="84"/>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J52" s="74" t="s">
+      <c r="J52" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="74"/>
-      <c r="L52" s="74"/>
-      <c r="M52" s="74"/>
+      <c r="K52" s="80"/>
+      <c r="L52" s="80"/>
+      <c r="M52" s="80"/>
     </row>
     <row r="53" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J53" s="75"/>
-      <c r="K53" s="76"/>
-      <c r="L53" s="76"/>
-      <c r="M53" s="77"/>
+      <c r="J53" s="70"/>
+      <c r="K53" s="71"/>
+      <c r="L53" s="71"/>
+      <c r="M53" s="72"/>
     </row>
     <row r="54" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J54" s="78"/>
-      <c r="K54" s="79"/>
-      <c r="L54" s="79"/>
-      <c r="M54" s="80"/>
+      <c r="J54" s="73"/>
+      <c r="K54" s="74"/>
+      <c r="L54" s="74"/>
+      <c r="M54" s="75"/>
     </row>
     <row r="55" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J55" s="81"/>
-      <c r="K55" s="82"/>
-      <c r="L55" s="82"/>
-      <c r="M55" s="83"/>
+      <c r="J55" s="76"/>
+      <c r="K55" s="77"/>
+      <c r="L55" s="77"/>
+      <c r="M55" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="K17:M17"/>
     <mergeCell ref="J40:M40"/>
     <mergeCell ref="J52:M52"/>
     <mergeCell ref="J53:M55"/>
@@ -7166,6 +7162,13 @@
     <mergeCell ref="J36:M38"/>
     <mergeCell ref="K34:M34"/>
     <mergeCell ref="K51:M51"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="K17:M17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7175,7 +7178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="E10" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
@@ -7192,13 +7195,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -7210,15 +7213,15 @@
       <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="F4" s="87" t="s">
+      <c r="B4" s="85"/>
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -7238,24 +7241,24 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="79" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="O6" s="73" t="s">
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="O6" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
-      <c r="T6" s="73" t="s">
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="T6" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="U6" s="73"/>
-      <c r="V6" s="73"/>
-      <c r="W6" s="73"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
@@ -7753,10 +7756,10 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="87"/>
+      <c r="B16" s="85"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -7804,47 +7807,47 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="70" t="s">
+      <c r="K17" s="82" t="s">
         <v>135</v>
       </c>
-      <c r="L17" s="71"/>
-      <c r="M17" s="72"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="84"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="70" t="s">
+      <c r="P17" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="72"/>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="84"/>
       <c r="T17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U17" s="70" t="s">
+      <c r="U17" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="V17" s="71"/>
-      <c r="W17" s="72"/>
+      <c r="V17" s="83"/>
+      <c r="W17" s="84"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J18" s="74" t="s">
+      <c r="J18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
-      <c r="O18" s="74" t="s">
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
+      <c r="O18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
-      <c r="T18" s="74" t="s">
+      <c r="P18" s="80"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="80"/>
+      <c r="T18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="U18" s="74"/>
-      <c r="V18" s="74"/>
-      <c r="W18" s="74"/>
+      <c r="U18" s="80"/>
+      <c r="V18" s="80"/>
+      <c r="W18" s="80"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -7856,18 +7859,18 @@
       <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="75"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="77"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="76"/>
-      <c r="R19" s="77"/>
-      <c r="T19" s="75"/>
-      <c r="U19" s="76"/>
-      <c r="V19" s="76"/>
-      <c r="W19" s="77"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="72"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="71"/>
+      <c r="Q19" s="71"/>
+      <c r="R19" s="72"/>
+      <c r="T19" s="70"/>
+      <c r="U19" s="71"/>
+      <c r="V19" s="71"/>
+      <c r="W19" s="72"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
@@ -7880,18 +7883,18 @@
         <f t="shared" ref="C20:C27" si="0">C7+($C$19-1)*(D7-C7)/98</f>
         <v>70</v>
       </c>
-      <c r="J20" s="78"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="80"/>
-      <c r="O20" s="78"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="80"/>
-      <c r="T20" s="78"/>
-      <c r="U20" s="79"/>
-      <c r="V20" s="79"/>
-      <c r="W20" s="80"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="75"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="74"/>
+      <c r="Q20" s="74"/>
+      <c r="R20" s="75"/>
+      <c r="T20" s="73"/>
+      <c r="U20" s="74"/>
+      <c r="V20" s="74"/>
+      <c r="W20" s="75"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
@@ -7904,18 +7907,18 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J21" s="81"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="82"/>
-      <c r="M21" s="83"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="82"/>
-      <c r="Q21" s="82"/>
-      <c r="R21" s="83"/>
-      <c r="T21" s="81"/>
-      <c r="U21" s="82"/>
-      <c r="V21" s="82"/>
-      <c r="W21" s="83"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="78"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="77"/>
+      <c r="Q21" s="77"/>
+      <c r="R21" s="78"/>
+      <c r="T21" s="76"/>
+      <c r="U21" s="77"/>
+      <c r="V21" s="77"/>
+      <c r="W21" s="78"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -7940,18 +7943,18 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J23" s="73" t="s">
+      <c r="J23" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="73"/>
-      <c r="O23" s="73" t="s">
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="O23" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="P23" s="73"/>
-      <c r="Q23" s="73"/>
-      <c r="R23" s="73"/>
+      <c r="P23" s="79"/>
+      <c r="Q23" s="79"/>
+      <c r="R23" s="79"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
@@ -8257,71 +8260,71 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="70" t="s">
+      <c r="K34" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="71"/>
-      <c r="M34" s="72"/>
+      <c r="L34" s="83"/>
+      <c r="M34" s="84"/>
       <c r="O34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P34" s="70" t="s">
+      <c r="P34" s="82" t="s">
         <v>137</v>
       </c>
-      <c r="Q34" s="71"/>
-      <c r="R34" s="72"/>
+      <c r="Q34" s="83"/>
+      <c r="R34" s="84"/>
     </row>
     <row r="35" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J35" s="74" t="s">
+      <c r="J35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="74"/>
-      <c r="O35" s="74" t="s">
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
+      <c r="O35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="P35" s="74"/>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="74"/>
+      <c r="P35" s="80"/>
+      <c r="Q35" s="80"/>
+      <c r="R35" s="80"/>
     </row>
     <row r="36" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J36" s="75"/>
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="77"/>
-      <c r="O36" s="75"/>
-      <c r="P36" s="76"/>
-      <c r="Q36" s="76"/>
-      <c r="R36" s="77"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="72"/>
+      <c r="O36" s="70"/>
+      <c r="P36" s="71"/>
+      <c r="Q36" s="71"/>
+      <c r="R36" s="72"/>
     </row>
     <row r="37" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J37" s="78"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="80"/>
-      <c r="O37" s="78"/>
-      <c r="P37" s="79"/>
-      <c r="Q37" s="79"/>
-      <c r="R37" s="80"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="74"/>
+      <c r="L37" s="74"/>
+      <c r="M37" s="75"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="74"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="75"/>
     </row>
     <row r="38" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J38" s="81"/>
-      <c r="K38" s="82"/>
-      <c r="L38" s="82"/>
-      <c r="M38" s="83"/>
-      <c r="O38" s="81"/>
-      <c r="P38" s="82"/>
-      <c r="Q38" s="82"/>
-      <c r="R38" s="83"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="77"/>
+      <c r="L38" s="77"/>
+      <c r="M38" s="78"/>
+      <c r="O38" s="76"/>
+      <c r="P38" s="77"/>
+      <c r="Q38" s="77"/>
+      <c r="R38" s="78"/>
     </row>
     <row r="40" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="O40" s="73" t="s">
+      <c r="O40" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="P40" s="73"/>
-      <c r="Q40" s="73"/>
-      <c r="R40" s="73"/>
+      <c r="P40" s="79"/>
+      <c r="Q40" s="79"/>
+      <c r="R40" s="79"/>
     </row>
     <row r="41" spans="10:18" x14ac:dyDescent="0.25">
       <c r="O41" s="54" t="s">
@@ -8467,50 +8470,45 @@
       <c r="O51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P51" s="70" t="s">
+      <c r="P51" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="Q51" s="71"/>
-      <c r="R51" s="72"/>
+      <c r="Q51" s="83"/>
+      <c r="R51" s="84"/>
     </row>
     <row r="52" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O52" s="74" t="s">
+      <c r="O52" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="P52" s="74"/>
-      <c r="Q52" s="74"/>
-      <c r="R52" s="74"/>
+      <c r="P52" s="80"/>
+      <c r="Q52" s="80"/>
+      <c r="R52" s="80"/>
     </row>
     <row r="53" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O53" s="75"/>
-      <c r="P53" s="76"/>
-      <c r="Q53" s="76"/>
-      <c r="R53" s="77"/>
+      <c r="O53" s="70"/>
+      <c r="P53" s="71"/>
+      <c r="Q53" s="71"/>
+      <c r="R53" s="72"/>
     </row>
     <row r="54" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O54" s="78"/>
-      <c r="P54" s="79"/>
-      <c r="Q54" s="79"/>
-      <c r="R54" s="80"/>
+      <c r="O54" s="73"/>
+      <c r="P54" s="74"/>
+      <c r="Q54" s="74"/>
+      <c r="R54" s="75"/>
     </row>
     <row r="55" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O55" s="81"/>
-      <c r="P55" s="82"/>
-      <c r="Q55" s="82"/>
-      <c r="R55" s="83"/>
+      <c r="O55" s="76"/>
+      <c r="P55" s="77"/>
+      <c r="Q55" s="77"/>
+      <c r="R55" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="O40:R40"/>
-    <mergeCell ref="O52:R52"/>
-    <mergeCell ref="O53:R55"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="T18:W18"/>
-    <mergeCell ref="T19:W21"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
     <mergeCell ref="J19:M21"/>
     <mergeCell ref="J23:M23"/>
     <mergeCell ref="J35:M35"/>
@@ -8524,11 +8522,16 @@
     <mergeCell ref="J18:M18"/>
     <mergeCell ref="K17:M17"/>
     <mergeCell ref="K34:M34"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="O40:R40"/>
+    <mergeCell ref="O52:R52"/>
+    <mergeCell ref="O53:R55"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="T19:W21"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="U17:W17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8553,13 +8556,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
@@ -8571,15 +8574,15 @@
       <c r="E2" s="17"/>
     </row>
     <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="F4" s="87" t="s">
+      <c r="B4" s="85"/>
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -8599,18 +8602,18 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="O6" s="73" t="s">
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="O6" s="79" t="s">
         <v>76</v>
       </c>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
@@ -9001,10 +9004,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="87"/>
+      <c r="B16" s="85"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -9039,33 +9042,33 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="70" t="s">
+      <c r="K17" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="L17" s="71"/>
-      <c r="M17" s="72"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="84"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="70" t="s">
+      <c r="P17" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="72"/>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="84"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J18" s="74" t="s">
+      <c r="J18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
-      <c r="O18" s="74" t="s">
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
+      <c r="O18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
+      <c r="P18" s="80"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="80"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -9077,14 +9080,14 @@
       <c r="C19" s="13">
         <v>6</v>
       </c>
-      <c r="J19" s="75"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="77"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="76"/>
-      <c r="R19" s="77"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="72"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="71"/>
+      <c r="Q19" s="71"/>
+      <c r="R19" s="72"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
@@ -9097,14 +9100,14 @@
         <f t="shared" ref="C20:C27" si="0">C7+($C$19-1)*(D7-C7)/98</f>
         <v>423.57142857142856</v>
       </c>
-      <c r="J20" s="78"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="80"/>
-      <c r="O20" s="78"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="80"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="75"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="74"/>
+      <c r="Q20" s="74"/>
+      <c r="R20" s="75"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
@@ -9117,14 +9120,14 @@
         <f t="shared" si="0"/>
         <v>90.765306122448976</v>
       </c>
-      <c r="J21" s="81"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="82"/>
-      <c r="M21" s="83"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="82"/>
-      <c r="Q21" s="82"/>
-      <c r="R21" s="83"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="78"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="77"/>
+      <c r="Q21" s="77"/>
+      <c r="R21" s="78"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -9149,18 +9152,18 @@
         <f t="shared" si="0"/>
         <v>29.54081632653061</v>
       </c>
-      <c r="J23" s="73" t="s">
+      <c r="J23" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="73"/>
-      <c r="O23" s="73" t="s">
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="O23" s="79" t="s">
         <v>84</v>
       </c>
-      <c r="P23" s="73"/>
-      <c r="Q23" s="73"/>
-      <c r="R23" s="73"/>
+      <c r="P23" s="79"/>
+      <c r="Q23" s="79"/>
+      <c r="R23" s="79"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
@@ -9466,71 +9469,71 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="70" t="s">
+      <c r="K34" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="71"/>
-      <c r="M34" s="72"/>
+      <c r="L34" s="83"/>
+      <c r="M34" s="84"/>
       <c r="O34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P34" s="70" t="s">
+      <c r="P34" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="Q34" s="71"/>
-      <c r="R34" s="72"/>
+      <c r="Q34" s="83"/>
+      <c r="R34" s="84"/>
     </row>
     <row r="35" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J35" s="74" t="s">
+      <c r="J35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="74"/>
-      <c r="O35" s="74" t="s">
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
+      <c r="O35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="P35" s="74"/>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="74"/>
+      <c r="P35" s="80"/>
+      <c r="Q35" s="80"/>
+      <c r="R35" s="80"/>
     </row>
     <row r="36" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J36" s="75"/>
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="77"/>
-      <c r="O36" s="75"/>
-      <c r="P36" s="76"/>
-      <c r="Q36" s="76"/>
-      <c r="R36" s="77"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="72"/>
+      <c r="O36" s="70"/>
+      <c r="P36" s="71"/>
+      <c r="Q36" s="71"/>
+      <c r="R36" s="72"/>
     </row>
     <row r="37" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J37" s="78"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="80"/>
-      <c r="O37" s="78"/>
-      <c r="P37" s="79"/>
-      <c r="Q37" s="79"/>
-      <c r="R37" s="80"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="74"/>
+      <c r="L37" s="74"/>
+      <c r="M37" s="75"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="74"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="75"/>
     </row>
     <row r="38" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J38" s="81"/>
-      <c r="K38" s="82"/>
-      <c r="L38" s="82"/>
-      <c r="M38" s="83"/>
-      <c r="O38" s="81"/>
-      <c r="P38" s="82"/>
-      <c r="Q38" s="82"/>
-      <c r="R38" s="83"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="77"/>
+      <c r="L38" s="77"/>
+      <c r="M38" s="78"/>
+      <c r="O38" s="76"/>
+      <c r="P38" s="77"/>
+      <c r="Q38" s="77"/>
+      <c r="R38" s="78"/>
     </row>
     <row r="40" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J40" s="73" t="s">
+      <c r="J40" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="K40" s="73"/>
-      <c r="L40" s="73"/>
-      <c r="M40" s="73"/>
+      <c r="K40" s="79"/>
+      <c r="L40" s="79"/>
+      <c r="M40" s="79"/>
     </row>
     <row r="41" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -9676,45 +9679,45 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="70" t="s">
+      <c r="K51" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="L51" s="71"/>
-      <c r="M51" s="72"/>
+      <c r="L51" s="83"/>
+      <c r="M51" s="84"/>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J52" s="74" t="s">
+      <c r="J52" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="74"/>
-      <c r="L52" s="74"/>
-      <c r="M52" s="74"/>
+      <c r="K52" s="80"/>
+      <c r="L52" s="80"/>
+      <c r="M52" s="80"/>
     </row>
     <row r="53" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J53" s="75"/>
-      <c r="K53" s="76"/>
-      <c r="L53" s="76"/>
-      <c r="M53" s="77"/>
+      <c r="J53" s="70"/>
+      <c r="K53" s="71"/>
+      <c r="L53" s="71"/>
+      <c r="M53" s="72"/>
     </row>
     <row r="54" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J54" s="78"/>
-      <c r="K54" s="79"/>
-      <c r="L54" s="79"/>
-      <c r="M54" s="80"/>
+      <c r="J54" s="73"/>
+      <c r="K54" s="74"/>
+      <c r="L54" s="74"/>
+      <c r="M54" s="75"/>
     </row>
     <row r="55" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J55" s="81"/>
-      <c r="K55" s="82"/>
-      <c r="L55" s="82"/>
-      <c r="M55" s="83"/>
+      <c r="J55" s="76"/>
+      <c r="K55" s="77"/>
+      <c r="L55" s="77"/>
+      <c r="M55" s="78"/>
     </row>
     <row r="57" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J57" s="73" t="s">
+      <c r="J57" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="K57" s="73"/>
-      <c r="L57" s="73"/>
-      <c r="M57" s="73"/>
+      <c r="K57" s="79"/>
+      <c r="L57" s="79"/>
+      <c r="M57" s="79"/>
     </row>
     <row r="58" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J58" s="54" t="s">
@@ -9860,52 +9863,40 @@
       <c r="J68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K68" s="70" t="s">
+      <c r="K68" s="82" t="s">
         <v>128</v>
       </c>
-      <c r="L68" s="71"/>
-      <c r="M68" s="72"/>
+      <c r="L68" s="83"/>
+      <c r="M68" s="84"/>
     </row>
     <row r="69" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J69" s="74" t="s">
+      <c r="J69" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K69" s="74"/>
-      <c r="L69" s="74"/>
-      <c r="M69" s="74"/>
+      <c r="K69" s="80"/>
+      <c r="L69" s="80"/>
+      <c r="M69" s="80"/>
     </row>
     <row r="70" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J70" s="75"/>
-      <c r="K70" s="76"/>
-      <c r="L70" s="76"/>
-      <c r="M70" s="77"/>
+      <c r="J70" s="70"/>
+      <c r="K70" s="71"/>
+      <c r="L70" s="71"/>
+      <c r="M70" s="72"/>
     </row>
     <row r="71" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J71" s="78"/>
-      <c r="K71" s="79"/>
-      <c r="L71" s="79"/>
-      <c r="M71" s="80"/>
+      <c r="J71" s="73"/>
+      <c r="K71" s="74"/>
+      <c r="L71" s="74"/>
+      <c r="M71" s="75"/>
     </row>
     <row r="72" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J72" s="81"/>
-      <c r="K72" s="82"/>
-      <c r="L72" s="82"/>
-      <c r="M72" s="83"/>
+      <c r="J72" s="76"/>
+      <c r="K72" s="77"/>
+      <c r="L72" s="77"/>
+      <c r="M72" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="O19:R21"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="O35:R35"/>
-    <mergeCell ref="O36:R38"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="P34:R34"/>
     <mergeCell ref="J57:M57"/>
     <mergeCell ref="J69:M69"/>
     <mergeCell ref="J70:M72"/>
@@ -9922,6 +9913,18 @@
     <mergeCell ref="J52:M52"/>
     <mergeCell ref="J53:M55"/>
     <mergeCell ref="K51:M51"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="O19:R21"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O35:R35"/>
+    <mergeCell ref="O36:R38"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="P34:R34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9931,8 +9934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69:M69"/>
+    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P58" sqref="P58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9946,13 +9949,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -9960,15 +9963,15 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="F4" s="87" t="s">
+      <c r="B4" s="85"/>
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -9988,18 +9991,18 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="73" t="s">
+      <c r="J6" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="73"/>
-      <c r="O6" s="73" t="s">
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="O6" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="73"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
@@ -10402,10 +10405,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="87" t="s">
+      <c r="A16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="87"/>
+      <c r="B16" s="85"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -10440,31 +10443,31 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="70" t="s">
+      <c r="K17" s="82" t="s">
         <v>137</v>
       </c>
-      <c r="L17" s="71"/>
-      <c r="M17" s="72"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="84"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="72"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="83"/>
+      <c r="R17" s="84"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J18" s="74" t="s">
+      <c r="J18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
-      <c r="O18" s="74" t="s">
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
+      <c r="O18" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
+      <c r="P18" s="80"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="80"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -10476,13 +10479,13 @@
       <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="88" t="s">
+      <c r="J19" s="81" t="s">
         <v>75</v>
       </c>
       <c r="K19" s="89"/>
       <c r="L19" s="89"/>
       <c r="M19" s="90"/>
-      <c r="O19" s="88" t="s">
+      <c r="O19" s="81" t="s">
         <v>99</v>
       </c>
       <c r="P19" s="89"/>
@@ -10552,12 +10555,12 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J23" s="73" t="s">
+      <c r="J23" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
-      <c r="M23" s="73"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
@@ -10743,22 +10746,22 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="70" t="s">
+      <c r="K34" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="L34" s="71"/>
-      <c r="M34" s="72"/>
+      <c r="L34" s="83"/>
+      <c r="M34" s="84"/>
     </row>
     <row r="35" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J35" s="74" t="s">
+      <c r="J35" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="74"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
     </row>
     <row r="36" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J36" s="88" t="s">
+      <c r="J36" s="81" t="s">
         <v>79</v>
       </c>
       <c r="K36" s="89"/>
@@ -10778,12 +10781,12 @@
       <c r="M38" s="96"/>
     </row>
     <row r="40" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J40" s="73" t="s">
+      <c r="J40" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="K40" s="73"/>
-      <c r="L40" s="73"/>
-      <c r="M40" s="73"/>
+      <c r="K40" s="79"/>
+      <c r="L40" s="79"/>
+      <c r="M40" s="79"/>
     </row>
     <row r="41" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -10929,20 +10932,22 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="70"/>
-      <c r="L51" s="71"/>
-      <c r="M51" s="72"/>
+      <c r="K51" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="L51" s="83"/>
+      <c r="M51" s="84"/>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J52" s="74" t="s">
+      <c r="J52" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="74"/>
-      <c r="L52" s="74"/>
-      <c r="M52" s="74"/>
+      <c r="K52" s="80"/>
+      <c r="L52" s="80"/>
+      <c r="M52" s="80"/>
     </row>
     <row r="53" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J53" s="88" t="s">
+      <c r="J53" s="81" t="s">
         <v>86</v>
       </c>
       <c r="K53" s="89"/>
@@ -10962,12 +10967,12 @@
       <c r="M55" s="96"/>
     </row>
     <row r="57" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J57" s="73" t="s">
+      <c r="J57" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="K57" s="73"/>
-      <c r="L57" s="73"/>
-      <c r="M57" s="73"/>
+      <c r="K57" s="79"/>
+      <c r="L57" s="79"/>
+      <c r="M57" s="79"/>
     </row>
     <row r="58" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J58" s="54" t="s">
@@ -11113,22 +11118,22 @@
       <c r="J68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K68" s="70" t="s">
+      <c r="K68" s="82" t="s">
         <v>128</v>
       </c>
-      <c r="L68" s="71"/>
-      <c r="M68" s="72"/>
+      <c r="L68" s="83"/>
+      <c r="M68" s="84"/>
     </row>
     <row r="69" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J69" s="74" t="s">
+      <c r="J69" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K69" s="74"/>
-      <c r="L69" s="74"/>
-      <c r="M69" s="74"/>
+      <c r="K69" s="80"/>
+      <c r="L69" s="80"/>
+      <c r="M69" s="80"/>
     </row>
     <row r="70" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J70" s="88" t="s">
+      <c r="J70" s="81" t="s">
         <v>101</v>
       </c>
       <c r="K70" s="89"/>
@@ -11148,12 +11153,12 @@
       <c r="M72" s="96"/>
     </row>
     <row r="74" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J74" s="73" t="s">
+      <c r="J74" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="K74" s="73"/>
-      <c r="L74" s="73"/>
-      <c r="M74" s="73"/>
+      <c r="K74" s="79"/>
+      <c r="L74" s="79"/>
+      <c r="M74" s="79"/>
     </row>
     <row r="75" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J75" s="54" t="s">
@@ -11299,22 +11304,22 @@
       <c r="J85" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K85" s="70" t="s">
+      <c r="K85" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="L85" s="71"/>
-      <c r="M85" s="72"/>
+      <c r="L85" s="83"/>
+      <c r="M85" s="84"/>
     </row>
     <row r="86" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J86" s="74" t="s">
+      <c r="J86" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="K86" s="74"/>
-      <c r="L86" s="74"/>
-      <c r="M86" s="74"/>
+      <c r="K86" s="80"/>
+      <c r="L86" s="80"/>
+      <c r="M86" s="80"/>
     </row>
     <row r="87" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J87" s="88" t="s">
+      <c r="J87" s="81" t="s">
         <v>108</v>
       </c>
       <c r="K87" s="89"/>
@@ -11335,21 +11340,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="J19:M21"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="O19:R21"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="K34:M34"/>
     <mergeCell ref="J36:M38"/>
     <mergeCell ref="J74:M74"/>
     <mergeCell ref="J86:M86"/>
@@ -11363,6 +11353,21 @@
     <mergeCell ref="K51:M51"/>
     <mergeCell ref="K68:M68"/>
     <mergeCell ref="K85:M85"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="J19:M21"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="O19:R21"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Memory Sprites, Witch Work
Memory sprites and accompanying enemies/stats created for the following:
-slime
-stupid rat
-spider
-mountain ogre
-ghoul cart
-tritops
-grumpy fish
-chubby fish

1 out of 2 extreme difficult enemies created:
-Enchantress
See puzzle room example for fight with Lvl 10 Tak, Vero, Witch

Witch now has starting weapons/armor. Dummy potions have realistic
effects. An additional weapon for witch has been created (cursed
pitchfork) but not placed in game.

All spreadsheets and MATLAB code is updated.
</commit_message>
<xml_diff>
--- a/Weapons and Armor.xlsx
+++ b/Weapons and Armor.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\electabuzz\Documents\RPGVXAce\Reminiscence_local\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="12435" windowHeight="7740"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="12435" windowHeight="7740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="1" r:id="rId1"/>
@@ -13,12 +18,12 @@
     <sheet name="Head" sheetId="4" r:id="rId4"/>
     <sheet name="Accessory" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="151">
   <si>
     <t>Reminiscence Weapons and Armor</t>
   </si>
@@ -446,12 +451,42 @@
   </si>
   <si>
     <t>Mine B1</t>
+  </si>
+  <si>
+    <t>Cursed</t>
+  </si>
+  <si>
+    <t>Witch Start</t>
+  </si>
+  <si>
+    <t>Cursed Scythe</t>
+  </si>
+  <si>
+    <t>Cursed Pitchfork</t>
+  </si>
+  <si>
+    <t>To be placed in time dungeon</t>
+  </si>
+  <si>
+    <t>Witch's Cloak</t>
+  </si>
+  <si>
+    <t>Magic Armor</t>
+  </si>
+  <si>
+    <t>Witch's Hat</t>
+  </si>
+  <si>
+    <t>Witch's Boots</t>
+  </si>
+  <si>
+    <t>Slight resistence to poison, confusion, paralysis, freeze, and burn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -977,15 +1012,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -995,7 +1021,10 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1005,6 +1034,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1051,6 +1086,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1099,7 +1137,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1132,9 +1170,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1167,6 +1222,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1343,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV123"/>
+  <dimension ref="A1:BA123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O69" sqref="O69:R69"/>
+    <sheetView topLeftCell="R1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AY30" sqref="AY30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,16 +1430,16 @@
     <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-    </row>
-    <row r="2" spans="1:48" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:53" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+    </row>
+    <row r="2" spans="1:53" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>31</v>
       </c>
@@ -1376,20 +1448,20 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="85" t="s">
+    <row r="4" spans="1:53" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="85"/>
+      <c r="B4" s="88"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="F4" s="85" t="s">
+      <c r="F4" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-    </row>
-    <row r="5" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+    </row>
+    <row r="5" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="12"/>
@@ -1398,7 +1470,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="10" t="s">
@@ -1410,56 +1482,62 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="79" t="s">
+      <c r="J6" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="O6" s="79" t="s">
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="O6" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="79"/>
-      <c r="T6" s="79" t="s">
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="T6" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="U6" s="79"/>
-      <c r="V6" s="79"/>
-      <c r="W6" s="79"/>
-      <c r="Y6" s="79" t="s">
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="82"/>
+      <c r="Y6" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="Z6" s="79"/>
-      <c r="AA6" s="79"/>
-      <c r="AB6" s="79"/>
-      <c r="AD6" s="79" t="s">
+      <c r="Z6" s="82"/>
+      <c r="AA6" s="82"/>
+      <c r="AB6" s="82"/>
+      <c r="AD6" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="AE6" s="79"/>
-      <c r="AF6" s="79"/>
-      <c r="AG6" s="79"/>
-      <c r="AI6" s="79" t="s">
+      <c r="AE6" s="82"/>
+      <c r="AF6" s="82"/>
+      <c r="AG6" s="82"/>
+      <c r="AI6" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="AJ6" s="79"/>
-      <c r="AK6" s="79"/>
-      <c r="AL6" s="79"/>
-      <c r="AN6" s="79" t="s">
+      <c r="AJ6" s="82"/>
+      <c r="AK6" s="82"/>
+      <c r="AL6" s="82"/>
+      <c r="AN6" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="AO6" s="79"/>
-      <c r="AP6" s="79"/>
-      <c r="AQ6" s="79"/>
-      <c r="AS6" s="79" t="s">
+      <c r="AO6" s="82"/>
+      <c r="AP6" s="82"/>
+      <c r="AQ6" s="82"/>
+      <c r="AS6" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="AT6" s="79"/>
-      <c r="AU6" s="79"/>
-      <c r="AV6" s="79"/>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AT6" s="82"/>
+      <c r="AU6" s="82"/>
+      <c r="AV6" s="82"/>
+      <c r="AX6" s="82" t="s">
+        <v>143</v>
+      </c>
+      <c r="AY6" s="82"/>
+      <c r="AZ6" s="82"/>
+      <c r="BA6" s="82"/>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>3</v>
       </c>
@@ -1543,8 +1621,16 @@
       </c>
       <c r="AU7" s="55"/>
       <c r="AV7" s="55"/>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX7" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY7" s="62">
+        <v>10</v>
+      </c>
+      <c r="AZ7" s="55"/>
+      <c r="BA7" s="55"/>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>5</v>
       </c>
@@ -1628,8 +1714,16 @@
       </c>
       <c r="AU8" s="55"/>
       <c r="AV8" s="55"/>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX8" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="AY8" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="AZ8" s="55"/>
+      <c r="BA8" s="55"/>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1755,8 +1849,21 @@
         <f>ROUND(AT9*($C$7+(AT7-1)*($D$7-$C$7)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX9" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY9" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA9" s="65">
+        <f>ROUND(AY9*($C$7+(AY7-1)*($D$7-$C$7)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1880,8 +1987,21 @@
         <f>ROUND(AT10*($C$8+(AT7-1)*($D$8-$C$8)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX10" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA10" s="65">
+        <f>ROUND(AY10*($C$8+(AY7-1)*($D$8-$C$8)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
         <v>11</v>
       </c>
@@ -2007,8 +2127,21 @@
         <f>ROUND(AT11*($C$9+(AT7-1)*($D$9-$C$9)/98),0)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX11" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY11" s="63">
+        <v>0.25</v>
+      </c>
+      <c r="AZ11" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA11" s="65">
+        <f>ROUND(AY11*($C$9+(AY7-1)*($D$9-$C$9)/98),0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
         <v>13</v>
       </c>
@@ -2132,8 +2265,21 @@
         <f>ROUND(AT12*($C$10+(AT7-1)*($D$10-$C$10)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX12" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="AY12" s="63">
+        <v>-0.03</v>
+      </c>
+      <c r="AZ12" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA12" s="65">
+        <f>ROUND(AY12*($C$10+(AY7-1)*($D$10-$C$10)/98),0)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -2257,8 +2403,21 @@
         <f>ROUND(AT13*($C$11+(AT7-1)*($D$11-$C$11)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AX13" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY13" s="63">
+        <v>0.05</v>
+      </c>
+      <c r="AZ13" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA13" s="65">
+        <f>ROUND(AY13*($C$11+(AY7-1)*($D$11-$C$11)/98),0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -2382,8 +2541,21 @@
         <f>ROUND(AT14*($C$12+(AT7-1)*($D$12-$C$12)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX14" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="AY14" s="63">
+        <v>0.03</v>
+      </c>
+      <c r="AZ14" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA14" s="65">
+        <f>ROUND(AY14*($C$12+(AY7-1)*($D$12-$C$12)/98),0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="J15" s="54" t="s">
         <v>45</v>
       </c>
@@ -2488,12 +2660,25 @@
         <f>ROUND(AT15*($C$13+(AT7-1)*($D$13-$C$13)/98),0)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="85" t="s">
+      <c r="AX15" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY15" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ15" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="BA15" s="65">
+        <f>ROUND(AY15*($C$13+(AY7-1)*($D$13-$C$13)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="85"/>
+      <c r="B16" s="88"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -2598,127 +2783,154 @@
         <f>ROUND(AT16*($C$14+(AT7-1)*($D$14-$C$14)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX16" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY16" s="64">
+        <v>0</v>
+      </c>
+      <c r="AZ16" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="BA16" s="65">
+        <f>ROUND(AY16*($C$14+(AY7-1)*($D$14-$C$14)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="82" t="s">
+      <c r="K17" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="L17" s="83"/>
-      <c r="M17" s="84"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="81"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="82" t="s">
+      <c r="P17" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="Q17" s="83"/>
-      <c r="R17" s="84"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="81"/>
       <c r="T17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U17" s="82" t="s">
+      <c r="U17" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="V17" s="83"/>
-      <c r="W17" s="84"/>
+      <c r="V17" s="80"/>
+      <c r="W17" s="81"/>
       <c r="Y17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Z17" s="82" t="s">
+      <c r="Z17" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="AA17" s="83"/>
-      <c r="AB17" s="84"/>
+      <c r="AA17" s="80"/>
+      <c r="AB17" s="81"/>
       <c r="AD17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE17" s="82" t="s">
+      <c r="AE17" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="AF17" s="83"/>
-      <c r="AG17" s="84"/>
+      <c r="AF17" s="80"/>
+      <c r="AG17" s="81"/>
       <c r="AI17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ17" s="82" t="s">
+      <c r="AJ17" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="AK17" s="83"/>
-      <c r="AL17" s="84"/>
+      <c r="AK17" s="80"/>
+      <c r="AL17" s="81"/>
       <c r="AN17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AO17" s="82" t="s">
+      <c r="AO17" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="AP17" s="83"/>
-      <c r="AQ17" s="84"/>
+      <c r="AP17" s="80"/>
+      <c r="AQ17" s="81"/>
       <c r="AS17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AT17" s="82" t="s">
+      <c r="AT17" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="AU17" s="83"/>
-      <c r="AV17" s="84"/>
-    </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="J18" s="80" t="s">
+      <c r="AU17" s="80"/>
+      <c r="AV17" s="81"/>
+      <c r="AX17" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="AY17" s="79" t="s">
+        <v>142</v>
+      </c>
+      <c r="AZ17" s="80"/>
+      <c r="BA17" s="81"/>
+    </row>
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="J18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="O18" s="80" t="s">
+      <c r="K18" s="83"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="83"/>
+      <c r="O18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="80"/>
-      <c r="Q18" s="80"/>
-      <c r="R18" s="80"/>
-      <c r="T18" s="80" t="s">
+      <c r="P18" s="83"/>
+      <c r="Q18" s="83"/>
+      <c r="R18" s="83"/>
+      <c r="T18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="U18" s="80"/>
-      <c r="V18" s="80"/>
-      <c r="W18" s="80"/>
-      <c r="Y18" s="80" t="s">
+      <c r="U18" s="83"/>
+      <c r="V18" s="83"/>
+      <c r="W18" s="83"/>
+      <c r="Y18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="Z18" s="80"/>
-      <c r="AA18" s="80"/>
-      <c r="AB18" s="80"/>
-      <c r="AD18" s="80" t="s">
+      <c r="Z18" s="83"/>
+      <c r="AA18" s="83"/>
+      <c r="AB18" s="83"/>
+      <c r="AD18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AE18" s="80"/>
-      <c r="AF18" s="80"/>
-      <c r="AG18" s="80"/>
-      <c r="AI18" s="80" t="s">
+      <c r="AE18" s="83"/>
+      <c r="AF18" s="83"/>
+      <c r="AG18" s="83"/>
+      <c r="AI18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AJ18" s="80"/>
-      <c r="AK18" s="80"/>
-      <c r="AL18" s="80"/>
-      <c r="AN18" s="80" t="s">
+      <c r="AJ18" s="83"/>
+      <c r="AK18" s="83"/>
+      <c r="AL18" s="83"/>
+      <c r="AN18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AO18" s="80"/>
-      <c r="AP18" s="80"/>
-      <c r="AQ18" s="80"/>
-      <c r="AS18" s="80" t="s">
+      <c r="AO18" s="83"/>
+      <c r="AP18" s="83"/>
+      <c r="AQ18" s="83"/>
+      <c r="AS18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AT18" s="80"/>
-      <c r="AU18" s="80"/>
-      <c r="AV18" s="80"/>
-    </row>
-    <row r="19" spans="1:48" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AT18" s="83"/>
+      <c r="AU18" s="83"/>
+      <c r="AV18" s="83"/>
+      <c r="AX18" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="AY18" s="83"/>
+      <c r="AZ18" s="83"/>
+      <c r="BA18" s="83"/>
+    </row>
+    <row r="19" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>22</v>
       </c>
@@ -2754,7 +2966,7 @@
       <c r="AJ19" s="71"/>
       <c r="AK19" s="71"/>
       <c r="AL19" s="72"/>
-      <c r="AN19" s="81" t="s">
+      <c r="AN19" s="87" t="s">
         <v>104</v>
       </c>
       <c r="AO19" s="71"/>
@@ -2764,8 +2976,12 @@
       <c r="AT19" s="71"/>
       <c r="AU19" s="71"/>
       <c r="AV19" s="72"/>
-    </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX19" s="70"/>
+      <c r="AY19" s="71"/>
+      <c r="AZ19" s="71"/>
+      <c r="BA19" s="72"/>
+    </row>
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
         <v>3</v>
       </c>
@@ -2808,8 +3024,12 @@
       <c r="AT20" s="74"/>
       <c r="AU20" s="74"/>
       <c r="AV20" s="75"/>
-    </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX20" s="73"/>
+      <c r="AY20" s="74"/>
+      <c r="AZ20" s="74"/>
+      <c r="BA20" s="75"/>
+    </row>
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
         <v>5</v>
       </c>
@@ -2852,8 +3072,12 @@
       <c r="AT21" s="77"/>
       <c r="AU21" s="77"/>
       <c r="AV21" s="78"/>
-    </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX21" s="76"/>
+      <c r="AY21" s="77"/>
+      <c r="AZ21" s="77"/>
+      <c r="BA21" s="78"/>
+    </row>
+    <row r="22" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -2865,7 +3089,7 @@
         <v>35.357142857142861</v>
       </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -2876,44 +3100,50 @@
         <f t="shared" si="0"/>
         <v>35.357142857142861</v>
       </c>
-      <c r="J23" s="79" t="s">
+      <c r="J23" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="O23" s="79" t="s">
+      <c r="K23" s="82"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
+      <c r="O23" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="79"/>
-      <c r="T23" s="79" t="s">
+      <c r="P23" s="82"/>
+      <c r="Q23" s="82"/>
+      <c r="R23" s="82"/>
+      <c r="T23" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="U23" s="79"/>
-      <c r="V23" s="79"/>
-      <c r="W23" s="79"/>
-      <c r="Y23" s="79" t="s">
+      <c r="U23" s="82"/>
+      <c r="V23" s="82"/>
+      <c r="W23" s="82"/>
+      <c r="Y23" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="Z23" s="79"/>
-      <c r="AA23" s="79"/>
-      <c r="AB23" s="79"/>
-      <c r="AD23" s="79" t="s">
+      <c r="Z23" s="82"/>
+      <c r="AA23" s="82"/>
+      <c r="AB23" s="82"/>
+      <c r="AD23" s="82" t="s">
         <v>93</v>
       </c>
-      <c r="AE23" s="79"/>
-      <c r="AF23" s="79"/>
-      <c r="AG23" s="79"/>
-      <c r="AI23" s="79" t="s">
+      <c r="AE23" s="82"/>
+      <c r="AF23" s="82"/>
+      <c r="AG23" s="82"/>
+      <c r="AI23" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="AJ23" s="79"/>
-      <c r="AK23" s="79"/>
-      <c r="AL23" s="79"/>
-    </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AJ23" s="82"/>
+      <c r="AK23" s="82"/>
+      <c r="AL23" s="82"/>
+      <c r="AX23" s="82" t="s">
+        <v>144</v>
+      </c>
+      <c r="AY23" s="82"/>
+      <c r="AZ23" s="82"/>
+      <c r="BA23" s="82"/>
+    </row>
+    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
         <v>11</v>
       </c>
@@ -2972,8 +3202,16 @@
       </c>
       <c r="AK24" s="55"/>
       <c r="AL24" s="55"/>
-    </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX24" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="AY24" s="62">
+        <v>13</v>
+      </c>
+      <c r="AZ24" s="55"/>
+      <c r="BA24" s="55"/>
+    </row>
+    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>13</v>
       </c>
@@ -3032,8 +3270,16 @@
       </c>
       <c r="AK25" s="55"/>
       <c r="AL25" s="55"/>
-    </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX25" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="AY25" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="AZ25" s="55"/>
+      <c r="BA25" s="55"/>
+    </row>
+    <row r="26" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -3122,8 +3368,21 @@
         <f>ROUND(AJ26*($C$7+(AJ24-1)*($D$7-$C$7)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX26" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY26" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ26" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA26" s="65">
+        <f>ROUND(AY26*($C$7+(AY24-1)*($D$7-$C$7)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
@@ -3212,8 +3471,21 @@
         <f>ROUND(AJ27*($C$8+(AJ24-1)*($D$8-$C$8)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX27" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY27" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ27" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA27" s="65">
+        <f>ROUND(AY27*($C$8+(AY24-1)*($D$8-$C$8)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
       <c r="J28" s="54" t="s">
         <v>41</v>
       </c>
@@ -3292,8 +3564,21 @@
         <f>ROUND(AJ28*($C$9+(AJ24-1)*($D$9-$C$9)/98),0)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX28" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY28" s="63">
+        <v>0.25</v>
+      </c>
+      <c r="AZ28" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA28" s="65">
+        <f>ROUND(AY28*($C$9+(AY24-1)*($D$9-$C$9)/98),0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
       <c r="J29" s="54" t="s">
         <v>42</v>
       </c>
@@ -3372,8 +3657,21 @@
         <f>ROUND(AJ29*($C$10+(AJ24-1)*($D$10-$C$10)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX29" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="AY29" s="63">
+        <v>-0.04</v>
+      </c>
+      <c r="AZ29" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA29" s="65">
+        <f>ROUND(AY29*($C$10+(AY24-1)*($D$10-$C$10)/98),0)</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:53" x14ac:dyDescent="0.25">
       <c r="J30" s="54" t="s">
         <v>43</v>
       </c>
@@ -3452,8 +3750,21 @@
         <f>ROUND(AJ30*($C$11+(AJ24-1)*($D$11-$C$11)/98),0)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX30" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY30" s="63">
+        <v>0.16</v>
+      </c>
+      <c r="AZ30" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA30" s="65">
+        <f>ROUND(AY30*($C$11+(AY24-1)*($D$11-$C$11)/98),0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
       <c r="J31" s="54" t="s">
         <v>44</v>
       </c>
@@ -3532,8 +3843,21 @@
         <f>ROUND(AJ31*($C$12+(AJ24-1)*($D$12-$C$12)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX31" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="AY31" s="63">
+        <v>0.06</v>
+      </c>
+      <c r="AZ31" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA31" s="65">
+        <f>ROUND(AY31*($C$12+(AY24-1)*($D$12-$C$12)/98),0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
       <c r="J32" s="54" t="s">
         <v>45</v>
       </c>
@@ -3612,8 +3936,21 @@
         <f>ROUND(AJ32*($C$13+(AJ24-1)*($D$13-$C$13)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="10:38" x14ac:dyDescent="0.25">
+      <c r="AX32" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY32" s="63">
+        <v>0</v>
+      </c>
+      <c r="AZ32" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="BA32" s="65">
+        <f>ROUND(AY32*($C$13+(AY24-1)*($D$13-$C$13)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J33" s="56" t="s">
         <v>46</v>
       </c>
@@ -3692,97 +4029,124 @@
         <f>ROUND(AJ33*($C$14+(AJ24-1)*($D$14-$C$14)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="10:38" x14ac:dyDescent="0.25">
+      <c r="AX33" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="AY33" s="64">
+        <v>0</v>
+      </c>
+      <c r="AZ33" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="BA33" s="65">
+        <f>ROUND(AY33*($C$14+(AY24-1)*($D$14-$C$14)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="82" t="s">
+      <c r="K34" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="L34" s="83"/>
-      <c r="M34" s="84"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="81"/>
       <c r="O34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P34" s="82" t="s">
+      <c r="P34" s="79" t="s">
         <v>130</v>
       </c>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="84"/>
+      <c r="Q34" s="80"/>
+      <c r="R34" s="81"/>
       <c r="T34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U34" s="82" t="s">
+      <c r="U34" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="V34" s="83"/>
-      <c r="W34" s="84"/>
+      <c r="V34" s="80"/>
+      <c r="W34" s="81"/>
       <c r="Y34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Z34" s="82" t="s">
+      <c r="Z34" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="AA34" s="83"/>
-      <c r="AB34" s="84"/>
+      <c r="AA34" s="80"/>
+      <c r="AB34" s="81"/>
       <c r="AD34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE34" s="82" t="s">
+      <c r="AE34" s="79" t="s">
         <v>129</v>
       </c>
-      <c r="AF34" s="83"/>
-      <c r="AG34" s="84"/>
+      <c r="AF34" s="80"/>
+      <c r="AG34" s="81"/>
       <c r="AI34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ34" s="82" t="s">
+      <c r="AJ34" s="79" t="s">
         <v>129</v>
       </c>
-      <c r="AK34" s="83"/>
-      <c r="AL34" s="84"/>
-    </row>
-    <row r="35" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J35" s="80" t="s">
+      <c r="AK34" s="80"/>
+      <c r="AL34" s="81"/>
+      <c r="AX34" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="AY34" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="AZ34" s="80"/>
+      <c r="BA34" s="81"/>
+    </row>
+    <row r="35" spans="10:53" x14ac:dyDescent="0.25">
+      <c r="J35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
-      <c r="O35" s="80" t="s">
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
+      <c r="O35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="P35" s="80"/>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="80"/>
-      <c r="T35" s="80" t="s">
+      <c r="P35" s="83"/>
+      <c r="Q35" s="83"/>
+      <c r="R35" s="83"/>
+      <c r="T35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="U35" s="80"/>
-      <c r="V35" s="80"/>
-      <c r="W35" s="80"/>
-      <c r="Y35" s="80" t="s">
+      <c r="U35" s="83"/>
+      <c r="V35" s="83"/>
+      <c r="W35" s="83"/>
+      <c r="Y35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="Z35" s="80"/>
-      <c r="AA35" s="80"/>
-      <c r="AB35" s="80"/>
-      <c r="AD35" s="80" t="s">
+      <c r="Z35" s="83"/>
+      <c r="AA35" s="83"/>
+      <c r="AB35" s="83"/>
+      <c r="AD35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AE35" s="80"/>
-      <c r="AF35" s="80"/>
-      <c r="AG35" s="80"/>
-      <c r="AI35" s="86" t="s">
+      <c r="AE35" s="83"/>
+      <c r="AF35" s="83"/>
+      <c r="AG35" s="83"/>
+      <c r="AI35" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="AJ35" s="87"/>
-      <c r="AK35" s="87"/>
-      <c r="AL35" s="88"/>
-    </row>
-    <row r="36" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J36" s="81" t="s">
+      <c r="AJ35" s="85"/>
+      <c r="AK35" s="85"/>
+      <c r="AL35" s="86"/>
+      <c r="AX35" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="AY35" s="83"/>
+      <c r="AZ35" s="83"/>
+      <c r="BA35" s="83"/>
+    </row>
+    <row r="36" spans="10:53" x14ac:dyDescent="0.25">
+      <c r="J36" s="87" t="s">
         <v>119</v>
       </c>
       <c r="K36" s="71"/>
@@ -3810,8 +4174,12 @@
       <c r="AJ36" s="71"/>
       <c r="AK36" s="71"/>
       <c r="AL36" s="72"/>
-    </row>
-    <row r="37" spans="10:38" x14ac:dyDescent="0.25">
+      <c r="AX36" s="70"/>
+      <c r="AY36" s="71"/>
+      <c r="AZ36" s="71"/>
+      <c r="BA36" s="72"/>
+    </row>
+    <row r="37" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J37" s="73"/>
       <c r="K37" s="74"/>
       <c r="L37" s="74"/>
@@ -3836,8 +4204,12 @@
       <c r="AJ37" s="74"/>
       <c r="AK37" s="74"/>
       <c r="AL37" s="75"/>
-    </row>
-    <row r="38" spans="10:38" x14ac:dyDescent="0.25">
+      <c r="AX37" s="73"/>
+      <c r="AY37" s="74"/>
+      <c r="AZ37" s="74"/>
+      <c r="BA37" s="75"/>
+    </row>
+    <row r="38" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J38" s="76"/>
       <c r="K38" s="77"/>
       <c r="L38" s="77"/>
@@ -3862,46 +4234,50 @@
       <c r="AJ38" s="77"/>
       <c r="AK38" s="77"/>
       <c r="AL38" s="78"/>
-    </row>
-    <row r="40" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J40" s="79" t="s">
+      <c r="AX38" s="76"/>
+      <c r="AY38" s="77"/>
+      <c r="AZ38" s="77"/>
+      <c r="BA38" s="78"/>
+    </row>
+    <row r="40" spans="10:53" x14ac:dyDescent="0.25">
+      <c r="J40" s="82" t="s">
         <v>122</v>
       </c>
-      <c r="K40" s="79"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="79"/>
-      <c r="O40" s="79" t="s">
+      <c r="K40" s="82"/>
+      <c r="L40" s="82"/>
+      <c r="M40" s="82"/>
+      <c r="O40" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="P40" s="79"/>
-      <c r="Q40" s="79"/>
-      <c r="R40" s="79"/>
-      <c r="T40" s="79" t="s">
+      <c r="P40" s="82"/>
+      <c r="Q40" s="82"/>
+      <c r="R40" s="82"/>
+      <c r="T40" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="U40" s="79"/>
-      <c r="V40" s="79"/>
-      <c r="W40" s="79"/>
-      <c r="Y40" s="79" t="s">
+      <c r="U40" s="82"/>
+      <c r="V40" s="82"/>
+      <c r="W40" s="82"/>
+      <c r="Y40" s="82" t="s">
         <v>123</v>
       </c>
-      <c r="Z40" s="79"/>
-      <c r="AA40" s="79"/>
-      <c r="AB40" s="79"/>
-      <c r="AD40" s="79" t="s">
+      <c r="Z40" s="82"/>
+      <c r="AA40" s="82"/>
+      <c r="AB40" s="82"/>
+      <c r="AD40" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="AE40" s="79"/>
-      <c r="AF40" s="79"/>
-      <c r="AG40" s="79"/>
-      <c r="AI40" s="79" t="s">
+      <c r="AE40" s="82"/>
+      <c r="AF40" s="82"/>
+      <c r="AG40" s="82"/>
+      <c r="AI40" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="AJ40" s="79"/>
-      <c r="AK40" s="79"/>
-      <c r="AL40" s="79"/>
-    </row>
-    <row r="41" spans="10:38" x14ac:dyDescent="0.25">
+      <c r="AJ40" s="82"/>
+      <c r="AK40" s="82"/>
+      <c r="AL40" s="82"/>
+    </row>
+    <row r="41" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
         <v>22</v>
       </c>
@@ -3951,7 +4327,7 @@
       <c r="AK41" s="55"/>
       <c r="AL41" s="55"/>
     </row>
-    <row r="42" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="42" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J42" s="54" t="s">
         <v>32</v>
       </c>
@@ -4001,7 +4377,7 @@
       <c r="AK42" s="55"/>
       <c r="AL42" s="55"/>
     </row>
-    <row r="43" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="43" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J43" s="54" t="s">
         <v>47</v>
       </c>
@@ -4081,7 +4457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="44" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J44" s="54" t="s">
         <v>48</v>
       </c>
@@ -4161,7 +4537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="45" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J45" s="54" t="s">
         <v>41</v>
       </c>
@@ -4241,7 +4617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="46" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J46" s="54" t="s">
         <v>42</v>
       </c>
@@ -4321,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="47" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J47" s="54" t="s">
         <v>43</v>
       </c>
@@ -4401,7 +4777,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="48" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J48" s="54" t="s">
         <v>44</v>
       </c>
@@ -4645,88 +5021,88 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="82"/>
-      <c r="L51" s="83"/>
-      <c r="M51" s="84"/>
+      <c r="K51" s="79"/>
+      <c r="L51" s="80"/>
+      <c r="M51" s="81"/>
       <c r="O51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P51" s="82" t="s">
+      <c r="P51" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="Q51" s="83"/>
-      <c r="R51" s="84"/>
+      <c r="Q51" s="80"/>
+      <c r="R51" s="81"/>
       <c r="T51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U51" s="82" t="s">
+      <c r="U51" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="V51" s="83"/>
-      <c r="W51" s="84"/>
+      <c r="V51" s="80"/>
+      <c r="W51" s="81"/>
       <c r="Y51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Z51" s="82"/>
-      <c r="AA51" s="83"/>
-      <c r="AB51" s="84"/>
+      <c r="Z51" s="79"/>
+      <c r="AA51" s="80"/>
+      <c r="AB51" s="81"/>
       <c r="AD51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE51" s="82" t="s">
+      <c r="AE51" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="AF51" s="83"/>
-      <c r="AG51" s="84"/>
+      <c r="AF51" s="80"/>
+      <c r="AG51" s="81"/>
       <c r="AI51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ51" s="82" t="s">
+      <c r="AJ51" s="79" t="s">
         <v>132</v>
       </c>
-      <c r="AK51" s="83"/>
-      <c r="AL51" s="84"/>
+      <c r="AK51" s="80"/>
+      <c r="AL51" s="81"/>
     </row>
     <row r="52" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J52" s="80" t="s">
+      <c r="J52" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="80"/>
-      <c r="L52" s="80"/>
-      <c r="M52" s="80"/>
-      <c r="O52" s="80" t="s">
+      <c r="K52" s="83"/>
+      <c r="L52" s="83"/>
+      <c r="M52" s="83"/>
+      <c r="O52" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="P52" s="80"/>
-      <c r="Q52" s="80"/>
-      <c r="R52" s="80"/>
-      <c r="T52" s="80" t="s">
+      <c r="P52" s="83"/>
+      <c r="Q52" s="83"/>
+      <c r="R52" s="83"/>
+      <c r="T52" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="U52" s="80"/>
-      <c r="V52" s="80"/>
-      <c r="W52" s="80"/>
-      <c r="Y52" s="80" t="s">
+      <c r="U52" s="83"/>
+      <c r="V52" s="83"/>
+      <c r="W52" s="83"/>
+      <c r="Y52" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="Z52" s="80"/>
-      <c r="AA52" s="80"/>
-      <c r="AB52" s="80"/>
-      <c r="AD52" s="80" t="s">
+      <c r="Z52" s="83"/>
+      <c r="AA52" s="83"/>
+      <c r="AB52" s="83"/>
+      <c r="AD52" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AE52" s="80"/>
-      <c r="AF52" s="80"/>
-      <c r="AG52" s="80"/>
-      <c r="AI52" s="80" t="s">
+      <c r="AE52" s="83"/>
+      <c r="AF52" s="83"/>
+      <c r="AG52" s="83"/>
+      <c r="AI52" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AJ52" s="80"/>
-      <c r="AK52" s="80"/>
-      <c r="AL52" s="80"/>
+      <c r="AJ52" s="83"/>
+      <c r="AK52" s="83"/>
+      <c r="AL52" s="83"/>
     </row>
     <row r="53" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J53" s="81"/>
+      <c r="J53" s="87"/>
       <c r="K53" s="71"/>
       <c r="L53" s="71"/>
       <c r="M53" s="72"/>
@@ -4748,7 +5124,7 @@
       <c r="AE53" s="71"/>
       <c r="AF53" s="71"/>
       <c r="AG53" s="72"/>
-      <c r="AI53" s="81" t="s">
+      <c r="AI53" s="87" t="s">
         <v>114</v>
       </c>
       <c r="AJ53" s="71"/>
@@ -4808,30 +5184,30 @@
       <c r="AL55" s="78"/>
     </row>
     <row r="57" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="O57" s="79" t="s">
+      <c r="O57" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="P57" s="79"/>
-      <c r="Q57" s="79"/>
-      <c r="R57" s="79"/>
-      <c r="T57" s="79" t="s">
+      <c r="P57" s="82"/>
+      <c r="Q57" s="82"/>
+      <c r="R57" s="82"/>
+      <c r="T57" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="U57" s="79"/>
-      <c r="V57" s="79"/>
-      <c r="W57" s="79"/>
-      <c r="AD57" s="79" t="s">
+      <c r="U57" s="82"/>
+      <c r="V57" s="82"/>
+      <c r="W57" s="82"/>
+      <c r="AD57" s="82" t="s">
         <v>118</v>
       </c>
-      <c r="AE57" s="79"/>
-      <c r="AF57" s="79"/>
-      <c r="AG57" s="79"/>
-      <c r="AI57" s="79" t="s">
+      <c r="AE57" s="82"/>
+      <c r="AF57" s="82"/>
+      <c r="AG57" s="82"/>
+      <c r="AI57" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="AJ57" s="79"/>
-      <c r="AK57" s="79"/>
-      <c r="AL57" s="79"/>
+      <c r="AJ57" s="82"/>
+      <c r="AK57" s="82"/>
+      <c r="AL57" s="82"/>
     </row>
     <row r="58" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O58" s="54" t="s">
@@ -5337,64 +5713,64 @@
       <c r="O68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P68" s="82" t="s">
+      <c r="P68" s="79" t="s">
         <v>137</v>
       </c>
-      <c r="Q68" s="83"/>
-      <c r="R68" s="84"/>
+      <c r="Q68" s="80"/>
+      <c r="R68" s="81"/>
       <c r="T68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U68" s="82" t="s">
+      <c r="U68" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="V68" s="83"/>
-      <c r="W68" s="84"/>
+      <c r="V68" s="80"/>
+      <c r="W68" s="81"/>
       <c r="AD68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE68" s="82" t="s">
+      <c r="AE68" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="AF68" s="83"/>
-      <c r="AG68" s="84"/>
+      <c r="AF68" s="80"/>
+      <c r="AG68" s="81"/>
       <c r="AI68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ68" s="82" t="s">
+      <c r="AJ68" s="79" t="s">
         <v>132</v>
       </c>
-      <c r="AK68" s="83"/>
-      <c r="AL68" s="84"/>
+      <c r="AK68" s="80"/>
+      <c r="AL68" s="81"/>
     </row>
     <row r="69" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="O69" s="80" t="s">
+      <c r="O69" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="P69" s="80"/>
-      <c r="Q69" s="80"/>
-      <c r="R69" s="80"/>
-      <c r="T69" s="80" t="s">
+      <c r="P69" s="83"/>
+      <c r="Q69" s="83"/>
+      <c r="R69" s="83"/>
+      <c r="T69" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="U69" s="80"/>
-      <c r="V69" s="80"/>
-      <c r="W69" s="80"/>
-      <c r="AD69" s="80" t="s">
+      <c r="U69" s="83"/>
+      <c r="V69" s="83"/>
+      <c r="W69" s="83"/>
+      <c r="AD69" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AE69" s="80"/>
-      <c r="AF69" s="80"/>
-      <c r="AG69" s="80"/>
-      <c r="AI69" s="80" t="s">
+      <c r="AE69" s="83"/>
+      <c r="AF69" s="83"/>
+      <c r="AG69" s="83"/>
+      <c r="AI69" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AJ69" s="80"/>
-      <c r="AK69" s="80"/>
-      <c r="AL69" s="80"/>
+      <c r="AJ69" s="83"/>
+      <c r="AK69" s="83"/>
+      <c r="AL69" s="83"/>
     </row>
     <row r="70" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="O70" s="81" t="s">
+      <c r="O70" s="87" t="s">
         <v>88</v>
       </c>
       <c r="P70" s="71"/>
@@ -5410,7 +5786,7 @@
       <c r="AE70" s="71"/>
       <c r="AF70" s="71"/>
       <c r="AG70" s="72"/>
-      <c r="AI70" s="81" t="s">
+      <c r="AI70" s="87" t="s">
         <v>116</v>
       </c>
       <c r="AJ70" s="71"/>
@@ -5454,18 +5830,18 @@
       <c r="AL72" s="78"/>
     </row>
     <row r="74" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="T74" s="79" t="s">
+      <c r="T74" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="U74" s="79"/>
-      <c r="V74" s="79"/>
-      <c r="W74" s="79"/>
-      <c r="AI74" s="79" t="s">
+      <c r="U74" s="82"/>
+      <c r="V74" s="82"/>
+      <c r="W74" s="82"/>
+      <c r="AI74" s="82" t="s">
         <v>121</v>
       </c>
-      <c r="AJ74" s="79"/>
-      <c r="AK74" s="79"/>
-      <c r="AL74" s="79"/>
+      <c r="AJ74" s="82"/>
+      <c r="AK74" s="82"/>
+      <c r="AL74" s="82"/>
     </row>
     <row r="75" spans="15:38" x14ac:dyDescent="0.25">
       <c r="T75" s="54" t="s">
@@ -5731,33 +6107,33 @@
       <c r="T85" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U85" s="82" t="s">
+      <c r="U85" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="V85" s="83"/>
-      <c r="W85" s="84"/>
+      <c r="V85" s="80"/>
+      <c r="W85" s="81"/>
       <c r="AI85" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ85" s="82" t="s">
+      <c r="AJ85" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="AK85" s="83"/>
-      <c r="AL85" s="84"/>
+      <c r="AK85" s="80"/>
+      <c r="AL85" s="81"/>
     </row>
     <row r="86" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T86" s="80" t="s">
+      <c r="T86" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="U86" s="80"/>
-      <c r="V86" s="80"/>
-      <c r="W86" s="80"/>
-      <c r="AI86" s="80" t="s">
+      <c r="U86" s="83"/>
+      <c r="V86" s="83"/>
+      <c r="W86" s="83"/>
+      <c r="AI86" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AJ86" s="80"/>
-      <c r="AK86" s="80"/>
-      <c r="AL86" s="80"/>
+      <c r="AJ86" s="83"/>
+      <c r="AK86" s="83"/>
+      <c r="AL86" s="83"/>
     </row>
     <row r="87" spans="20:38" x14ac:dyDescent="0.25">
       <c r="T87" s="70"/>
@@ -5790,12 +6166,12 @@
       <c r="AL89" s="78"/>
     </row>
     <row r="91" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T91" s="79" t="s">
+      <c r="T91" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="U91" s="79"/>
-      <c r="V91" s="79"/>
-      <c r="W91" s="79"/>
+      <c r="U91" s="82"/>
+      <c r="V91" s="82"/>
+      <c r="W91" s="82"/>
     </row>
     <row r="92" spans="20:38" x14ac:dyDescent="0.25">
       <c r="T92" s="54" t="s">
@@ -5939,19 +6315,19 @@
       <c r="T102" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U102" s="82" t="s">
+      <c r="U102" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="V102" s="83"/>
-      <c r="W102" s="84"/>
+      <c r="V102" s="80"/>
+      <c r="W102" s="81"/>
     </row>
     <row r="103" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T103" s="80" t="s">
+      <c r="T103" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="U103" s="80"/>
-      <c r="V103" s="80"/>
-      <c r="W103" s="80"/>
+      <c r="U103" s="83"/>
+      <c r="V103" s="83"/>
+      <c r="W103" s="83"/>
     </row>
     <row r="104" spans="20:23" x14ac:dyDescent="0.25">
       <c r="T104" s="70"/>
@@ -5972,12 +6348,12 @@
       <c r="W106" s="78"/>
     </row>
     <row r="108" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T108" s="79" t="s">
+      <c r="T108" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="U108" s="79"/>
-      <c r="V108" s="79"/>
-      <c r="W108" s="79"/>
+      <c r="U108" s="82"/>
+      <c r="V108" s="82"/>
+      <c r="W108" s="82"/>
     </row>
     <row r="109" spans="20:23" x14ac:dyDescent="0.25">
       <c r="T109" s="54" t="s">
@@ -6123,19 +6499,19 @@
       <c r="T119" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U119" s="82" t="s">
+      <c r="U119" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="V119" s="83"/>
-      <c r="W119" s="84"/>
+      <c r="V119" s="80"/>
+      <c r="W119" s="81"/>
     </row>
     <row r="120" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T120" s="80" t="s">
+      <c r="T120" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="U120" s="80"/>
-      <c r="V120" s="80"/>
-      <c r="W120" s="80"/>
+      <c r="U120" s="83"/>
+      <c r="V120" s="83"/>
+      <c r="W120" s="83"/>
     </row>
     <row r="121" spans="20:23" x14ac:dyDescent="0.25">
       <c r="T121" s="70"/>
@@ -6156,100 +6532,15 @@
       <c r="W123" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="116">
-    <mergeCell ref="Y36:AB38"/>
-    <mergeCell ref="U119:W119"/>
-    <mergeCell ref="AE68:AG68"/>
-    <mergeCell ref="AJ68:AL68"/>
-    <mergeCell ref="AJ85:AL85"/>
-    <mergeCell ref="U85:W85"/>
-    <mergeCell ref="U102:W102"/>
-    <mergeCell ref="AT17:AV17"/>
-    <mergeCell ref="AJ34:AL34"/>
-    <mergeCell ref="AE34:AG34"/>
-    <mergeCell ref="Z34:AB34"/>
-    <mergeCell ref="Y40:AB40"/>
-    <mergeCell ref="Y52:AB52"/>
-    <mergeCell ref="Y53:AB55"/>
-    <mergeCell ref="AD69:AG69"/>
-    <mergeCell ref="AD70:AG72"/>
-    <mergeCell ref="AI74:AL74"/>
-    <mergeCell ref="AI86:AL86"/>
-    <mergeCell ref="AI87:AL89"/>
-    <mergeCell ref="T57:W57"/>
-    <mergeCell ref="U68:W68"/>
-    <mergeCell ref="T87:W89"/>
-    <mergeCell ref="AS6:AV6"/>
-    <mergeCell ref="AS18:AV18"/>
-    <mergeCell ref="AS19:AV21"/>
-    <mergeCell ref="AD36:AG38"/>
-    <mergeCell ref="AI6:AL6"/>
-    <mergeCell ref="AI18:AL18"/>
-    <mergeCell ref="AI19:AL21"/>
-    <mergeCell ref="AI23:AL23"/>
-    <mergeCell ref="AI35:AL35"/>
-    <mergeCell ref="AI36:AL38"/>
-    <mergeCell ref="AD6:AG6"/>
-    <mergeCell ref="AD18:AG18"/>
-    <mergeCell ref="AD19:AG21"/>
-    <mergeCell ref="AD23:AG23"/>
-    <mergeCell ref="AD35:AG35"/>
-    <mergeCell ref="AN18:AQ18"/>
-    <mergeCell ref="AN19:AQ21"/>
-    <mergeCell ref="AN6:AQ6"/>
-    <mergeCell ref="AE17:AG17"/>
-    <mergeCell ref="AJ17:AL17"/>
-    <mergeCell ref="AO17:AQ17"/>
-    <mergeCell ref="Y6:AB6"/>
-    <mergeCell ref="Y18:AB18"/>
-    <mergeCell ref="Y19:AB21"/>
-    <mergeCell ref="Y23:AB23"/>
-    <mergeCell ref="Y35:AB35"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="J19:M21"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="Z17:AB17"/>
-    <mergeCell ref="U34:W34"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J36:M38"/>
-    <mergeCell ref="O36:R38"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M55"/>
-    <mergeCell ref="P68:R68"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="O19:R21"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="O35:R35"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="O70:R72"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="T18:W18"/>
-    <mergeCell ref="T19:W21"/>
-    <mergeCell ref="T23:W23"/>
-    <mergeCell ref="T35:W35"/>
-    <mergeCell ref="T36:W38"/>
-    <mergeCell ref="T40:W40"/>
-    <mergeCell ref="T52:W52"/>
-    <mergeCell ref="T53:W55"/>
-    <mergeCell ref="O40:R40"/>
-    <mergeCell ref="O52:R52"/>
-    <mergeCell ref="O53:R55"/>
-    <mergeCell ref="O57:R57"/>
-    <mergeCell ref="O69:R69"/>
-    <mergeCell ref="U51:W51"/>
+  <mergeCells count="124">
+    <mergeCell ref="AX6:BA6"/>
+    <mergeCell ref="AY17:BA17"/>
+    <mergeCell ref="AX18:BA18"/>
+    <mergeCell ref="AX19:BA21"/>
+    <mergeCell ref="AX23:BA23"/>
+    <mergeCell ref="AY34:BA34"/>
+    <mergeCell ref="AX35:BA35"/>
+    <mergeCell ref="AX36:BA38"/>
     <mergeCell ref="T121:W123"/>
     <mergeCell ref="AI40:AL40"/>
     <mergeCell ref="AI52:AL52"/>
@@ -6273,6 +6564,99 @@
     <mergeCell ref="AE51:AG51"/>
     <mergeCell ref="AJ51:AL51"/>
     <mergeCell ref="Z51:AB51"/>
+    <mergeCell ref="O70:R72"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="T19:W21"/>
+    <mergeCell ref="T23:W23"/>
+    <mergeCell ref="T35:W35"/>
+    <mergeCell ref="T36:W38"/>
+    <mergeCell ref="T40:W40"/>
+    <mergeCell ref="T52:W52"/>
+    <mergeCell ref="T53:W55"/>
+    <mergeCell ref="O40:R40"/>
+    <mergeCell ref="O52:R52"/>
+    <mergeCell ref="O53:R55"/>
+    <mergeCell ref="O57:R57"/>
+    <mergeCell ref="O69:R69"/>
+    <mergeCell ref="U51:W51"/>
+    <mergeCell ref="J36:M38"/>
+    <mergeCell ref="O36:R38"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M55"/>
+    <mergeCell ref="P68:R68"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="O19:R21"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O35:R35"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="Y18:AB18"/>
+    <mergeCell ref="Y19:AB21"/>
+    <mergeCell ref="Y23:AB23"/>
+    <mergeCell ref="Y35:AB35"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J19:M21"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="Z17:AB17"/>
+    <mergeCell ref="U34:W34"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="AS6:AV6"/>
+    <mergeCell ref="AS18:AV18"/>
+    <mergeCell ref="AS19:AV21"/>
+    <mergeCell ref="AD36:AG38"/>
+    <mergeCell ref="AI6:AL6"/>
+    <mergeCell ref="AI18:AL18"/>
+    <mergeCell ref="AI19:AL21"/>
+    <mergeCell ref="AI23:AL23"/>
+    <mergeCell ref="AI35:AL35"/>
+    <mergeCell ref="AI36:AL38"/>
+    <mergeCell ref="AD6:AG6"/>
+    <mergeCell ref="AD18:AG18"/>
+    <mergeCell ref="AD19:AG21"/>
+    <mergeCell ref="AD23:AG23"/>
+    <mergeCell ref="AD35:AG35"/>
+    <mergeCell ref="AN18:AQ18"/>
+    <mergeCell ref="AN19:AQ21"/>
+    <mergeCell ref="AN6:AQ6"/>
+    <mergeCell ref="AE17:AG17"/>
+    <mergeCell ref="AJ17:AL17"/>
+    <mergeCell ref="AO17:AQ17"/>
+    <mergeCell ref="Y36:AB38"/>
+    <mergeCell ref="U119:W119"/>
+    <mergeCell ref="AE68:AG68"/>
+    <mergeCell ref="AJ68:AL68"/>
+    <mergeCell ref="AJ85:AL85"/>
+    <mergeCell ref="U85:W85"/>
+    <mergeCell ref="U102:W102"/>
+    <mergeCell ref="AT17:AV17"/>
+    <mergeCell ref="AJ34:AL34"/>
+    <mergeCell ref="AE34:AG34"/>
+    <mergeCell ref="Z34:AB34"/>
+    <mergeCell ref="Y40:AB40"/>
+    <mergeCell ref="Y52:AB52"/>
+    <mergeCell ref="Y53:AB55"/>
+    <mergeCell ref="AD69:AG69"/>
+    <mergeCell ref="AD70:AG72"/>
+    <mergeCell ref="AI74:AL74"/>
+    <mergeCell ref="AI86:AL86"/>
+    <mergeCell ref="AI87:AL89"/>
+    <mergeCell ref="T57:W57"/>
+    <mergeCell ref="U68:W68"/>
+    <mergeCell ref="T87:W89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6283,7 +6667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
@@ -6300,13 +6684,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
@@ -6318,15 +6702,15 @@
       <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="F4" s="85" t="s">
+      <c r="B4" s="88"/>
+      <c r="F4" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -6346,12 +6730,12 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="79" t="s">
+      <c r="J6" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
@@ -6635,10 +7019,10 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="85" t="s">
+      <c r="A16" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="85"/>
+      <c r="B16" s="88"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -6660,19 +7044,19 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="82" t="s">
+      <c r="K17" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="L17" s="83"/>
-      <c r="M17" s="84"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="81"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="80" t="s">
+      <c r="J18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
+      <c r="K18" s="83"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="83"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -6744,12 +7128,12 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J23" s="79" t="s">
+      <c r="J23" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
@@ -6935,19 +7319,19 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="82" t="s">
+      <c r="K34" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="83"/>
-      <c r="M34" s="84"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="81"/>
     </row>
     <row r="35" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J35" s="80" t="s">
+      <c r="J35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
     </row>
     <row r="36" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J36" s="70"/>
@@ -6968,12 +7352,12 @@
       <c r="M38" s="78"/>
     </row>
     <row r="40" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J40" s="79" t="s">
+      <c r="J40" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="K40" s="79"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="79"/>
+      <c r="K40" s="82"/>
+      <c r="L40" s="82"/>
+      <c r="M40" s="82"/>
     </row>
     <row r="41" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -7119,19 +7503,19 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="82" t="s">
+      <c r="K51" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="L51" s="83"/>
-      <c r="M51" s="84"/>
+      <c r="L51" s="80"/>
+      <c r="M51" s="81"/>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J52" s="80" t="s">
+      <c r="J52" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="80"/>
-      <c r="L52" s="80"/>
-      <c r="M52" s="80"/>
+      <c r="K52" s="83"/>
+      <c r="L52" s="83"/>
+      <c r="M52" s="83"/>
     </row>
     <row r="53" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J53" s="70"/>
@@ -7153,6 +7537,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="K17:M17"/>
     <mergeCell ref="J40:M40"/>
     <mergeCell ref="J52:M52"/>
     <mergeCell ref="J53:M55"/>
@@ -7162,13 +7553,6 @@
     <mergeCell ref="J36:M38"/>
     <mergeCell ref="K34:M34"/>
     <mergeCell ref="K51:M51"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="K17:M17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7176,10 +7560,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W55"/>
+  <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="W28" sqref="W28"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19:AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7194,16 +7578,16 @@
     <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-    </row>
-    <row r="2" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+    </row>
+    <row r="2" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>29</v>
       </c>
@@ -7212,18 +7596,18 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="85" t="s">
+    <row r="4" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="F4" s="85" t="s">
+      <c r="B4" s="88"/>
+      <c r="F4" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-    </row>
-    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -7231,7 +7615,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
         <v>1</v>
       </c>
@@ -7241,26 +7625,32 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="79" t="s">
+      <c r="J6" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="O6" s="79" t="s">
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="O6" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="79"/>
-      <c r="T6" s="79" t="s">
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="T6" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="U6" s="79"/>
-      <c r="V6" s="79"/>
-      <c r="W6" s="79"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="82"/>
+      <c r="Y6" s="82" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z6" s="82"/>
+      <c r="AA6" s="82"/>
+      <c r="AB6" s="82"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>3</v>
       </c>
@@ -7304,8 +7694,16 @@
       </c>
       <c r="V7" s="55"/>
       <c r="W7" s="55"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y7" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z7" s="62">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="55"/>
+      <c r="AB7" s="55"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>5</v>
       </c>
@@ -7349,8 +7747,16 @@
       </c>
       <c r="V8" s="55"/>
       <c r="W8" s="55"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y8" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z8" s="62" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA8" s="55"/>
+      <c r="AB8" s="55"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -7409,8 +7815,21 @@
         <f>ROUND(U9*($C$7+(U7-1)*($D$7-$C$7)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y9" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z9" s="63">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB9" s="67">
+        <f>ROUND(Z9*($C$7+(Z7-1)*($D$7-$C$7)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -7471,8 +7890,21 @@
         <f>ROUND(U10*($C$8+(U7-1)*($D$8-$C$8)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y10" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z10" s="63">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB10" s="67">
+        <f>ROUND(Z10*($C$8+(Z7-1)*($D$8-$C$8)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>11</v>
       </c>
@@ -7531,8 +7963,21 @@
         <f>ROUND(U11*($C$9+(U7-1)*($D$9-$C$9)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y11" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z11" s="63">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB11" s="67">
+        <f>ROUND(Z11*($C$9+(Z7-1)*($D$9-$C$9)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>13</v>
       </c>
@@ -7593,8 +8038,21 @@
         <f>ROUND(U12*($C$10+(U7-1)*($D$10-$C$10)/98),0)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y12" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z12" s="63">
+        <v>0.2</v>
+      </c>
+      <c r="AA12" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB12" s="67">
+        <f>ROUND(Z12*($C$10+(Z7-1)*($D$10-$C$10)/98),0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -7653,8 +8111,21 @@
         <f>ROUND(U13*($C$11+(U7-1)*($D$11-$C$11)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y13" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z13" s="63">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB13" s="67">
+        <f>ROUND(Z13*($C$11+(Z7-1)*($D$11-$C$11)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -7713,8 +8184,21 @@
         <f>ROUND(U14*($C$12+(U7-1)*($D$12-$C$12)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y14" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z14" s="63">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AA14" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB14" s="67">
+        <f>ROUND(Z14*($C$12+(Z7-1)*($D$12-$C$12)/98),0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="J15" s="54" t="s">
         <v>45</v>
       </c>
@@ -7754,12 +8238,25 @@
         <f>ROUND(U15*($C$13+(U7-1)*($D$13-$C$13)/98),0)</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="85" t="s">
+      <c r="Y15" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z15" s="63">
+        <v>0.03</v>
+      </c>
+      <c r="AA15" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB15" s="67">
+        <f>ROUND(Z15*($C$13+(Z7-1)*($D$13-$C$13)/98),0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="85"/>
+      <c r="B16" s="88"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -7799,57 +8296,84 @@
         <f>ROUND(U16*($C$14+(U7-1)*($D$14-$C$14)/98),0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y16" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z16" s="64">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB16" s="67">
+        <f>ROUND(Z16*($C$14+(Z7-1)*($D$14-$C$14)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="82" t="s">
+      <c r="K17" s="79" t="s">
         <v>135</v>
       </c>
-      <c r="L17" s="83"/>
-      <c r="M17" s="84"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="81"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="82" t="s">
+      <c r="P17" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="Q17" s="83"/>
-      <c r="R17" s="84"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="81"/>
       <c r="T17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U17" s="82" t="s">
+      <c r="U17" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="V17" s="83"/>
-      <c r="W17" s="84"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="J18" s="80" t="s">
+      <c r="V17" s="80"/>
+      <c r="W17" s="81"/>
+      <c r="Y17" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z17" s="79" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA17" s="80"/>
+      <c r="AB17" s="81"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="J18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="O18" s="80" t="s">
+      <c r="K18" s="83"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="83"/>
+      <c r="O18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="80"/>
-      <c r="Q18" s="80"/>
-      <c r="R18" s="80"/>
-      <c r="T18" s="80" t="s">
+      <c r="P18" s="83"/>
+      <c r="Q18" s="83"/>
+      <c r="R18" s="83"/>
+      <c r="T18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="U18" s="80"/>
-      <c r="V18" s="80"/>
-      <c r="W18" s="80"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U18" s="83"/>
+      <c r="V18" s="83"/>
+      <c r="W18" s="83"/>
+      <c r="Y18" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z18" s="83"/>
+      <c r="AA18" s="83"/>
+      <c r="AB18" s="83"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>22</v>
       </c>
@@ -7871,8 +8395,14 @@
       <c r="U19" s="71"/>
       <c r="V19" s="71"/>
       <c r="W19" s="72"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y19" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z19" s="89"/>
+      <c r="AA19" s="89"/>
+      <c r="AB19" s="90"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>3</v>
       </c>
@@ -7895,8 +8425,12 @@
       <c r="U20" s="74"/>
       <c r="V20" s="74"/>
       <c r="W20" s="75"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y20" s="91"/>
+      <c r="Z20" s="92"/>
+      <c r="AA20" s="92"/>
+      <c r="AB20" s="93"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
         <v>5</v>
       </c>
@@ -7919,8 +8453,12 @@
       <c r="U21" s="77"/>
       <c r="V21" s="77"/>
       <c r="W21" s="78"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y21" s="94"/>
+      <c r="Z21" s="95"/>
+      <c r="AA21" s="95"/>
+      <c r="AB21" s="96"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -7932,7 +8470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -7943,20 +8481,20 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J23" s="79" t="s">
+      <c r="J23" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="O23" s="79" t="s">
+      <c r="K23" s="82"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
+      <c r="O23" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="79"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P23" s="82"/>
+      <c r="Q23" s="82"/>
+      <c r="R23" s="82"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
         <v>11</v>
       </c>
@@ -7984,7 +8522,7 @@
       <c r="Q24" s="55"/>
       <c r="R24" s="55"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
         <v>13</v>
       </c>
@@ -8012,7 +8550,7 @@
       <c r="Q25" s="55"/>
       <c r="R25" s="55"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -8050,7 +8588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
@@ -8088,7 +8626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="J28" s="54" t="s">
         <v>41</v>
       </c>
@@ -8116,7 +8654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="J29" s="54" t="s">
         <v>42</v>
       </c>
@@ -8144,7 +8682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="J30" s="54" t="s">
         <v>43</v>
       </c>
@@ -8172,7 +8710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="J31" s="54" t="s">
         <v>44</v>
       </c>
@@ -8200,7 +8738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="J32" s="54" t="s">
         <v>45</v>
       </c>
@@ -8260,33 +8798,33 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="82" t="s">
+      <c r="K34" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="83"/>
-      <c r="M34" s="84"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="81"/>
       <c r="O34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P34" s="82" t="s">
+      <c r="P34" s="79" t="s">
         <v>137</v>
       </c>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="84"/>
+      <c r="Q34" s="80"/>
+      <c r="R34" s="81"/>
     </row>
     <row r="35" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J35" s="80" t="s">
+      <c r="J35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
-      <c r="O35" s="80" t="s">
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
+      <c r="O35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="P35" s="80"/>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="80"/>
+      <c r="P35" s="83"/>
+      <c r="Q35" s="83"/>
+      <c r="R35" s="83"/>
     </row>
     <row r="36" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J36" s="70"/>
@@ -8319,12 +8857,12 @@
       <c r="R38" s="78"/>
     </row>
     <row r="40" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="O40" s="79" t="s">
+      <c r="O40" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="P40" s="79"/>
-      <c r="Q40" s="79"/>
-      <c r="R40" s="79"/>
+      <c r="P40" s="82"/>
+      <c r="Q40" s="82"/>
+      <c r="R40" s="82"/>
     </row>
     <row r="41" spans="10:18" x14ac:dyDescent="0.25">
       <c r="O41" s="54" t="s">
@@ -8470,19 +9008,19 @@
       <c r="O51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P51" s="82" t="s">
+      <c r="P51" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="Q51" s="83"/>
-      <c r="R51" s="84"/>
+      <c r="Q51" s="80"/>
+      <c r="R51" s="81"/>
     </row>
     <row r="52" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O52" s="80" t="s">
+      <c r="O52" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="P52" s="80"/>
-      <c r="Q52" s="80"/>
-      <c r="R52" s="80"/>
+      <c r="P52" s="83"/>
+      <c r="Q52" s="83"/>
+      <c r="R52" s="83"/>
     </row>
     <row r="53" spans="15:18" x14ac:dyDescent="0.25">
       <c r="O53" s="70"/>
@@ -8503,12 +9041,21 @@
       <c r="R55" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
+  <mergeCells count="32">
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="Z17:AB17"/>
+    <mergeCell ref="Y18:AB18"/>
+    <mergeCell ref="Y19:AB21"/>
+    <mergeCell ref="O40:R40"/>
+    <mergeCell ref="O52:R52"/>
+    <mergeCell ref="O53:R55"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="T19:W21"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="U17:W17"/>
     <mergeCell ref="J19:M21"/>
     <mergeCell ref="J23:M23"/>
     <mergeCell ref="J35:M35"/>
@@ -8522,16 +9069,11 @@
     <mergeCell ref="J18:M18"/>
     <mergeCell ref="K17:M17"/>
     <mergeCell ref="K34:M34"/>
-    <mergeCell ref="O40:R40"/>
-    <mergeCell ref="O52:R52"/>
-    <mergeCell ref="O53:R55"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="T18:W18"/>
-    <mergeCell ref="T19:W21"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8539,10 +9081,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R72"/>
+  <dimension ref="A1:R89"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18:R18"/>
+    <sheetView topLeftCell="D49" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J87" sqref="J87:M89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8556,13 +9098,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
@@ -8574,15 +9116,15 @@
       <c r="E2" s="17"/>
     </row>
     <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="F4" s="85" t="s">
+      <c r="B4" s="88"/>
+      <c r="F4" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -8602,18 +9144,18 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="79" t="s">
+      <c r="J6" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="O6" s="79" t="s">
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="O6" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="79"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
@@ -9004,10 +9546,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="85" t="s">
+      <c r="A16" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="85"/>
+      <c r="B16" s="88"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -9042,33 +9584,33 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="82" t="s">
+      <c r="K17" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="L17" s="83"/>
-      <c r="M17" s="84"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="81"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="82" t="s">
+      <c r="P17" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="Q17" s="83"/>
-      <c r="R17" s="84"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="81"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J18" s="80" t="s">
+      <c r="J18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="O18" s="80" t="s">
+      <c r="K18" s="83"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="83"/>
+      <c r="O18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="80"/>
-      <c r="Q18" s="80"/>
-      <c r="R18" s="80"/>
+      <c r="P18" s="83"/>
+      <c r="Q18" s="83"/>
+      <c r="R18" s="83"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -9152,18 +9694,18 @@
         <f t="shared" si="0"/>
         <v>29.54081632653061</v>
       </c>
-      <c r="J23" s="79" t="s">
+      <c r="J23" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="O23" s="79" t="s">
+      <c r="K23" s="82"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
+      <c r="O23" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="P23" s="79"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="79"/>
+      <c r="P23" s="82"/>
+      <c r="Q23" s="82"/>
+      <c r="R23" s="82"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
@@ -9469,33 +10011,33 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="82" t="s">
+      <c r="K34" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="83"/>
-      <c r="M34" s="84"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="81"/>
       <c r="O34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P34" s="82" t="s">
+      <c r="P34" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="Q34" s="83"/>
-      <c r="R34" s="84"/>
+      <c r="Q34" s="80"/>
+      <c r="R34" s="81"/>
     </row>
     <row r="35" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J35" s="80" t="s">
+      <c r="J35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
-      <c r="O35" s="80" t="s">
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
+      <c r="O35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="P35" s="80"/>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="80"/>
+      <c r="P35" s="83"/>
+      <c r="Q35" s="83"/>
+      <c r="R35" s="83"/>
     </row>
     <row r="36" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J36" s="70"/>
@@ -9528,12 +10070,12 @@
       <c r="R38" s="78"/>
     </row>
     <row r="40" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J40" s="79" t="s">
+      <c r="J40" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="K40" s="79"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="79"/>
+      <c r="K40" s="82"/>
+      <c r="L40" s="82"/>
+      <c r="M40" s="82"/>
     </row>
     <row r="41" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -9679,19 +10221,19 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="82" t="s">
+      <c r="K51" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="L51" s="83"/>
-      <c r="M51" s="84"/>
+      <c r="L51" s="80"/>
+      <c r="M51" s="81"/>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J52" s="80" t="s">
+      <c r="J52" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="80"/>
-      <c r="L52" s="80"/>
-      <c r="M52" s="80"/>
+      <c r="K52" s="83"/>
+      <c r="L52" s="83"/>
+      <c r="M52" s="83"/>
     </row>
     <row r="53" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J53" s="70"/>
@@ -9712,12 +10254,12 @@
       <c r="M55" s="78"/>
     </row>
     <row r="57" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J57" s="79" t="s">
+      <c r="J57" s="82" t="s">
         <v>127</v>
       </c>
-      <c r="K57" s="79"/>
-      <c r="L57" s="79"/>
-      <c r="M57" s="79"/>
+      <c r="K57" s="82"/>
+      <c r="L57" s="82"/>
+      <c r="M57" s="82"/>
     </row>
     <row r="58" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J58" s="54" t="s">
@@ -9863,19 +10405,19 @@
       <c r="J68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K68" s="82" t="s">
+      <c r="K68" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="L68" s="83"/>
-      <c r="M68" s="84"/>
+      <c r="L68" s="80"/>
+      <c r="M68" s="81"/>
     </row>
     <row r="69" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J69" s="80" t="s">
+      <c r="J69" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K69" s="80"/>
-      <c r="L69" s="80"/>
-      <c r="M69" s="80"/>
+      <c r="K69" s="83"/>
+      <c r="L69" s="83"/>
+      <c r="M69" s="83"/>
     </row>
     <row r="70" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J70" s="70"/>
@@ -9895,8 +10437,210 @@
       <c r="L72" s="77"/>
       <c r="M72" s="78"/>
     </row>
+    <row r="74" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J74" s="82" t="s">
+        <v>148</v>
+      </c>
+      <c r="K74" s="82"/>
+      <c r="L74" s="82"/>
+      <c r="M74" s="82"/>
+    </row>
+    <row r="75" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J75" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="K75" s="62">
+        <v>10</v>
+      </c>
+      <c r="L75" s="55"/>
+      <c r="M75" s="55"/>
+    </row>
+    <row r="76" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J76" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="K76" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="L76" s="55"/>
+      <c r="M76" s="55"/>
+    </row>
+    <row r="77" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J77" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="K77" s="63">
+        <v>0</v>
+      </c>
+      <c r="L77" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="M77" s="68">
+        <f>ROUND(K77*($C$7+(K75-1)*($D$7-$C$7)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J78" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="K78" s="63">
+        <v>0</v>
+      </c>
+      <c r="L78" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="M78" s="68">
+        <f>ROUND(K78*($C$8+(K75-1)*($D$8-$C$8)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J79" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="K79" s="63">
+        <v>0</v>
+      </c>
+      <c r="L79" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="M79" s="68">
+        <f>ROUND(K79*($C$9+(K75-1)*($D$9-$C$9)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J80" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="K80" s="63">
+        <v>0.12</v>
+      </c>
+      <c r="L80" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="M80" s="68">
+        <f>ROUND(K80*($C$10+(K75-1)*($D$10-$C$10)/98),0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J81" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="K81" s="63">
+        <v>0</v>
+      </c>
+      <c r="L81" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="M81" s="68">
+        <f>ROUND(K81*($C$11+(K75-1)*($D$11-$C$11)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J82" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="K82" s="63">
+        <v>0.15</v>
+      </c>
+      <c r="L82" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="M82" s="68">
+        <f>ROUND(K82*($C$12+(K75-1)*($D$12-$C$12)/98),0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J83" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="K83" s="63">
+        <v>0</v>
+      </c>
+      <c r="L83" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="M83" s="68">
+        <f>ROUND(K83*($C$13+(K75-1)*($D$13-$C$13)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J84" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="K84" s="64">
+        <v>0</v>
+      </c>
+      <c r="L84" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="M84" s="68">
+        <f>ROUND(K84*($C$14+(K75-1)*($D$14-$C$14)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J85" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="K85" s="79" t="s">
+        <v>142</v>
+      </c>
+      <c r="L85" s="80"/>
+      <c r="M85" s="81"/>
+    </row>
+    <row r="86" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J86" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="K86" s="83"/>
+      <c r="L86" s="83"/>
+      <c r="M86" s="83"/>
+    </row>
+    <row r="87" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J87" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="K87" s="89"/>
+      <c r="L87" s="89"/>
+      <c r="M87" s="90"/>
+    </row>
+    <row r="88" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J88" s="91"/>
+      <c r="K88" s="92"/>
+      <c r="L88" s="92"/>
+      <c r="M88" s="93"/>
+    </row>
+    <row r="89" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J89" s="94"/>
+      <c r="K89" s="95"/>
+      <c r="L89" s="95"/>
+      <c r="M89" s="96"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="32">
+    <mergeCell ref="J74:M74"/>
+    <mergeCell ref="K85:M85"/>
+    <mergeCell ref="J86:M86"/>
+    <mergeCell ref="J87:M89"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="O19:R21"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O35:R35"/>
+    <mergeCell ref="O36:R38"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="P34:R34"/>
     <mergeCell ref="J57:M57"/>
     <mergeCell ref="J69:M69"/>
     <mergeCell ref="J70:M72"/>
@@ -9913,18 +10657,6 @@
     <mergeCell ref="J52:M52"/>
     <mergeCell ref="J53:M55"/>
     <mergeCell ref="K51:M51"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="O19:R21"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="O35:R35"/>
-    <mergeCell ref="O36:R38"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="P34:R34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9932,10 +10664,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P58" sqref="P58"/>
+    <sheetView topLeftCell="B64" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104:M106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9949,13 +10681,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
+      <c r="A1" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -9963,15 +10695,15 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="F4" s="85" t="s">
+      <c r="B4" s="88"/>
+      <c r="F4" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -9991,18 +10723,18 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="79" t="s">
+      <c r="J6" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="79"/>
-      <c r="O6" s="79" t="s">
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="O6" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="79"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
@@ -10405,10 +11137,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="85" t="s">
+      <c r="A16" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="85"/>
+      <c r="B16" s="88"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -10443,31 +11175,31 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="82" t="s">
+      <c r="K17" s="79" t="s">
         <v>137</v>
       </c>
-      <c r="L17" s="83"/>
-      <c r="M17" s="84"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="81"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="83"/>
-      <c r="R17" s="84"/>
+      <c r="P17" s="79"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="81"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J18" s="80" t="s">
+      <c r="J18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="O18" s="80" t="s">
+      <c r="K18" s="83"/>
+      <c r="L18" s="83"/>
+      <c r="M18" s="83"/>
+      <c r="O18" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="80"/>
-      <c r="Q18" s="80"/>
-      <c r="R18" s="80"/>
+      <c r="P18" s="83"/>
+      <c r="Q18" s="83"/>
+      <c r="R18" s="83"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -10479,13 +11211,13 @@
       <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="81" t="s">
+      <c r="J19" s="87" t="s">
         <v>75</v>
       </c>
       <c r="K19" s="89"/>
       <c r="L19" s="89"/>
       <c r="M19" s="90"/>
-      <c r="O19" s="81" t="s">
+      <c r="O19" s="87" t="s">
         <v>99</v>
       </c>
       <c r="P19" s="89"/>
@@ -10555,12 +11287,12 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J23" s="79" t="s">
+      <c r="J23" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="82"/>
+      <c r="M23" s="82"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
@@ -10746,22 +11478,22 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="82" t="s">
+      <c r="K34" s="79" t="s">
         <v>126</v>
       </c>
-      <c r="L34" s="83"/>
-      <c r="M34" s="84"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="81"/>
     </row>
     <row r="35" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J35" s="80" t="s">
+      <c r="J35" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
     </row>
     <row r="36" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J36" s="81" t="s">
+      <c r="J36" s="87" t="s">
         <v>79</v>
       </c>
       <c r="K36" s="89"/>
@@ -10781,12 +11513,12 @@
       <c r="M38" s="96"/>
     </row>
     <row r="40" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J40" s="79" t="s">
+      <c r="J40" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="K40" s="79"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="79"/>
+      <c r="K40" s="82"/>
+      <c r="L40" s="82"/>
+      <c r="M40" s="82"/>
     </row>
     <row r="41" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -10932,22 +11664,22 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="82" t="s">
+      <c r="K51" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="L51" s="83"/>
-      <c r="M51" s="84"/>
+      <c r="L51" s="80"/>
+      <c r="M51" s="81"/>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J52" s="80" t="s">
+      <c r="J52" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="80"/>
-      <c r="L52" s="80"/>
-      <c r="M52" s="80"/>
+      <c r="K52" s="83"/>
+      <c r="L52" s="83"/>
+      <c r="M52" s="83"/>
     </row>
     <row r="53" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J53" s="81" t="s">
+      <c r="J53" s="87" t="s">
         <v>86</v>
       </c>
       <c r="K53" s="89"/>
@@ -10967,12 +11699,12 @@
       <c r="M55" s="96"/>
     </row>
     <row r="57" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J57" s="79" t="s">
+      <c r="J57" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="K57" s="79"/>
-      <c r="L57" s="79"/>
-      <c r="M57" s="79"/>
+      <c r="K57" s="82"/>
+      <c r="L57" s="82"/>
+      <c r="M57" s="82"/>
     </row>
     <row r="58" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J58" s="54" t="s">
@@ -11118,22 +11850,22 @@
       <c r="J68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K68" s="82" t="s">
+      <c r="K68" s="79" t="s">
         <v>128</v>
       </c>
-      <c r="L68" s="83"/>
-      <c r="M68" s="84"/>
+      <c r="L68" s="80"/>
+      <c r="M68" s="81"/>
     </row>
     <row r="69" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J69" s="80" t="s">
+      <c r="J69" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K69" s="80"/>
-      <c r="L69" s="80"/>
-      <c r="M69" s="80"/>
+      <c r="K69" s="83"/>
+      <c r="L69" s="83"/>
+      <c r="M69" s="83"/>
     </row>
     <row r="70" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J70" s="81" t="s">
+      <c r="J70" s="87" t="s">
         <v>101</v>
       </c>
       <c r="K70" s="89"/>
@@ -11153,12 +11885,12 @@
       <c r="M72" s="96"/>
     </row>
     <row r="74" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J74" s="79" t="s">
+      <c r="J74" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="K74" s="79"/>
-      <c r="L74" s="79"/>
-      <c r="M74" s="79"/>
+      <c r="K74" s="82"/>
+      <c r="L74" s="82"/>
+      <c r="M74" s="82"/>
     </row>
     <row r="75" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J75" s="54" t="s">
@@ -11304,22 +12036,22 @@
       <c r="J85" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K85" s="82" t="s">
+      <c r="K85" s="79" t="s">
         <v>138</v>
       </c>
-      <c r="L85" s="83"/>
-      <c r="M85" s="84"/>
+      <c r="L85" s="80"/>
+      <c r="M85" s="81"/>
     </row>
     <row r="86" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J86" s="80" t="s">
+      <c r="J86" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="K86" s="80"/>
-      <c r="L86" s="80"/>
-      <c r="M86" s="80"/>
+      <c r="K86" s="83"/>
+      <c r="L86" s="83"/>
+      <c r="M86" s="83"/>
     </row>
     <row r="87" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J87" s="81" t="s">
+      <c r="J87" s="87" t="s">
         <v>108</v>
       </c>
       <c r="K87" s="89"/>
@@ -11338,8 +12070,213 @@
       <c r="L89" s="95"/>
       <c r="M89" s="96"/>
     </row>
+    <row r="91" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J91" s="82" t="s">
+        <v>149</v>
+      </c>
+      <c r="K91" s="82"/>
+      <c r="L91" s="82"/>
+      <c r="M91" s="82"/>
+    </row>
+    <row r="92" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J92" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="K92" s="62">
+        <v>10</v>
+      </c>
+      <c r="L92" s="55"/>
+      <c r="M92" s="55"/>
+    </row>
+    <row r="93" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J93" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="K93" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="L93" s="55"/>
+      <c r="M93" s="55"/>
+    </row>
+    <row r="94" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J94" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="K94" s="63">
+        <v>0</v>
+      </c>
+      <c r="L94" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="M94" s="69">
+        <f>ROUND(K94*($C$7+(K92-1)*($D$7-$C$7)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J95" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="K95" s="63">
+        <v>0</v>
+      </c>
+      <c r="L95" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="M95" s="69">
+        <f>ROUND(K95*($C$8+(K92-1)*($D$8-$C$8)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J96" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="K96" s="63">
+        <v>0</v>
+      </c>
+      <c r="L96" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="M96" s="69">
+        <f>ROUND(K96*($C$9+(K92-1)*($D$9-$C$9)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J97" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="K97" s="63">
+        <v>0</v>
+      </c>
+      <c r="L97" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="M97" s="69">
+        <f>ROUND(K97*($C$10+(K92-1)*($D$10-$C$10)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J98" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="K98" s="63">
+        <v>0</v>
+      </c>
+      <c r="L98" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="M98" s="69">
+        <f>ROUND(K98*($C$11+(K92-1)*($D$11-$C$11)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J99" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="K99" s="63">
+        <v>0</v>
+      </c>
+      <c r="L99" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="M99" s="69">
+        <f>ROUND(K99*($C$12+(K92-1)*($D$12-$C$12)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J100" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="K100" s="63">
+        <v>0</v>
+      </c>
+      <c r="L100" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="M100" s="69">
+        <f>ROUND(K100*($C$13+(K92-1)*($D$13-$C$13)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J101" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="K101" s="64">
+        <v>0</v>
+      </c>
+      <c r="L101" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="M101" s="69">
+        <f>ROUND(K101*($C$14+(K92-1)*($D$14-$C$14)/98),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J102" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="K102" s="79" t="s">
+        <v>142</v>
+      </c>
+      <c r="L102" s="80"/>
+      <c r="M102" s="81"/>
+    </row>
+    <row r="103" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J103" s="83" t="s">
+        <v>51</v>
+      </c>
+      <c r="K103" s="83"/>
+      <c r="L103" s="83"/>
+      <c r="M103" s="83"/>
+    </row>
+    <row r="104" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J104" s="87" t="s">
+        <v>150</v>
+      </c>
+      <c r="K104" s="89"/>
+      <c r="L104" s="89"/>
+      <c r="M104" s="90"/>
+    </row>
+    <row r="105" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J105" s="91"/>
+      <c r="K105" s="92"/>
+      <c r="L105" s="92"/>
+      <c r="M105" s="93"/>
+    </row>
+    <row r="106" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J106" s="94"/>
+      <c r="K106" s="95"/>
+      <c r="L106" s="95"/>
+      <c r="M106" s="96"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="32">
+    <mergeCell ref="J91:M91"/>
+    <mergeCell ref="K102:M102"/>
+    <mergeCell ref="J103:M103"/>
+    <mergeCell ref="J104:M106"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="J19:M21"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="O19:R21"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="K34:M34"/>
     <mergeCell ref="J36:M38"/>
     <mergeCell ref="J74:M74"/>
     <mergeCell ref="J86:M86"/>
@@ -11353,21 +12290,6 @@
     <mergeCell ref="K51:M51"/>
     <mergeCell ref="K68:M68"/>
     <mergeCell ref="K85:M85"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="J19:M21"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="O19:R21"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Chronowitch skill, misc. bug fixes, time animation/sound
</commit_message>
<xml_diff>
--- a/Weapons and Armor.xlsx
+++ b/Weapons and Armor.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="12435" windowHeight="7740" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="12435" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon" sheetId="1" r:id="rId1"/>
@@ -465,9 +465,6 @@
     <t>Cursed Pitchfork</t>
   </si>
   <si>
-    <t>To be placed in time dungeon</t>
-  </si>
-  <si>
     <t>Witch's Cloak</t>
   </si>
   <si>
@@ -481,6 +478,9 @@
   </si>
   <si>
     <t>Slight resistence to poison, confusion, paralysis, freeze, and burn</t>
+  </si>
+  <si>
+    <t>Time Dungeon 1 B2R2U2</t>
   </si>
 </sst>
 </file>
@@ -985,6 +985,21 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1012,19 +1027,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1034,12 +1040,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1417,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA123"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AY30" sqref="AY30"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AX35" sqref="AX35:BA35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,13 +1431,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:53" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
@@ -1449,17 +1449,17 @@
       <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:53" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="88"/>
+      <c r="B4" s="85"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="F4" s="88" t="s">
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -1482,60 +1482,60 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="82" t="s">
+      <c r="J6" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="O6" s="82" t="s">
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="O6" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
-      <c r="T6" s="82" t="s">
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="T6" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="U6" s="82"/>
-      <c r="V6" s="82"/>
-      <c r="W6" s="82"/>
-      <c r="Y6" s="82" t="s">
+      <c r="U6" s="70"/>
+      <c r="V6" s="70"/>
+      <c r="W6" s="70"/>
+      <c r="Y6" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="Z6" s="82"/>
-      <c r="AA6" s="82"/>
-      <c r="AB6" s="82"/>
-      <c r="AD6" s="82" t="s">
+      <c r="Z6" s="70"/>
+      <c r="AA6" s="70"/>
+      <c r="AB6" s="70"/>
+      <c r="AD6" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="AE6" s="82"/>
-      <c r="AF6" s="82"/>
-      <c r="AG6" s="82"/>
-      <c r="AI6" s="82" t="s">
+      <c r="AE6" s="70"/>
+      <c r="AF6" s="70"/>
+      <c r="AG6" s="70"/>
+      <c r="AI6" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="AJ6" s="82"/>
-      <c r="AK6" s="82"/>
-      <c r="AL6" s="82"/>
-      <c r="AN6" s="82" t="s">
+      <c r="AJ6" s="70"/>
+      <c r="AK6" s="70"/>
+      <c r="AL6" s="70"/>
+      <c r="AN6" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="AO6" s="82"/>
-      <c r="AP6" s="82"/>
-      <c r="AQ6" s="82"/>
-      <c r="AS6" s="82" t="s">
+      <c r="AO6" s="70"/>
+      <c r="AP6" s="70"/>
+      <c r="AQ6" s="70"/>
+      <c r="AS6" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="AT6" s="82"/>
-      <c r="AU6" s="82"/>
-      <c r="AV6" s="82"/>
-      <c r="AX6" s="82" t="s">
+      <c r="AT6" s="70"/>
+      <c r="AU6" s="70"/>
+      <c r="AV6" s="70"/>
+      <c r="AX6" s="70" t="s">
         <v>143</v>
       </c>
-      <c r="AY6" s="82"/>
-      <c r="AZ6" s="82"/>
-      <c r="BA6" s="82"/>
+      <c r="AY6" s="70"/>
+      <c r="AZ6" s="70"/>
+      <c r="BA6" s="70"/>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
@@ -2675,10 +2675,10 @@
       </c>
     </row>
     <row r="16" spans="1:53" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="88"/>
+      <c r="B16" s="85"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -2804,131 +2804,131 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="79" t="s">
+      <c r="K17" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="L17" s="80"/>
-      <c r="M17" s="81"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="73"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="79" t="s">
+      <c r="P17" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="Q17" s="80"/>
-      <c r="R17" s="81"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="73"/>
       <c r="T17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U17" s="79" t="s">
+      <c r="U17" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="V17" s="80"/>
-      <c r="W17" s="81"/>
+      <c r="V17" s="72"/>
+      <c r="W17" s="73"/>
       <c r="Y17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Z17" s="79" t="s">
+      <c r="Z17" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="AA17" s="80"/>
-      <c r="AB17" s="81"/>
+      <c r="AA17" s="72"/>
+      <c r="AB17" s="73"/>
       <c r="AD17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE17" s="79" t="s">
+      <c r="AE17" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="AF17" s="80"/>
-      <c r="AG17" s="81"/>
+      <c r="AF17" s="72"/>
+      <c r="AG17" s="73"/>
       <c r="AI17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ17" s="79" t="s">
+      <c r="AJ17" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="AK17" s="80"/>
-      <c r="AL17" s="81"/>
+      <c r="AK17" s="72"/>
+      <c r="AL17" s="73"/>
       <c r="AN17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AO17" s="79" t="s">
+      <c r="AO17" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="AP17" s="80"/>
-      <c r="AQ17" s="81"/>
+      <c r="AP17" s="72"/>
+      <c r="AQ17" s="73"/>
       <c r="AS17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AT17" s="79" t="s">
+      <c r="AT17" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="AU17" s="80"/>
-      <c r="AV17" s="81"/>
+      <c r="AU17" s="72"/>
+      <c r="AV17" s="73"/>
       <c r="AX17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AY17" s="79" t="s">
+      <c r="AY17" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="AZ17" s="80"/>
-      <c r="BA17" s="81"/>
+      <c r="AZ17" s="72"/>
+      <c r="BA17" s="73"/>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="J18" s="83" t="s">
+      <c r="J18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="O18" s="83" t="s">
+      <c r="K18" s="74"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="74"/>
+      <c r="O18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="83"/>
-      <c r="R18" s="83"/>
-      <c r="T18" s="83" t="s">
+      <c r="P18" s="74"/>
+      <c r="Q18" s="74"/>
+      <c r="R18" s="74"/>
+      <c r="T18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="U18" s="83"/>
-      <c r="V18" s="83"/>
-      <c r="W18" s="83"/>
-      <c r="Y18" s="83" t="s">
+      <c r="U18" s="74"/>
+      <c r="V18" s="74"/>
+      <c r="W18" s="74"/>
+      <c r="Y18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="Z18" s="83"/>
-      <c r="AA18" s="83"/>
-      <c r="AB18" s="83"/>
-      <c r="AD18" s="83" t="s">
+      <c r="Z18" s="74"/>
+      <c r="AA18" s="74"/>
+      <c r="AB18" s="74"/>
+      <c r="AD18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AE18" s="83"/>
-      <c r="AF18" s="83"/>
-      <c r="AG18" s="83"/>
-      <c r="AI18" s="83" t="s">
+      <c r="AE18" s="74"/>
+      <c r="AF18" s="74"/>
+      <c r="AG18" s="74"/>
+      <c r="AI18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AJ18" s="83"/>
-      <c r="AK18" s="83"/>
-      <c r="AL18" s="83"/>
-      <c r="AN18" s="83" t="s">
+      <c r="AJ18" s="74"/>
+      <c r="AK18" s="74"/>
+      <c r="AL18" s="74"/>
+      <c r="AN18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AO18" s="83"/>
-      <c r="AP18" s="83"/>
-      <c r="AQ18" s="83"/>
-      <c r="AS18" s="83" t="s">
+      <c r="AO18" s="74"/>
+      <c r="AP18" s="74"/>
+      <c r="AQ18" s="74"/>
+      <c r="AS18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AT18" s="83"/>
-      <c r="AU18" s="83"/>
-      <c r="AV18" s="83"/>
-      <c r="AX18" s="83" t="s">
+      <c r="AT18" s="74"/>
+      <c r="AU18" s="74"/>
+      <c r="AV18" s="74"/>
+      <c r="AX18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AY18" s="83"/>
-      <c r="AZ18" s="83"/>
-      <c r="BA18" s="83"/>
+      <c r="AY18" s="74"/>
+      <c r="AZ18" s="74"/>
+      <c r="BA18" s="74"/>
     </row>
     <row r="19" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -2940,46 +2940,46 @@
       <c r="C19" s="13">
         <v>8</v>
       </c>
-      <c r="J19" s="70"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="71"/>
-      <c r="M19" s="72"/>
-      <c r="O19" s="70"/>
-      <c r="P19" s="71"/>
-      <c r="Q19" s="71"/>
-      <c r="R19" s="72"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="71"/>
-      <c r="V19" s="71"/>
-      <c r="W19" s="72"/>
-      <c r="Y19" s="70"/>
-      <c r="Z19" s="71"/>
-      <c r="AA19" s="71"/>
-      <c r="AB19" s="72"/>
-      <c r="AD19" s="70" t="s">
+      <c r="J19" s="75"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="77"/>
+      <c r="O19" s="75"/>
+      <c r="P19" s="76"/>
+      <c r="Q19" s="76"/>
+      <c r="R19" s="77"/>
+      <c r="T19" s="75"/>
+      <c r="U19" s="76"/>
+      <c r="V19" s="76"/>
+      <c r="W19" s="77"/>
+      <c r="Y19" s="75"/>
+      <c r="Z19" s="76"/>
+      <c r="AA19" s="76"/>
+      <c r="AB19" s="77"/>
+      <c r="AD19" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="AE19" s="71"/>
-      <c r="AF19" s="71"/>
-      <c r="AG19" s="72"/>
-      <c r="AI19" s="70"/>
-      <c r="AJ19" s="71"/>
-      <c r="AK19" s="71"/>
-      <c r="AL19" s="72"/>
-      <c r="AN19" s="87" t="s">
+      <c r="AE19" s="76"/>
+      <c r="AF19" s="76"/>
+      <c r="AG19" s="77"/>
+      <c r="AI19" s="75"/>
+      <c r="AJ19" s="76"/>
+      <c r="AK19" s="76"/>
+      <c r="AL19" s="77"/>
+      <c r="AN19" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="AO19" s="71"/>
-      <c r="AP19" s="71"/>
-      <c r="AQ19" s="72"/>
-      <c r="AS19" s="70"/>
-      <c r="AT19" s="71"/>
-      <c r="AU19" s="71"/>
-      <c r="AV19" s="72"/>
-      <c r="AX19" s="70"/>
-      <c r="AY19" s="71"/>
-      <c r="AZ19" s="71"/>
-      <c r="BA19" s="72"/>
+      <c r="AO19" s="76"/>
+      <c r="AP19" s="76"/>
+      <c r="AQ19" s="77"/>
+      <c r="AS19" s="75"/>
+      <c r="AT19" s="76"/>
+      <c r="AU19" s="76"/>
+      <c r="AV19" s="77"/>
+      <c r="AX19" s="75"/>
+      <c r="AY19" s="76"/>
+      <c r="AZ19" s="76"/>
+      <c r="BA19" s="77"/>
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
@@ -2992,42 +2992,42 @@
         <f t="shared" ref="C20:C27" si="0">C7+($C$19-1)*(D7-C7)/98</f>
         <v>565</v>
       </c>
-      <c r="J20" s="73"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="75"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="75"/>
-      <c r="T20" s="73"/>
-      <c r="U20" s="74"/>
-      <c r="V20" s="74"/>
-      <c r="W20" s="75"/>
-      <c r="Y20" s="73"/>
-      <c r="Z20" s="74"/>
-      <c r="AA20" s="74"/>
-      <c r="AB20" s="75"/>
-      <c r="AD20" s="73"/>
-      <c r="AE20" s="74"/>
-      <c r="AF20" s="74"/>
-      <c r="AG20" s="75"/>
-      <c r="AI20" s="73"/>
-      <c r="AJ20" s="74"/>
-      <c r="AK20" s="74"/>
-      <c r="AL20" s="75"/>
-      <c r="AN20" s="73"/>
-      <c r="AO20" s="74"/>
-      <c r="AP20" s="74"/>
-      <c r="AQ20" s="75"/>
-      <c r="AS20" s="73"/>
-      <c r="AT20" s="74"/>
-      <c r="AU20" s="74"/>
-      <c r="AV20" s="75"/>
-      <c r="AX20" s="73"/>
-      <c r="AY20" s="74"/>
-      <c r="AZ20" s="74"/>
-      <c r="BA20" s="75"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="80"/>
+      <c r="O20" s="78"/>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="80"/>
+      <c r="T20" s="78"/>
+      <c r="U20" s="79"/>
+      <c r="V20" s="79"/>
+      <c r="W20" s="80"/>
+      <c r="Y20" s="78"/>
+      <c r="Z20" s="79"/>
+      <c r="AA20" s="79"/>
+      <c r="AB20" s="80"/>
+      <c r="AD20" s="78"/>
+      <c r="AE20" s="79"/>
+      <c r="AF20" s="79"/>
+      <c r="AG20" s="80"/>
+      <c r="AI20" s="78"/>
+      <c r="AJ20" s="79"/>
+      <c r="AK20" s="79"/>
+      <c r="AL20" s="80"/>
+      <c r="AN20" s="78"/>
+      <c r="AO20" s="79"/>
+      <c r="AP20" s="79"/>
+      <c r="AQ20" s="80"/>
+      <c r="AS20" s="78"/>
+      <c r="AT20" s="79"/>
+      <c r="AU20" s="79"/>
+      <c r="AV20" s="80"/>
+      <c r="AX20" s="78"/>
+      <c r="AY20" s="79"/>
+      <c r="AZ20" s="79"/>
+      <c r="BA20" s="80"/>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
@@ -3040,42 +3040,42 @@
         <f t="shared" si="0"/>
         <v>121.07142857142857</v>
       </c>
-      <c r="J21" s="76"/>
-      <c r="K21" s="77"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="78"/>
-      <c r="O21" s="76"/>
-      <c r="P21" s="77"/>
-      <c r="Q21" s="77"/>
-      <c r="R21" s="78"/>
-      <c r="T21" s="76"/>
-      <c r="U21" s="77"/>
-      <c r="V21" s="77"/>
-      <c r="W21" s="78"/>
-      <c r="Y21" s="76"/>
-      <c r="Z21" s="77"/>
-      <c r="AA21" s="77"/>
-      <c r="AB21" s="78"/>
-      <c r="AD21" s="76"/>
-      <c r="AE21" s="77"/>
-      <c r="AF21" s="77"/>
-      <c r="AG21" s="78"/>
-      <c r="AI21" s="76"/>
-      <c r="AJ21" s="77"/>
-      <c r="AK21" s="77"/>
-      <c r="AL21" s="78"/>
-      <c r="AN21" s="76"/>
-      <c r="AO21" s="77"/>
-      <c r="AP21" s="77"/>
-      <c r="AQ21" s="78"/>
-      <c r="AS21" s="76"/>
-      <c r="AT21" s="77"/>
-      <c r="AU21" s="77"/>
-      <c r="AV21" s="78"/>
-      <c r="AX21" s="76"/>
-      <c r="AY21" s="77"/>
-      <c r="AZ21" s="77"/>
-      <c r="BA21" s="78"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="83"/>
+      <c r="O21" s="81"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="82"/>
+      <c r="R21" s="83"/>
+      <c r="T21" s="81"/>
+      <c r="U21" s="82"/>
+      <c r="V21" s="82"/>
+      <c r="W21" s="83"/>
+      <c r="Y21" s="81"/>
+      <c r="Z21" s="82"/>
+      <c r="AA21" s="82"/>
+      <c r="AB21" s="83"/>
+      <c r="AD21" s="81"/>
+      <c r="AE21" s="82"/>
+      <c r="AF21" s="82"/>
+      <c r="AG21" s="83"/>
+      <c r="AI21" s="81"/>
+      <c r="AJ21" s="82"/>
+      <c r="AK21" s="82"/>
+      <c r="AL21" s="83"/>
+      <c r="AN21" s="81"/>
+      <c r="AO21" s="82"/>
+      <c r="AP21" s="82"/>
+      <c r="AQ21" s="83"/>
+      <c r="AS21" s="81"/>
+      <c r="AT21" s="82"/>
+      <c r="AU21" s="82"/>
+      <c r="AV21" s="83"/>
+      <c r="AX21" s="81"/>
+      <c r="AY21" s="82"/>
+      <c r="AZ21" s="82"/>
+      <c r="BA21" s="83"/>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -3100,48 +3100,48 @@
         <f t="shared" si="0"/>
         <v>35.357142857142861</v>
       </c>
-      <c r="J23" s="82" t="s">
+      <c r="J23" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="O23" s="82" t="s">
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
+      <c r="O23" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="82"/>
-      <c r="R23" s="82"/>
-      <c r="T23" s="82" t="s">
+      <c r="P23" s="70"/>
+      <c r="Q23" s="70"/>
+      <c r="R23" s="70"/>
+      <c r="T23" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="U23" s="82"/>
-      <c r="V23" s="82"/>
-      <c r="W23" s="82"/>
-      <c r="Y23" s="82" t="s">
+      <c r="U23" s="70"/>
+      <c r="V23" s="70"/>
+      <c r="W23" s="70"/>
+      <c r="Y23" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="Z23" s="82"/>
-      <c r="AA23" s="82"/>
-      <c r="AB23" s="82"/>
-      <c r="AD23" s="82" t="s">
+      <c r="Z23" s="70"/>
+      <c r="AA23" s="70"/>
+      <c r="AB23" s="70"/>
+      <c r="AD23" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="AE23" s="82"/>
-      <c r="AF23" s="82"/>
-      <c r="AG23" s="82"/>
-      <c r="AI23" s="82" t="s">
+      <c r="AE23" s="70"/>
+      <c r="AF23" s="70"/>
+      <c r="AG23" s="70"/>
+      <c r="AI23" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="AJ23" s="82"/>
-      <c r="AK23" s="82"/>
-      <c r="AL23" s="82"/>
-      <c r="AX23" s="82" t="s">
+      <c r="AJ23" s="70"/>
+      <c r="AK23" s="70"/>
+      <c r="AL23" s="70"/>
+      <c r="AX23" s="70" t="s">
         <v>144</v>
       </c>
-      <c r="AY23" s="82"/>
-      <c r="AZ23" s="82"/>
-      <c r="BA23" s="82"/>
+      <c r="AY23" s="70"/>
+      <c r="AZ23" s="70"/>
+      <c r="BA23" s="70"/>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
@@ -4047,235 +4047,235 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="79" t="s">
+      <c r="K34" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="L34" s="80"/>
-      <c r="M34" s="81"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="73"/>
       <c r="O34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P34" s="79" t="s">
+      <c r="P34" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="Q34" s="80"/>
-      <c r="R34" s="81"/>
+      <c r="Q34" s="72"/>
+      <c r="R34" s="73"/>
       <c r="T34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U34" s="79" t="s">
+      <c r="U34" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="V34" s="80"/>
-      <c r="W34" s="81"/>
+      <c r="V34" s="72"/>
+      <c r="W34" s="73"/>
       <c r="Y34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Z34" s="79" t="s">
+      <c r="Z34" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="AA34" s="80"/>
-      <c r="AB34" s="81"/>
+      <c r="AA34" s="72"/>
+      <c r="AB34" s="73"/>
       <c r="AD34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE34" s="79" t="s">
+      <c r="AE34" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="AF34" s="80"/>
-      <c r="AG34" s="81"/>
+      <c r="AF34" s="72"/>
+      <c r="AG34" s="73"/>
       <c r="AI34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ34" s="79" t="s">
+      <c r="AJ34" s="71" t="s">
         <v>129</v>
       </c>
-      <c r="AK34" s="80"/>
-      <c r="AL34" s="81"/>
+      <c r="AK34" s="72"/>
+      <c r="AL34" s="73"/>
       <c r="AX34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AY34" s="79" t="s">
-        <v>145</v>
-      </c>
-      <c r="AZ34" s="80"/>
-      <c r="BA34" s="81"/>
+      <c r="AY34" s="71" t="s">
+        <v>150</v>
+      </c>
+      <c r="AZ34" s="72"/>
+      <c r="BA34" s="73"/>
     </row>
     <row r="35" spans="10:53" x14ac:dyDescent="0.25">
-      <c r="J35" s="83" t="s">
+      <c r="J35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="83"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="83"/>
-      <c r="O35" s="83" t="s">
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="74"/>
+      <c r="O35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="P35" s="83"/>
-      <c r="Q35" s="83"/>
-      <c r="R35" s="83"/>
-      <c r="T35" s="83" t="s">
+      <c r="P35" s="74"/>
+      <c r="Q35" s="74"/>
+      <c r="R35" s="74"/>
+      <c r="T35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="U35" s="83"/>
-      <c r="V35" s="83"/>
-      <c r="W35" s="83"/>
-      <c r="Y35" s="83" t="s">
+      <c r="U35" s="74"/>
+      <c r="V35" s="74"/>
+      <c r="W35" s="74"/>
+      <c r="Y35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="Z35" s="83"/>
-      <c r="AA35" s="83"/>
-      <c r="AB35" s="83"/>
-      <c r="AD35" s="83" t="s">
+      <c r="Z35" s="74"/>
+      <c r="AA35" s="74"/>
+      <c r="AB35" s="74"/>
+      <c r="AD35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AE35" s="83"/>
-      <c r="AF35" s="83"/>
-      <c r="AG35" s="83"/>
-      <c r="AI35" s="84" t="s">
+      <c r="AE35" s="74"/>
+      <c r="AF35" s="74"/>
+      <c r="AG35" s="74"/>
+      <c r="AI35" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="AJ35" s="85"/>
-      <c r="AK35" s="85"/>
-      <c r="AL35" s="86"/>
-      <c r="AX35" s="83" t="s">
+      <c r="AJ35" s="87"/>
+      <c r="AK35" s="87"/>
+      <c r="AL35" s="88"/>
+      <c r="AX35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AY35" s="83"/>
-      <c r="AZ35" s="83"/>
-      <c r="BA35" s="83"/>
+      <c r="AY35" s="74"/>
+      <c r="AZ35" s="74"/>
+      <c r="BA35" s="74"/>
     </row>
     <row r="36" spans="10:53" x14ac:dyDescent="0.25">
-      <c r="J36" s="87" t="s">
+      <c r="J36" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="K36" s="71"/>
-      <c r="L36" s="71"/>
-      <c r="M36" s="72"/>
-      <c r="O36" s="70"/>
-      <c r="P36" s="71"/>
-      <c r="Q36" s="71"/>
-      <c r="R36" s="72"/>
-      <c r="T36" s="70" t="s">
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="77"/>
+      <c r="O36" s="75"/>
+      <c r="P36" s="76"/>
+      <c r="Q36" s="76"/>
+      <c r="R36" s="77"/>
+      <c r="T36" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="U36" s="71"/>
-      <c r="V36" s="71"/>
-      <c r="W36" s="72"/>
-      <c r="Y36" s="70"/>
-      <c r="Z36" s="71"/>
-      <c r="AA36" s="71"/>
-      <c r="AB36" s="72"/>
-      <c r="AD36" s="70"/>
-      <c r="AE36" s="71"/>
-      <c r="AF36" s="71"/>
-      <c r="AG36" s="72"/>
-      <c r="AI36" s="70"/>
-      <c r="AJ36" s="71"/>
-      <c r="AK36" s="71"/>
-      <c r="AL36" s="72"/>
-      <c r="AX36" s="70"/>
-      <c r="AY36" s="71"/>
-      <c r="AZ36" s="71"/>
-      <c r="BA36" s="72"/>
+      <c r="U36" s="76"/>
+      <c r="V36" s="76"/>
+      <c r="W36" s="77"/>
+      <c r="Y36" s="75"/>
+      <c r="Z36" s="76"/>
+      <c r="AA36" s="76"/>
+      <c r="AB36" s="77"/>
+      <c r="AD36" s="75"/>
+      <c r="AE36" s="76"/>
+      <c r="AF36" s="76"/>
+      <c r="AG36" s="77"/>
+      <c r="AI36" s="75"/>
+      <c r="AJ36" s="76"/>
+      <c r="AK36" s="76"/>
+      <c r="AL36" s="77"/>
+      <c r="AX36" s="75"/>
+      <c r="AY36" s="76"/>
+      <c r="AZ36" s="76"/>
+      <c r="BA36" s="77"/>
     </row>
     <row r="37" spans="10:53" x14ac:dyDescent="0.25">
-      <c r="J37" s="73"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="75"/>
-      <c r="O37" s="73"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="75"/>
-      <c r="T37" s="73"/>
-      <c r="U37" s="74"/>
-      <c r="V37" s="74"/>
-      <c r="W37" s="75"/>
-      <c r="Y37" s="73"/>
-      <c r="Z37" s="74"/>
-      <c r="AA37" s="74"/>
-      <c r="AB37" s="75"/>
-      <c r="AD37" s="73"/>
-      <c r="AE37" s="74"/>
-      <c r="AF37" s="74"/>
-      <c r="AG37" s="75"/>
-      <c r="AI37" s="73"/>
-      <c r="AJ37" s="74"/>
-      <c r="AK37" s="74"/>
-      <c r="AL37" s="75"/>
-      <c r="AX37" s="73"/>
-      <c r="AY37" s="74"/>
-      <c r="AZ37" s="74"/>
-      <c r="BA37" s="75"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="80"/>
+      <c r="O37" s="78"/>
+      <c r="P37" s="79"/>
+      <c r="Q37" s="79"/>
+      <c r="R37" s="80"/>
+      <c r="T37" s="78"/>
+      <c r="U37" s="79"/>
+      <c r="V37" s="79"/>
+      <c r="W37" s="80"/>
+      <c r="Y37" s="78"/>
+      <c r="Z37" s="79"/>
+      <c r="AA37" s="79"/>
+      <c r="AB37" s="80"/>
+      <c r="AD37" s="78"/>
+      <c r="AE37" s="79"/>
+      <c r="AF37" s="79"/>
+      <c r="AG37" s="80"/>
+      <c r="AI37" s="78"/>
+      <c r="AJ37" s="79"/>
+      <c r="AK37" s="79"/>
+      <c r="AL37" s="80"/>
+      <c r="AX37" s="78"/>
+      <c r="AY37" s="79"/>
+      <c r="AZ37" s="79"/>
+      <c r="BA37" s="80"/>
     </row>
     <row r="38" spans="10:53" x14ac:dyDescent="0.25">
-      <c r="J38" s="76"/>
-      <c r="K38" s="77"/>
-      <c r="L38" s="77"/>
-      <c r="M38" s="78"/>
-      <c r="O38" s="76"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77"/>
-      <c r="R38" s="78"/>
-      <c r="T38" s="76"/>
-      <c r="U38" s="77"/>
-      <c r="V38" s="77"/>
-      <c r="W38" s="78"/>
-      <c r="Y38" s="76"/>
-      <c r="Z38" s="77"/>
-      <c r="AA38" s="77"/>
-      <c r="AB38" s="78"/>
-      <c r="AD38" s="76"/>
-      <c r="AE38" s="77"/>
-      <c r="AF38" s="77"/>
-      <c r="AG38" s="78"/>
-      <c r="AI38" s="76"/>
-      <c r="AJ38" s="77"/>
-      <c r="AK38" s="77"/>
-      <c r="AL38" s="78"/>
-      <c r="AX38" s="76"/>
-      <c r="AY38" s="77"/>
-      <c r="AZ38" s="77"/>
-      <c r="BA38" s="78"/>
+      <c r="J38" s="81"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="83"/>
+      <c r="O38" s="81"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="82"/>
+      <c r="R38" s="83"/>
+      <c r="T38" s="81"/>
+      <c r="U38" s="82"/>
+      <c r="V38" s="82"/>
+      <c r="W38" s="83"/>
+      <c r="Y38" s="81"/>
+      <c r="Z38" s="82"/>
+      <c r="AA38" s="82"/>
+      <c r="AB38" s="83"/>
+      <c r="AD38" s="81"/>
+      <c r="AE38" s="82"/>
+      <c r="AF38" s="82"/>
+      <c r="AG38" s="83"/>
+      <c r="AI38" s="81"/>
+      <c r="AJ38" s="82"/>
+      <c r="AK38" s="82"/>
+      <c r="AL38" s="83"/>
+      <c r="AX38" s="81"/>
+      <c r="AY38" s="82"/>
+      <c r="AZ38" s="82"/>
+      <c r="BA38" s="83"/>
     </row>
     <row r="40" spans="10:53" x14ac:dyDescent="0.25">
-      <c r="J40" s="82" t="s">
+      <c r="J40" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="K40" s="82"/>
-      <c r="L40" s="82"/>
-      <c r="M40" s="82"/>
-      <c r="O40" s="82" t="s">
+      <c r="K40" s="70"/>
+      <c r="L40" s="70"/>
+      <c r="M40" s="70"/>
+      <c r="O40" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="P40" s="82"/>
-      <c r="Q40" s="82"/>
-      <c r="R40" s="82"/>
-      <c r="T40" s="82" t="s">
+      <c r="P40" s="70"/>
+      <c r="Q40" s="70"/>
+      <c r="R40" s="70"/>
+      <c r="T40" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="U40" s="82"/>
-      <c r="V40" s="82"/>
-      <c r="W40" s="82"/>
-      <c r="Y40" s="82" t="s">
+      <c r="U40" s="70"/>
+      <c r="V40" s="70"/>
+      <c r="W40" s="70"/>
+      <c r="Y40" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="Z40" s="82"/>
-      <c r="AA40" s="82"/>
-      <c r="AB40" s="82"/>
-      <c r="AD40" s="82" t="s">
+      <c r="Z40" s="70"/>
+      <c r="AA40" s="70"/>
+      <c r="AB40" s="70"/>
+      <c r="AD40" s="70" t="s">
         <v>117</v>
       </c>
-      <c r="AE40" s="82"/>
-      <c r="AF40" s="82"/>
-      <c r="AG40" s="82"/>
-      <c r="AI40" s="82" t="s">
+      <c r="AE40" s="70"/>
+      <c r="AF40" s="70"/>
+      <c r="AG40" s="70"/>
+      <c r="AI40" s="70" t="s">
         <v>113</v>
       </c>
-      <c r="AJ40" s="82"/>
-      <c r="AK40" s="82"/>
-      <c r="AL40" s="82"/>
+      <c r="AJ40" s="70"/>
+      <c r="AK40" s="70"/>
+      <c r="AL40" s="70"/>
     </row>
     <row r="41" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -5021,193 +5021,193 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="79"/>
-      <c r="L51" s="80"/>
-      <c r="M51" s="81"/>
+      <c r="K51" s="71"/>
+      <c r="L51" s="72"/>
+      <c r="M51" s="73"/>
       <c r="O51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P51" s="79" t="s">
+      <c r="P51" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="Q51" s="80"/>
-      <c r="R51" s="81"/>
+      <c r="Q51" s="72"/>
+      <c r="R51" s="73"/>
       <c r="T51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U51" s="79" t="s">
+      <c r="U51" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="V51" s="80"/>
-      <c r="W51" s="81"/>
+      <c r="V51" s="72"/>
+      <c r="W51" s="73"/>
       <c r="Y51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Z51" s="79"/>
-      <c r="AA51" s="80"/>
-      <c r="AB51" s="81"/>
+      <c r="Z51" s="71"/>
+      <c r="AA51" s="72"/>
+      <c r="AB51" s="73"/>
       <c r="AD51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE51" s="79" t="s">
+      <c r="AE51" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="AF51" s="80"/>
-      <c r="AG51" s="81"/>
+      <c r="AF51" s="72"/>
+      <c r="AG51" s="73"/>
       <c r="AI51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ51" s="79" t="s">
+      <c r="AJ51" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="AK51" s="80"/>
-      <c r="AL51" s="81"/>
+      <c r="AK51" s="72"/>
+      <c r="AL51" s="73"/>
     </row>
     <row r="52" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J52" s="83" t="s">
+      <c r="J52" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="83"/>
-      <c r="L52" s="83"/>
-      <c r="M52" s="83"/>
-      <c r="O52" s="83" t="s">
+      <c r="K52" s="74"/>
+      <c r="L52" s="74"/>
+      <c r="M52" s="74"/>
+      <c r="O52" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="P52" s="83"/>
-      <c r="Q52" s="83"/>
-      <c r="R52" s="83"/>
-      <c r="T52" s="83" t="s">
+      <c r="P52" s="74"/>
+      <c r="Q52" s="74"/>
+      <c r="R52" s="74"/>
+      <c r="T52" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="U52" s="83"/>
-      <c r="V52" s="83"/>
-      <c r="W52" s="83"/>
-      <c r="Y52" s="83" t="s">
+      <c r="U52" s="74"/>
+      <c r="V52" s="74"/>
+      <c r="W52" s="74"/>
+      <c r="Y52" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="Z52" s="83"/>
-      <c r="AA52" s="83"/>
-      <c r="AB52" s="83"/>
-      <c r="AD52" s="83" t="s">
+      <c r="Z52" s="74"/>
+      <c r="AA52" s="74"/>
+      <c r="AB52" s="74"/>
+      <c r="AD52" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AE52" s="83"/>
-      <c r="AF52" s="83"/>
-      <c r="AG52" s="83"/>
-      <c r="AI52" s="83" t="s">
+      <c r="AE52" s="74"/>
+      <c r="AF52" s="74"/>
+      <c r="AG52" s="74"/>
+      <c r="AI52" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AJ52" s="83"/>
-      <c r="AK52" s="83"/>
-      <c r="AL52" s="83"/>
+      <c r="AJ52" s="74"/>
+      <c r="AK52" s="74"/>
+      <c r="AL52" s="74"/>
     </row>
     <row r="53" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J53" s="87"/>
-      <c r="K53" s="71"/>
-      <c r="L53" s="71"/>
-      <c r="M53" s="72"/>
-      <c r="O53" s="70"/>
-      <c r="P53" s="71"/>
-      <c r="Q53" s="71"/>
-      <c r="R53" s="72"/>
-      <c r="T53" s="70" t="s">
+      <c r="J53" s="84"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="77"/>
+      <c r="O53" s="75"/>
+      <c r="P53" s="76"/>
+      <c r="Q53" s="76"/>
+      <c r="R53" s="77"/>
+      <c r="T53" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="U53" s="71"/>
-      <c r="V53" s="71"/>
-      <c r="W53" s="72"/>
-      <c r="Y53" s="70"/>
-      <c r="Z53" s="71"/>
-      <c r="AA53" s="71"/>
-      <c r="AB53" s="72"/>
-      <c r="AD53" s="70"/>
-      <c r="AE53" s="71"/>
-      <c r="AF53" s="71"/>
-      <c r="AG53" s="72"/>
-      <c r="AI53" s="87" t="s">
+      <c r="U53" s="76"/>
+      <c r="V53" s="76"/>
+      <c r="W53" s="77"/>
+      <c r="Y53" s="75"/>
+      <c r="Z53" s="76"/>
+      <c r="AA53" s="76"/>
+      <c r="AB53" s="77"/>
+      <c r="AD53" s="75"/>
+      <c r="AE53" s="76"/>
+      <c r="AF53" s="76"/>
+      <c r="AG53" s="77"/>
+      <c r="AI53" s="84" t="s">
         <v>114</v>
       </c>
-      <c r="AJ53" s="71"/>
-      <c r="AK53" s="71"/>
-      <c r="AL53" s="72"/>
+      <c r="AJ53" s="76"/>
+      <c r="AK53" s="76"/>
+      <c r="AL53" s="77"/>
     </row>
     <row r="54" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J54" s="73"/>
-      <c r="K54" s="74"/>
-      <c r="L54" s="74"/>
-      <c r="M54" s="75"/>
-      <c r="O54" s="73"/>
-      <c r="P54" s="74"/>
-      <c r="Q54" s="74"/>
-      <c r="R54" s="75"/>
-      <c r="T54" s="73"/>
-      <c r="U54" s="74"/>
-      <c r="V54" s="74"/>
-      <c r="W54" s="75"/>
-      <c r="Y54" s="73"/>
-      <c r="Z54" s="74"/>
-      <c r="AA54" s="74"/>
-      <c r="AB54" s="75"/>
-      <c r="AD54" s="73"/>
-      <c r="AE54" s="74"/>
-      <c r="AF54" s="74"/>
-      <c r="AG54" s="75"/>
-      <c r="AI54" s="73"/>
-      <c r="AJ54" s="74"/>
-      <c r="AK54" s="74"/>
-      <c r="AL54" s="75"/>
+      <c r="J54" s="78"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="80"/>
+      <c r="O54" s="78"/>
+      <c r="P54" s="79"/>
+      <c r="Q54" s="79"/>
+      <c r="R54" s="80"/>
+      <c r="T54" s="78"/>
+      <c r="U54" s="79"/>
+      <c r="V54" s="79"/>
+      <c r="W54" s="80"/>
+      <c r="Y54" s="78"/>
+      <c r="Z54" s="79"/>
+      <c r="AA54" s="79"/>
+      <c r="AB54" s="80"/>
+      <c r="AD54" s="78"/>
+      <c r="AE54" s="79"/>
+      <c r="AF54" s="79"/>
+      <c r="AG54" s="80"/>
+      <c r="AI54" s="78"/>
+      <c r="AJ54" s="79"/>
+      <c r="AK54" s="79"/>
+      <c r="AL54" s="80"/>
     </row>
     <row r="55" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="J55" s="76"/>
-      <c r="K55" s="77"/>
-      <c r="L55" s="77"/>
-      <c r="M55" s="78"/>
-      <c r="O55" s="76"/>
-      <c r="P55" s="77"/>
-      <c r="Q55" s="77"/>
-      <c r="R55" s="78"/>
-      <c r="T55" s="76"/>
-      <c r="U55" s="77"/>
-      <c r="V55" s="77"/>
-      <c r="W55" s="78"/>
-      <c r="Y55" s="76"/>
-      <c r="Z55" s="77"/>
-      <c r="AA55" s="77"/>
-      <c r="AB55" s="78"/>
-      <c r="AD55" s="76"/>
-      <c r="AE55" s="77"/>
-      <c r="AF55" s="77"/>
-      <c r="AG55" s="78"/>
-      <c r="AI55" s="76"/>
-      <c r="AJ55" s="77"/>
-      <c r="AK55" s="77"/>
-      <c r="AL55" s="78"/>
+      <c r="J55" s="81"/>
+      <c r="K55" s="82"/>
+      <c r="L55" s="82"/>
+      <c r="M55" s="83"/>
+      <c r="O55" s="81"/>
+      <c r="P55" s="82"/>
+      <c r="Q55" s="82"/>
+      <c r="R55" s="83"/>
+      <c r="T55" s="81"/>
+      <c r="U55" s="82"/>
+      <c r="V55" s="82"/>
+      <c r="W55" s="83"/>
+      <c r="Y55" s="81"/>
+      <c r="Z55" s="82"/>
+      <c r="AA55" s="82"/>
+      <c r="AB55" s="83"/>
+      <c r="AD55" s="81"/>
+      <c r="AE55" s="82"/>
+      <c r="AF55" s="82"/>
+      <c r="AG55" s="83"/>
+      <c r="AI55" s="81"/>
+      <c r="AJ55" s="82"/>
+      <c r="AK55" s="82"/>
+      <c r="AL55" s="83"/>
     </row>
     <row r="57" spans="10:38" x14ac:dyDescent="0.25">
-      <c r="O57" s="82" t="s">
+      <c r="O57" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="P57" s="82"/>
-      <c r="Q57" s="82"/>
-      <c r="R57" s="82"/>
-      <c r="T57" s="82" t="s">
+      <c r="P57" s="70"/>
+      <c r="Q57" s="70"/>
+      <c r="R57" s="70"/>
+      <c r="T57" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="U57" s="82"/>
-      <c r="V57" s="82"/>
-      <c r="W57" s="82"/>
-      <c r="AD57" s="82" t="s">
+      <c r="U57" s="70"/>
+      <c r="V57" s="70"/>
+      <c r="W57" s="70"/>
+      <c r="AD57" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="AE57" s="82"/>
-      <c r="AF57" s="82"/>
-      <c r="AG57" s="82"/>
-      <c r="AI57" s="82" t="s">
+      <c r="AE57" s="70"/>
+      <c r="AF57" s="70"/>
+      <c r="AG57" s="70"/>
+      <c r="AI57" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="AJ57" s="82"/>
-      <c r="AK57" s="82"/>
-      <c r="AL57" s="82"/>
+      <c r="AJ57" s="70"/>
+      <c r="AK57" s="70"/>
+      <c r="AL57" s="70"/>
     </row>
     <row r="58" spans="10:38" x14ac:dyDescent="0.25">
       <c r="O58" s="54" t="s">
@@ -5713,135 +5713,135 @@
       <c r="O68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P68" s="79" t="s">
+      <c r="P68" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="Q68" s="80"/>
-      <c r="R68" s="81"/>
+      <c r="Q68" s="72"/>
+      <c r="R68" s="73"/>
       <c r="T68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U68" s="79" t="s">
+      <c r="U68" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="V68" s="80"/>
-      <c r="W68" s="81"/>
+      <c r="V68" s="72"/>
+      <c r="W68" s="73"/>
       <c r="AD68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AE68" s="79" t="s">
+      <c r="AE68" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="AF68" s="80"/>
-      <c r="AG68" s="81"/>
+      <c r="AF68" s="72"/>
+      <c r="AG68" s="73"/>
       <c r="AI68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ68" s="79" t="s">
+      <c r="AJ68" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="AK68" s="80"/>
-      <c r="AL68" s="81"/>
+      <c r="AK68" s="72"/>
+      <c r="AL68" s="73"/>
     </row>
     <row r="69" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="O69" s="83" t="s">
+      <c r="O69" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="P69" s="83"/>
-      <c r="Q69" s="83"/>
-      <c r="R69" s="83"/>
-      <c r="T69" s="83" t="s">
+      <c r="P69" s="74"/>
+      <c r="Q69" s="74"/>
+      <c r="R69" s="74"/>
+      <c r="T69" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="U69" s="83"/>
-      <c r="V69" s="83"/>
-      <c r="W69" s="83"/>
-      <c r="AD69" s="83" t="s">
+      <c r="U69" s="74"/>
+      <c r="V69" s="74"/>
+      <c r="W69" s="74"/>
+      <c r="AD69" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AE69" s="83"/>
-      <c r="AF69" s="83"/>
-      <c r="AG69" s="83"/>
-      <c r="AI69" s="83" t="s">
+      <c r="AE69" s="74"/>
+      <c r="AF69" s="74"/>
+      <c r="AG69" s="74"/>
+      <c r="AI69" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AJ69" s="83"/>
-      <c r="AK69" s="83"/>
-      <c r="AL69" s="83"/>
+      <c r="AJ69" s="74"/>
+      <c r="AK69" s="74"/>
+      <c r="AL69" s="74"/>
     </row>
     <row r="70" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="O70" s="87" t="s">
+      <c r="O70" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="P70" s="71"/>
-      <c r="Q70" s="71"/>
-      <c r="R70" s="72"/>
-      <c r="T70" s="70"/>
-      <c r="U70" s="71"/>
-      <c r="V70" s="71"/>
-      <c r="W70" s="72"/>
-      <c r="AD70" s="70" t="s">
+      <c r="P70" s="76"/>
+      <c r="Q70" s="76"/>
+      <c r="R70" s="77"/>
+      <c r="T70" s="75"/>
+      <c r="U70" s="76"/>
+      <c r="V70" s="76"/>
+      <c r="W70" s="77"/>
+      <c r="AD70" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="AE70" s="71"/>
-      <c r="AF70" s="71"/>
-      <c r="AG70" s="72"/>
-      <c r="AI70" s="87" t="s">
+      <c r="AE70" s="76"/>
+      <c r="AF70" s="76"/>
+      <c r="AG70" s="77"/>
+      <c r="AI70" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="AJ70" s="71"/>
-      <c r="AK70" s="71"/>
-      <c r="AL70" s="72"/>
+      <c r="AJ70" s="76"/>
+      <c r="AK70" s="76"/>
+      <c r="AL70" s="77"/>
     </row>
     <row r="71" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="O71" s="73"/>
-      <c r="P71" s="74"/>
-      <c r="Q71" s="74"/>
-      <c r="R71" s="75"/>
-      <c r="T71" s="73"/>
-      <c r="U71" s="74"/>
-      <c r="V71" s="74"/>
-      <c r="W71" s="75"/>
-      <c r="AD71" s="73"/>
-      <c r="AE71" s="74"/>
-      <c r="AF71" s="74"/>
-      <c r="AG71" s="75"/>
-      <c r="AI71" s="73"/>
-      <c r="AJ71" s="74"/>
-      <c r="AK71" s="74"/>
-      <c r="AL71" s="75"/>
+      <c r="O71" s="78"/>
+      <c r="P71" s="79"/>
+      <c r="Q71" s="79"/>
+      <c r="R71" s="80"/>
+      <c r="T71" s="78"/>
+      <c r="U71" s="79"/>
+      <c r="V71" s="79"/>
+      <c r="W71" s="80"/>
+      <c r="AD71" s="78"/>
+      <c r="AE71" s="79"/>
+      <c r="AF71" s="79"/>
+      <c r="AG71" s="80"/>
+      <c r="AI71" s="78"/>
+      <c r="AJ71" s="79"/>
+      <c r="AK71" s="79"/>
+      <c r="AL71" s="80"/>
     </row>
     <row r="72" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="O72" s="76"/>
-      <c r="P72" s="77"/>
-      <c r="Q72" s="77"/>
-      <c r="R72" s="78"/>
-      <c r="T72" s="76"/>
-      <c r="U72" s="77"/>
-      <c r="V72" s="77"/>
-      <c r="W72" s="78"/>
-      <c r="AD72" s="76"/>
-      <c r="AE72" s="77"/>
-      <c r="AF72" s="77"/>
-      <c r="AG72" s="78"/>
-      <c r="AI72" s="76"/>
-      <c r="AJ72" s="77"/>
-      <c r="AK72" s="77"/>
-      <c r="AL72" s="78"/>
+      <c r="O72" s="81"/>
+      <c r="P72" s="82"/>
+      <c r="Q72" s="82"/>
+      <c r="R72" s="83"/>
+      <c r="T72" s="81"/>
+      <c r="U72" s="82"/>
+      <c r="V72" s="82"/>
+      <c r="W72" s="83"/>
+      <c r="AD72" s="81"/>
+      <c r="AE72" s="82"/>
+      <c r="AF72" s="82"/>
+      <c r="AG72" s="83"/>
+      <c r="AI72" s="81"/>
+      <c r="AJ72" s="82"/>
+      <c r="AK72" s="82"/>
+      <c r="AL72" s="83"/>
     </row>
     <row r="74" spans="15:38" x14ac:dyDescent="0.25">
-      <c r="T74" s="82" t="s">
+      <c r="T74" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="U74" s="82"/>
-      <c r="V74" s="82"/>
-      <c r="W74" s="82"/>
-      <c r="AI74" s="82" t="s">
+      <c r="U74" s="70"/>
+      <c r="V74" s="70"/>
+      <c r="W74" s="70"/>
+      <c r="AI74" s="70" t="s">
         <v>121</v>
       </c>
-      <c r="AJ74" s="82"/>
-      <c r="AK74" s="82"/>
-      <c r="AL74" s="82"/>
+      <c r="AJ74" s="70"/>
+      <c r="AK74" s="70"/>
+      <c r="AL74" s="70"/>
     </row>
     <row r="75" spans="15:38" x14ac:dyDescent="0.25">
       <c r="T75" s="54" t="s">
@@ -6107,71 +6107,71 @@
       <c r="T85" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U85" s="79" t="s">
+      <c r="U85" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="V85" s="80"/>
-      <c r="W85" s="81"/>
+      <c r="V85" s="72"/>
+      <c r="W85" s="73"/>
       <c r="AI85" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="AJ85" s="79" t="s">
+      <c r="AJ85" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="AK85" s="80"/>
-      <c r="AL85" s="81"/>
+      <c r="AK85" s="72"/>
+      <c r="AL85" s="73"/>
     </row>
     <row r="86" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T86" s="83" t="s">
+      <c r="T86" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="U86" s="83"/>
-      <c r="V86" s="83"/>
-      <c r="W86" s="83"/>
-      <c r="AI86" s="83" t="s">
+      <c r="U86" s="74"/>
+      <c r="V86" s="74"/>
+      <c r="W86" s="74"/>
+      <c r="AI86" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="AJ86" s="83"/>
-      <c r="AK86" s="83"/>
-      <c r="AL86" s="83"/>
+      <c r="AJ86" s="74"/>
+      <c r="AK86" s="74"/>
+      <c r="AL86" s="74"/>
     </row>
     <row r="87" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T87" s="70"/>
-      <c r="U87" s="71"/>
-      <c r="V87" s="71"/>
-      <c r="W87" s="72"/>
-      <c r="AI87" s="70"/>
-      <c r="AJ87" s="71"/>
-      <c r="AK87" s="71"/>
-      <c r="AL87" s="72"/>
+      <c r="T87" s="75"/>
+      <c r="U87" s="76"/>
+      <c r="V87" s="76"/>
+      <c r="W87" s="77"/>
+      <c r="AI87" s="75"/>
+      <c r="AJ87" s="76"/>
+      <c r="AK87" s="76"/>
+      <c r="AL87" s="77"/>
     </row>
     <row r="88" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T88" s="73"/>
-      <c r="U88" s="74"/>
-      <c r="V88" s="74"/>
-      <c r="W88" s="75"/>
-      <c r="AI88" s="73"/>
-      <c r="AJ88" s="74"/>
-      <c r="AK88" s="74"/>
-      <c r="AL88" s="75"/>
+      <c r="T88" s="78"/>
+      <c r="U88" s="79"/>
+      <c r="V88" s="79"/>
+      <c r="W88" s="80"/>
+      <c r="AI88" s="78"/>
+      <c r="AJ88" s="79"/>
+      <c r="AK88" s="79"/>
+      <c r="AL88" s="80"/>
     </row>
     <row r="89" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T89" s="76"/>
-      <c r="U89" s="77"/>
-      <c r="V89" s="77"/>
-      <c r="W89" s="78"/>
-      <c r="AI89" s="76"/>
-      <c r="AJ89" s="77"/>
-      <c r="AK89" s="77"/>
-      <c r="AL89" s="78"/>
+      <c r="T89" s="81"/>
+      <c r="U89" s="82"/>
+      <c r="V89" s="82"/>
+      <c r="W89" s="83"/>
+      <c r="AI89" s="81"/>
+      <c r="AJ89" s="82"/>
+      <c r="AK89" s="82"/>
+      <c r="AL89" s="83"/>
     </row>
     <row r="91" spans="20:38" x14ac:dyDescent="0.25">
-      <c r="T91" s="82" t="s">
+      <c r="T91" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="U91" s="82"/>
-      <c r="V91" s="82"/>
-      <c r="W91" s="82"/>
+      <c r="U91" s="70"/>
+      <c r="V91" s="70"/>
+      <c r="W91" s="70"/>
     </row>
     <row r="92" spans="20:38" x14ac:dyDescent="0.25">
       <c r="T92" s="54" t="s">
@@ -6315,45 +6315,45 @@
       <c r="T102" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U102" s="79" t="s">
+      <c r="U102" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="V102" s="80"/>
-      <c r="W102" s="81"/>
+      <c r="V102" s="72"/>
+      <c r="W102" s="73"/>
     </row>
     <row r="103" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T103" s="83" t="s">
+      <c r="T103" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="U103" s="83"/>
-      <c r="V103" s="83"/>
-      <c r="W103" s="83"/>
+      <c r="U103" s="74"/>
+      <c r="V103" s="74"/>
+      <c r="W103" s="74"/>
     </row>
     <row r="104" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T104" s="70"/>
-      <c r="U104" s="71"/>
-      <c r="V104" s="71"/>
-      <c r="W104" s="72"/>
+      <c r="T104" s="75"/>
+      <c r="U104" s="76"/>
+      <c r="V104" s="76"/>
+      <c r="W104" s="77"/>
     </row>
     <row r="105" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T105" s="73"/>
-      <c r="U105" s="74"/>
-      <c r="V105" s="74"/>
-      <c r="W105" s="75"/>
+      <c r="T105" s="78"/>
+      <c r="U105" s="79"/>
+      <c r="V105" s="79"/>
+      <c r="W105" s="80"/>
     </row>
     <row r="106" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T106" s="76"/>
-      <c r="U106" s="77"/>
-      <c r="V106" s="77"/>
-      <c r="W106" s="78"/>
+      <c r="T106" s="81"/>
+      <c r="U106" s="82"/>
+      <c r="V106" s="82"/>
+      <c r="W106" s="83"/>
     </row>
     <row r="108" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T108" s="82" t="s">
+      <c r="T108" s="70" t="s">
         <v>112</v>
       </c>
-      <c r="U108" s="82"/>
-      <c r="V108" s="82"/>
-      <c r="W108" s="82"/>
+      <c r="U108" s="70"/>
+      <c r="V108" s="70"/>
+      <c r="W108" s="70"/>
     </row>
     <row r="109" spans="20:23" x14ac:dyDescent="0.25">
       <c r="T109" s="54" t="s">
@@ -6499,40 +6499,140 @@
       <c r="T119" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U119" s="79" t="s">
+      <c r="U119" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="V119" s="80"/>
-      <c r="W119" s="81"/>
+      <c r="V119" s="72"/>
+      <c r="W119" s="73"/>
     </row>
     <row r="120" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T120" s="83" t="s">
+      <c r="T120" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="U120" s="83"/>
-      <c r="V120" s="83"/>
-      <c r="W120" s="83"/>
+      <c r="U120" s="74"/>
+      <c r="V120" s="74"/>
+      <c r="W120" s="74"/>
     </row>
     <row r="121" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T121" s="70"/>
-      <c r="U121" s="71"/>
-      <c r="V121" s="71"/>
-      <c r="W121" s="72"/>
+      <c r="T121" s="75"/>
+      <c r="U121" s="76"/>
+      <c r="V121" s="76"/>
+      <c r="W121" s="77"/>
     </row>
     <row r="122" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T122" s="73"/>
-      <c r="U122" s="74"/>
-      <c r="V122" s="74"/>
-      <c r="W122" s="75"/>
+      <c r="T122" s="78"/>
+      <c r="U122" s="79"/>
+      <c r="V122" s="79"/>
+      <c r="W122" s="80"/>
     </row>
     <row r="123" spans="20:23" x14ac:dyDescent="0.25">
-      <c r="T123" s="76"/>
-      <c r="U123" s="77"/>
-      <c r="V123" s="77"/>
-      <c r="W123" s="78"/>
+      <c r="T123" s="81"/>
+      <c r="U123" s="82"/>
+      <c r="V123" s="82"/>
+      <c r="W123" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="Y36:AB38"/>
+    <mergeCell ref="U119:W119"/>
+    <mergeCell ref="AE68:AG68"/>
+    <mergeCell ref="AJ68:AL68"/>
+    <mergeCell ref="AJ85:AL85"/>
+    <mergeCell ref="U85:W85"/>
+    <mergeCell ref="U102:W102"/>
+    <mergeCell ref="AT17:AV17"/>
+    <mergeCell ref="AJ34:AL34"/>
+    <mergeCell ref="AE34:AG34"/>
+    <mergeCell ref="Z34:AB34"/>
+    <mergeCell ref="Y40:AB40"/>
+    <mergeCell ref="Y52:AB52"/>
+    <mergeCell ref="Y53:AB55"/>
+    <mergeCell ref="AD69:AG69"/>
+    <mergeCell ref="AD70:AG72"/>
+    <mergeCell ref="AI74:AL74"/>
+    <mergeCell ref="AI86:AL86"/>
+    <mergeCell ref="AI87:AL89"/>
+    <mergeCell ref="T57:W57"/>
+    <mergeCell ref="U68:W68"/>
+    <mergeCell ref="T87:W89"/>
+    <mergeCell ref="AS6:AV6"/>
+    <mergeCell ref="AS18:AV18"/>
+    <mergeCell ref="AS19:AV21"/>
+    <mergeCell ref="AD36:AG38"/>
+    <mergeCell ref="AI6:AL6"/>
+    <mergeCell ref="AI18:AL18"/>
+    <mergeCell ref="AI19:AL21"/>
+    <mergeCell ref="AI23:AL23"/>
+    <mergeCell ref="AI35:AL35"/>
+    <mergeCell ref="AI36:AL38"/>
+    <mergeCell ref="AD6:AG6"/>
+    <mergeCell ref="AD18:AG18"/>
+    <mergeCell ref="AD19:AG21"/>
+    <mergeCell ref="AD23:AG23"/>
+    <mergeCell ref="AD35:AG35"/>
+    <mergeCell ref="AN18:AQ18"/>
+    <mergeCell ref="AN19:AQ21"/>
+    <mergeCell ref="AN6:AQ6"/>
+    <mergeCell ref="AE17:AG17"/>
+    <mergeCell ref="AJ17:AL17"/>
+    <mergeCell ref="AO17:AQ17"/>
+    <mergeCell ref="Y18:AB18"/>
+    <mergeCell ref="Y19:AB21"/>
+    <mergeCell ref="Y23:AB23"/>
+    <mergeCell ref="Y35:AB35"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J19:M21"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="Z17:AB17"/>
+    <mergeCell ref="U34:W34"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J36:M38"/>
+    <mergeCell ref="O36:R38"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M55"/>
+    <mergeCell ref="P68:R68"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="O19:R21"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O35:R35"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="AD40:AG40"/>
+    <mergeCell ref="AD52:AG52"/>
+    <mergeCell ref="AD53:AG55"/>
+    <mergeCell ref="AD57:AG57"/>
+    <mergeCell ref="AE51:AG51"/>
+    <mergeCell ref="AJ51:AL51"/>
+    <mergeCell ref="Z51:AB51"/>
+    <mergeCell ref="O70:R72"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="T19:W21"/>
+    <mergeCell ref="T23:W23"/>
+    <mergeCell ref="T35:W35"/>
+    <mergeCell ref="T36:W38"/>
+    <mergeCell ref="T40:W40"/>
+    <mergeCell ref="T52:W52"/>
+    <mergeCell ref="T53:W55"/>
+    <mergeCell ref="O40:R40"/>
+    <mergeCell ref="O52:R52"/>
+    <mergeCell ref="O53:R55"/>
+    <mergeCell ref="O57:R57"/>
+    <mergeCell ref="O69:R69"/>
+    <mergeCell ref="U51:W51"/>
+    <mergeCell ref="Y6:AB6"/>
     <mergeCell ref="AX6:BA6"/>
     <mergeCell ref="AY17:BA17"/>
     <mergeCell ref="AX18:BA18"/>
@@ -6557,106 +6657,6 @@
     <mergeCell ref="T70:W72"/>
     <mergeCell ref="T74:W74"/>
     <mergeCell ref="T86:W86"/>
-    <mergeCell ref="AD40:AG40"/>
-    <mergeCell ref="AD52:AG52"/>
-    <mergeCell ref="AD53:AG55"/>
-    <mergeCell ref="AD57:AG57"/>
-    <mergeCell ref="AE51:AG51"/>
-    <mergeCell ref="AJ51:AL51"/>
-    <mergeCell ref="Z51:AB51"/>
-    <mergeCell ref="O70:R72"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="T18:W18"/>
-    <mergeCell ref="T19:W21"/>
-    <mergeCell ref="T23:W23"/>
-    <mergeCell ref="T35:W35"/>
-    <mergeCell ref="T36:W38"/>
-    <mergeCell ref="T40:W40"/>
-    <mergeCell ref="T52:W52"/>
-    <mergeCell ref="T53:W55"/>
-    <mergeCell ref="O40:R40"/>
-    <mergeCell ref="O52:R52"/>
-    <mergeCell ref="O53:R55"/>
-    <mergeCell ref="O57:R57"/>
-    <mergeCell ref="O69:R69"/>
-    <mergeCell ref="U51:W51"/>
-    <mergeCell ref="J36:M38"/>
-    <mergeCell ref="O36:R38"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M55"/>
-    <mergeCell ref="P68:R68"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="O19:R21"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="O35:R35"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="Y6:AB6"/>
-    <mergeCell ref="Y18:AB18"/>
-    <mergeCell ref="Y19:AB21"/>
-    <mergeCell ref="Y23:AB23"/>
-    <mergeCell ref="Y35:AB35"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="J19:M21"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="Z17:AB17"/>
-    <mergeCell ref="U34:W34"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="AS6:AV6"/>
-    <mergeCell ref="AS18:AV18"/>
-    <mergeCell ref="AS19:AV21"/>
-    <mergeCell ref="AD36:AG38"/>
-    <mergeCell ref="AI6:AL6"/>
-    <mergeCell ref="AI18:AL18"/>
-    <mergeCell ref="AI19:AL21"/>
-    <mergeCell ref="AI23:AL23"/>
-    <mergeCell ref="AI35:AL35"/>
-    <mergeCell ref="AI36:AL38"/>
-    <mergeCell ref="AD6:AG6"/>
-    <mergeCell ref="AD18:AG18"/>
-    <mergeCell ref="AD19:AG21"/>
-    <mergeCell ref="AD23:AG23"/>
-    <mergeCell ref="AD35:AG35"/>
-    <mergeCell ref="AN18:AQ18"/>
-    <mergeCell ref="AN19:AQ21"/>
-    <mergeCell ref="AN6:AQ6"/>
-    <mergeCell ref="AE17:AG17"/>
-    <mergeCell ref="AJ17:AL17"/>
-    <mergeCell ref="AO17:AQ17"/>
-    <mergeCell ref="Y36:AB38"/>
-    <mergeCell ref="U119:W119"/>
-    <mergeCell ref="AE68:AG68"/>
-    <mergeCell ref="AJ68:AL68"/>
-    <mergeCell ref="AJ85:AL85"/>
-    <mergeCell ref="U85:W85"/>
-    <mergeCell ref="U102:W102"/>
-    <mergeCell ref="AT17:AV17"/>
-    <mergeCell ref="AJ34:AL34"/>
-    <mergeCell ref="AE34:AG34"/>
-    <mergeCell ref="Z34:AB34"/>
-    <mergeCell ref="Y40:AB40"/>
-    <mergeCell ref="Y52:AB52"/>
-    <mergeCell ref="Y53:AB55"/>
-    <mergeCell ref="AD69:AG69"/>
-    <mergeCell ref="AD70:AG72"/>
-    <mergeCell ref="AI74:AL74"/>
-    <mergeCell ref="AI86:AL86"/>
-    <mergeCell ref="AI87:AL89"/>
-    <mergeCell ref="T57:W57"/>
-    <mergeCell ref="U68:W68"/>
-    <mergeCell ref="T87:W89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6684,13 +6684,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
@@ -6702,15 +6702,15 @@
       <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="F4" s="88" t="s">
+      <c r="B4" s="85"/>
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -6730,12 +6730,12 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="82" t="s">
+      <c r="J6" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
@@ -7019,10 +7019,10 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="88"/>
+      <c r="B16" s="85"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -7044,19 +7044,19 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="79" t="s">
+      <c r="K17" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="L17" s="80"/>
-      <c r="M17" s="81"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="73"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J18" s="83" t="s">
+      <c r="J18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="74"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -7068,10 +7068,10 @@
       <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="70"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="71"/>
-      <c r="M19" s="72"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="77"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
@@ -7084,10 +7084,10 @@
         <f t="shared" ref="C20:C27" si="0">C7+($C$19-1)*(D7-C7)/98</f>
         <v>70</v>
       </c>
-      <c r="J20" s="73"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="75"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="80"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
@@ -7100,10 +7100,10 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J21" s="76"/>
-      <c r="K21" s="77"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="78"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="83"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -7128,12 +7128,12 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J23" s="82" t="s">
+      <c r="J23" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
@@ -7319,45 +7319,45 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="79" t="s">
+      <c r="K34" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="80"/>
-      <c r="M34" s="81"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="73"/>
     </row>
     <row r="35" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J35" s="83" t="s">
+      <c r="J35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="83"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="83"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="74"/>
     </row>
     <row r="36" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J36" s="70"/>
-      <c r="K36" s="71"/>
-      <c r="L36" s="71"/>
-      <c r="M36" s="72"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="77"/>
     </row>
     <row r="37" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J37" s="73"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="75"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="80"/>
     </row>
     <row r="38" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J38" s="76"/>
-      <c r="K38" s="77"/>
-      <c r="L38" s="77"/>
-      <c r="M38" s="78"/>
+      <c r="J38" s="81"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="83"/>
     </row>
     <row r="40" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J40" s="82" t="s">
+      <c r="J40" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="K40" s="82"/>
-      <c r="L40" s="82"/>
-      <c r="M40" s="82"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="70"/>
+      <c r="M40" s="70"/>
     </row>
     <row r="41" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -7503,47 +7503,40 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="79" t="s">
+      <c r="K51" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="L51" s="80"/>
-      <c r="M51" s="81"/>
+      <c r="L51" s="72"/>
+      <c r="M51" s="73"/>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J52" s="83" t="s">
+      <c r="J52" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="83"/>
-      <c r="L52" s="83"/>
-      <c r="M52" s="83"/>
+      <c r="K52" s="74"/>
+      <c r="L52" s="74"/>
+      <c r="M52" s="74"/>
     </row>
     <row r="53" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J53" s="70"/>
-      <c r="K53" s="71"/>
-      <c r="L53" s="71"/>
-      <c r="M53" s="72"/>
+      <c r="J53" s="75"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="77"/>
     </row>
     <row r="54" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J54" s="73"/>
-      <c r="K54" s="74"/>
-      <c r="L54" s="74"/>
-      <c r="M54" s="75"/>
+      <c r="J54" s="78"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="80"/>
     </row>
     <row r="55" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J55" s="76"/>
-      <c r="K55" s="77"/>
-      <c r="L55" s="77"/>
-      <c r="M55" s="78"/>
+      <c r="J55" s="81"/>
+      <c r="K55" s="82"/>
+      <c r="L55" s="82"/>
+      <c r="M55" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="K17:M17"/>
     <mergeCell ref="J40:M40"/>
     <mergeCell ref="J52:M52"/>
     <mergeCell ref="J53:M55"/>
@@ -7553,6 +7546,13 @@
     <mergeCell ref="J36:M38"/>
     <mergeCell ref="K34:M34"/>
     <mergeCell ref="K51:M51"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="K17:M17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7562,7 +7562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="E4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="Y19" sqref="Y19:AB21"/>
     </sheetView>
   </sheetViews>
@@ -7579,13 +7579,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
@@ -7597,15 +7597,15 @@
       <c r="E2" s="18"/>
     </row>
     <row r="4" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="F4" s="88" t="s">
+      <c r="B4" s="85"/>
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -7625,30 +7625,30 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="82" t="s">
+      <c r="J6" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="O6" s="82" t="s">
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="O6" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
-      <c r="T6" s="82" t="s">
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="T6" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="U6" s="82"/>
-      <c r="V6" s="82"/>
-      <c r="W6" s="82"/>
-      <c r="Y6" s="82" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z6" s="82"/>
-      <c r="AA6" s="82"/>
-      <c r="AB6" s="82"/>
+      <c r="U6" s="70"/>
+      <c r="V6" s="70"/>
+      <c r="W6" s="70"/>
+      <c r="Y6" s="70" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z6" s="70"/>
+      <c r="AA6" s="70"/>
+      <c r="AB6" s="70"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
@@ -7751,7 +7751,7 @@
         <v>32</v>
       </c>
       <c r="Z8" s="62" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AA8" s="55"/>
       <c r="AB8" s="55"/>
@@ -8253,10 +8253,10 @@
       </c>
     </row>
     <row r="16" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="88"/>
+      <c r="B16" s="85"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -8317,61 +8317,61 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="79" t="s">
+      <c r="K17" s="71" t="s">
         <v>135</v>
       </c>
-      <c r="L17" s="80"/>
-      <c r="M17" s="81"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="73"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="79" t="s">
+      <c r="P17" s="71" t="s">
         <v>136</v>
       </c>
-      <c r="Q17" s="80"/>
-      <c r="R17" s="81"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="73"/>
       <c r="T17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="U17" s="79" t="s">
+      <c r="U17" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="V17" s="80"/>
-      <c r="W17" s="81"/>
+      <c r="V17" s="72"/>
+      <c r="W17" s="73"/>
       <c r="Y17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="Z17" s="79" t="s">
+      <c r="Z17" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="AA17" s="80"/>
-      <c r="AB17" s="81"/>
+      <c r="AA17" s="72"/>
+      <c r="AB17" s="73"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="J18" s="83" t="s">
+      <c r="J18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="O18" s="83" t="s">
+      <c r="K18" s="74"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="74"/>
+      <c r="O18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="83"/>
-      <c r="R18" s="83"/>
-      <c r="T18" s="83" t="s">
+      <c r="P18" s="74"/>
+      <c r="Q18" s="74"/>
+      <c r="R18" s="74"/>
+      <c r="T18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="U18" s="83"/>
-      <c r="V18" s="83"/>
-      <c r="W18" s="83"/>
-      <c r="Y18" s="83" t="s">
+      <c r="U18" s="74"/>
+      <c r="V18" s="74"/>
+      <c r="W18" s="74"/>
+      <c r="Y18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="Z18" s="83"/>
-      <c r="AA18" s="83"/>
-      <c r="AB18" s="83"/>
+      <c r="Z18" s="74"/>
+      <c r="AA18" s="74"/>
+      <c r="AB18" s="74"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -8383,20 +8383,20 @@
       <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="70"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="71"/>
-      <c r="M19" s="72"/>
-      <c r="O19" s="70"/>
-      <c r="P19" s="71"/>
-      <c r="Q19" s="71"/>
-      <c r="R19" s="72"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="71"/>
-      <c r="V19" s="71"/>
-      <c r="W19" s="72"/>
-      <c r="Y19" s="87" t="s">
-        <v>150</v>
+      <c r="J19" s="75"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="77"/>
+      <c r="O19" s="75"/>
+      <c r="P19" s="76"/>
+      <c r="Q19" s="76"/>
+      <c r="R19" s="77"/>
+      <c r="T19" s="75"/>
+      <c r="U19" s="76"/>
+      <c r="V19" s="76"/>
+      <c r="W19" s="77"/>
+      <c r="Y19" s="84" t="s">
+        <v>149</v>
       </c>
       <c r="Z19" s="89"/>
       <c r="AA19" s="89"/>
@@ -8413,18 +8413,18 @@
         <f t="shared" ref="C20:C27" si="0">C7+($C$19-1)*(D7-C7)/98</f>
         <v>70</v>
       </c>
-      <c r="J20" s="73"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="75"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="75"/>
-      <c r="T20" s="73"/>
-      <c r="U20" s="74"/>
-      <c r="V20" s="74"/>
-      <c r="W20" s="75"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="80"/>
+      <c r="O20" s="78"/>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="80"/>
+      <c r="T20" s="78"/>
+      <c r="U20" s="79"/>
+      <c r="V20" s="79"/>
+      <c r="W20" s="80"/>
       <c r="Y20" s="91"/>
       <c r="Z20" s="92"/>
       <c r="AA20" s="92"/>
@@ -8441,18 +8441,18 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J21" s="76"/>
-      <c r="K21" s="77"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="78"/>
-      <c r="O21" s="76"/>
-      <c r="P21" s="77"/>
-      <c r="Q21" s="77"/>
-      <c r="R21" s="78"/>
-      <c r="T21" s="76"/>
-      <c r="U21" s="77"/>
-      <c r="V21" s="77"/>
-      <c r="W21" s="78"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="83"/>
+      <c r="O21" s="81"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="82"/>
+      <c r="R21" s="83"/>
+      <c r="T21" s="81"/>
+      <c r="U21" s="82"/>
+      <c r="V21" s="82"/>
+      <c r="W21" s="83"/>
       <c r="Y21" s="94"/>
       <c r="Z21" s="95"/>
       <c r="AA21" s="95"/>
@@ -8481,18 +8481,18 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J23" s="82" t="s">
+      <c r="J23" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="O23" s="82" t="s">
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
+      <c r="O23" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="82"/>
-      <c r="R23" s="82"/>
+      <c r="P23" s="70"/>
+      <c r="Q23" s="70"/>
+      <c r="R23" s="70"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
@@ -8798,71 +8798,71 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="79" t="s">
+      <c r="K34" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="80"/>
-      <c r="M34" s="81"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="73"/>
       <c r="O34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P34" s="79" t="s">
+      <c r="P34" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="Q34" s="80"/>
-      <c r="R34" s="81"/>
+      <c r="Q34" s="72"/>
+      <c r="R34" s="73"/>
     </row>
     <row r="35" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J35" s="83" t="s">
+      <c r="J35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="83"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="83"/>
-      <c r="O35" s="83" t="s">
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="74"/>
+      <c r="O35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="P35" s="83"/>
-      <c r="Q35" s="83"/>
-      <c r="R35" s="83"/>
+      <c r="P35" s="74"/>
+      <c r="Q35" s="74"/>
+      <c r="R35" s="74"/>
     </row>
     <row r="36" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J36" s="70"/>
-      <c r="K36" s="71"/>
-      <c r="L36" s="71"/>
-      <c r="M36" s="72"/>
-      <c r="O36" s="70"/>
-      <c r="P36" s="71"/>
-      <c r="Q36" s="71"/>
-      <c r="R36" s="72"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="77"/>
+      <c r="O36" s="75"/>
+      <c r="P36" s="76"/>
+      <c r="Q36" s="76"/>
+      <c r="R36" s="77"/>
     </row>
     <row r="37" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J37" s="73"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="75"/>
-      <c r="O37" s="73"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="75"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="80"/>
+      <c r="O37" s="78"/>
+      <c r="P37" s="79"/>
+      <c r="Q37" s="79"/>
+      <c r="R37" s="80"/>
     </row>
     <row r="38" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J38" s="76"/>
-      <c r="K38" s="77"/>
-      <c r="L38" s="77"/>
-      <c r="M38" s="78"/>
-      <c r="O38" s="76"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77"/>
-      <c r="R38" s="78"/>
+      <c r="J38" s="81"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="83"/>
+      <c r="O38" s="81"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="82"/>
+      <c r="R38" s="83"/>
     </row>
     <row r="40" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="O40" s="82" t="s">
+      <c r="O40" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="P40" s="82"/>
-      <c r="Q40" s="82"/>
-      <c r="R40" s="82"/>
+      <c r="P40" s="70"/>
+      <c r="Q40" s="70"/>
+      <c r="R40" s="70"/>
     </row>
     <row r="41" spans="10:18" x14ac:dyDescent="0.25">
       <c r="O41" s="54" t="s">
@@ -9008,54 +9008,45 @@
       <c r="O51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P51" s="79" t="s">
+      <c r="P51" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="Q51" s="80"/>
-      <c r="R51" s="81"/>
+      <c r="Q51" s="72"/>
+      <c r="R51" s="73"/>
     </row>
     <row r="52" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O52" s="83" t="s">
+      <c r="O52" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="P52" s="83"/>
-      <c r="Q52" s="83"/>
-      <c r="R52" s="83"/>
+      <c r="P52" s="74"/>
+      <c r="Q52" s="74"/>
+      <c r="R52" s="74"/>
     </row>
     <row r="53" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O53" s="70"/>
-      <c r="P53" s="71"/>
-      <c r="Q53" s="71"/>
-      <c r="R53" s="72"/>
+      <c r="O53" s="75"/>
+      <c r="P53" s="76"/>
+      <c r="Q53" s="76"/>
+      <c r="R53" s="77"/>
     </row>
     <row r="54" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O54" s="73"/>
-      <c r="P54" s="74"/>
-      <c r="Q54" s="74"/>
-      <c r="R54" s="75"/>
+      <c r="O54" s="78"/>
+      <c r="P54" s="79"/>
+      <c r="Q54" s="79"/>
+      <c r="R54" s="80"/>
     </row>
     <row r="55" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O55" s="76"/>
-      <c r="P55" s="77"/>
-      <c r="Q55" s="77"/>
-      <c r="R55" s="78"/>
+      <c r="O55" s="81"/>
+      <c r="P55" s="82"/>
+      <c r="Q55" s="82"/>
+      <c r="R55" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="Y6:AB6"/>
-    <mergeCell ref="Z17:AB17"/>
-    <mergeCell ref="Y18:AB18"/>
-    <mergeCell ref="Y19:AB21"/>
-    <mergeCell ref="O40:R40"/>
-    <mergeCell ref="O52:R52"/>
-    <mergeCell ref="O53:R55"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="T18:W18"/>
-    <mergeCell ref="T19:W21"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
     <mergeCell ref="J19:M21"/>
     <mergeCell ref="J23:M23"/>
     <mergeCell ref="J35:M35"/>
@@ -9069,11 +9060,20 @@
     <mergeCell ref="J18:M18"/>
     <mergeCell ref="K17:M17"/>
     <mergeCell ref="K34:M34"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="O52:R52"/>
+    <mergeCell ref="O53:R55"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="T19:W21"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="Z17:AB17"/>
+    <mergeCell ref="Y18:AB18"/>
+    <mergeCell ref="Y19:AB21"/>
+    <mergeCell ref="O40:R40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9098,13 +9098,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
@@ -9116,15 +9116,15 @@
       <c r="E2" s="17"/>
     </row>
     <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="F4" s="88" t="s">
+      <c r="B4" s="85"/>
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -9144,18 +9144,18 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="82" t="s">
+      <c r="J6" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="O6" s="82" t="s">
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="O6" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
@@ -9546,10 +9546,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="88"/>
+      <c r="B16" s="85"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -9584,33 +9584,33 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="79" t="s">
+      <c r="K17" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="L17" s="80"/>
-      <c r="M17" s="81"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="73"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="79" t="s">
+      <c r="P17" s="71" t="s">
         <v>136</v>
       </c>
-      <c r="Q17" s="80"/>
-      <c r="R17" s="81"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="73"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J18" s="83" t="s">
+      <c r="J18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="O18" s="83" t="s">
+      <c r="K18" s="74"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="74"/>
+      <c r="O18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="83"/>
-      <c r="R18" s="83"/>
+      <c r="P18" s="74"/>
+      <c r="Q18" s="74"/>
+      <c r="R18" s="74"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -9622,14 +9622,14 @@
       <c r="C19" s="13">
         <v>6</v>
       </c>
-      <c r="J19" s="70"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="71"/>
-      <c r="M19" s="72"/>
-      <c r="O19" s="70"/>
-      <c r="P19" s="71"/>
-      <c r="Q19" s="71"/>
-      <c r="R19" s="72"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="77"/>
+      <c r="O19" s="75"/>
+      <c r="P19" s="76"/>
+      <c r="Q19" s="76"/>
+      <c r="R19" s="77"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
@@ -9642,14 +9642,14 @@
         <f t="shared" ref="C20:C27" si="0">C7+($C$19-1)*(D7-C7)/98</f>
         <v>423.57142857142856</v>
       </c>
-      <c r="J20" s="73"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="75"/>
-      <c r="O20" s="73"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="75"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="80"/>
+      <c r="O20" s="78"/>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="80"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
@@ -9662,14 +9662,14 @@
         <f t="shared" si="0"/>
         <v>90.765306122448976</v>
       </c>
-      <c r="J21" s="76"/>
-      <c r="K21" s="77"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="78"/>
-      <c r="O21" s="76"/>
-      <c r="P21" s="77"/>
-      <c r="Q21" s="77"/>
-      <c r="R21" s="78"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="83"/>
+      <c r="O21" s="81"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="82"/>
+      <c r="R21" s="83"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -9694,18 +9694,18 @@
         <f t="shared" si="0"/>
         <v>29.54081632653061</v>
       </c>
-      <c r="J23" s="82" t="s">
+      <c r="J23" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="O23" s="82" t="s">
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
+      <c r="O23" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="82"/>
-      <c r="R23" s="82"/>
+      <c r="P23" s="70"/>
+      <c r="Q23" s="70"/>
+      <c r="R23" s="70"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
@@ -10011,71 +10011,71 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="79" t="s">
+      <c r="K34" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="80"/>
-      <c r="M34" s="81"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="73"/>
       <c r="O34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P34" s="79" t="s">
+      <c r="P34" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="Q34" s="80"/>
-      <c r="R34" s="81"/>
+      <c r="Q34" s="72"/>
+      <c r="R34" s="73"/>
     </row>
     <row r="35" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J35" s="83" t="s">
+      <c r="J35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="83"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="83"/>
-      <c r="O35" s="83" t="s">
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="74"/>
+      <c r="O35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="P35" s="83"/>
-      <c r="Q35" s="83"/>
-      <c r="R35" s="83"/>
+      <c r="P35" s="74"/>
+      <c r="Q35" s="74"/>
+      <c r="R35" s="74"/>
     </row>
     <row r="36" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J36" s="70"/>
-      <c r="K36" s="71"/>
-      <c r="L36" s="71"/>
-      <c r="M36" s="72"/>
-      <c r="O36" s="70"/>
-      <c r="P36" s="71"/>
-      <c r="Q36" s="71"/>
-      <c r="R36" s="72"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="76"/>
+      <c r="M36" s="77"/>
+      <c r="O36" s="75"/>
+      <c r="P36" s="76"/>
+      <c r="Q36" s="76"/>
+      <c r="R36" s="77"/>
     </row>
     <row r="37" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J37" s="73"/>
-      <c r="K37" s="74"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="75"/>
-      <c r="O37" s="73"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="75"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="80"/>
+      <c r="O37" s="78"/>
+      <c r="P37" s="79"/>
+      <c r="Q37" s="79"/>
+      <c r="R37" s="80"/>
     </row>
     <row r="38" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J38" s="76"/>
-      <c r="K38" s="77"/>
-      <c r="L38" s="77"/>
-      <c r="M38" s="78"/>
-      <c r="O38" s="76"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="77"/>
-      <c r="R38" s="78"/>
+      <c r="J38" s="81"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="83"/>
+      <c r="O38" s="81"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="82"/>
+      <c r="R38" s="83"/>
     </row>
     <row r="40" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J40" s="82" t="s">
+      <c r="J40" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="K40" s="82"/>
-      <c r="L40" s="82"/>
-      <c r="M40" s="82"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="70"/>
+      <c r="M40" s="70"/>
     </row>
     <row r="41" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -10221,45 +10221,45 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="79" t="s">
+      <c r="K51" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="L51" s="80"/>
-      <c r="M51" s="81"/>
+      <c r="L51" s="72"/>
+      <c r="M51" s="73"/>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J52" s="83" t="s">
+      <c r="J52" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="83"/>
-      <c r="L52" s="83"/>
-      <c r="M52" s="83"/>
+      <c r="K52" s="74"/>
+      <c r="L52" s="74"/>
+      <c r="M52" s="74"/>
     </row>
     <row r="53" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J53" s="70"/>
-      <c r="K53" s="71"/>
-      <c r="L53" s="71"/>
-      <c r="M53" s="72"/>
+      <c r="J53" s="75"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="77"/>
     </row>
     <row r="54" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J54" s="73"/>
-      <c r="K54" s="74"/>
-      <c r="L54" s="74"/>
-      <c r="M54" s="75"/>
+      <c r="J54" s="78"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="80"/>
     </row>
     <row r="55" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J55" s="76"/>
-      <c r="K55" s="77"/>
-      <c r="L55" s="77"/>
-      <c r="M55" s="78"/>
+      <c r="J55" s="81"/>
+      <c r="K55" s="82"/>
+      <c r="L55" s="82"/>
+      <c r="M55" s="83"/>
     </row>
     <row r="57" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J57" s="82" t="s">
+      <c r="J57" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="K57" s="82"/>
-      <c r="L57" s="82"/>
-      <c r="M57" s="82"/>
+      <c r="K57" s="70"/>
+      <c r="L57" s="70"/>
+      <c r="M57" s="70"/>
     </row>
     <row r="58" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J58" s="54" t="s">
@@ -10405,45 +10405,45 @@
       <c r="J68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K68" s="79" t="s">
+      <c r="K68" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="L68" s="80"/>
-      <c r="M68" s="81"/>
+      <c r="L68" s="72"/>
+      <c r="M68" s="73"/>
     </row>
     <row r="69" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J69" s="83" t="s">
+      <c r="J69" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K69" s="83"/>
-      <c r="L69" s="83"/>
-      <c r="M69" s="83"/>
+      <c r="K69" s="74"/>
+      <c r="L69" s="74"/>
+      <c r="M69" s="74"/>
     </row>
     <row r="70" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J70" s="70"/>
-      <c r="K70" s="71"/>
-      <c r="L70" s="71"/>
-      <c r="M70" s="72"/>
+      <c r="J70" s="75"/>
+      <c r="K70" s="76"/>
+      <c r="L70" s="76"/>
+      <c r="M70" s="77"/>
     </row>
     <row r="71" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J71" s="73"/>
-      <c r="K71" s="74"/>
-      <c r="L71" s="74"/>
-      <c r="M71" s="75"/>
+      <c r="J71" s="78"/>
+      <c r="K71" s="79"/>
+      <c r="L71" s="79"/>
+      <c r="M71" s="80"/>
     </row>
     <row r="72" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J72" s="76"/>
-      <c r="K72" s="77"/>
-      <c r="L72" s="77"/>
-      <c r="M72" s="78"/>
+      <c r="J72" s="81"/>
+      <c r="K72" s="82"/>
+      <c r="L72" s="82"/>
+      <c r="M72" s="83"/>
     </row>
     <row r="74" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J74" s="82" t="s">
-        <v>148</v>
-      </c>
-      <c r="K74" s="82"/>
-      <c r="L74" s="82"/>
-      <c r="M74" s="82"/>
+      <c r="J74" s="70" t="s">
+        <v>147</v>
+      </c>
+      <c r="K74" s="70"/>
+      <c r="L74" s="70"/>
+      <c r="M74" s="70"/>
     </row>
     <row r="75" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J75" s="54" t="s">
@@ -10589,23 +10589,23 @@
       <c r="J85" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K85" s="79" t="s">
+      <c r="K85" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="L85" s="80"/>
-      <c r="M85" s="81"/>
+      <c r="L85" s="72"/>
+      <c r="M85" s="73"/>
     </row>
     <row r="86" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J86" s="83" t="s">
+      <c r="J86" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K86" s="83"/>
-      <c r="L86" s="83"/>
-      <c r="M86" s="83"/>
+      <c r="K86" s="74"/>
+      <c r="L86" s="74"/>
+      <c r="M86" s="74"/>
     </row>
     <row r="87" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J87" s="87" t="s">
-        <v>150</v>
+      <c r="J87" s="84" t="s">
+        <v>149</v>
       </c>
       <c r="K87" s="89"/>
       <c r="L87" s="89"/>
@@ -10625,6 +10625,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J69:M69"/>
+    <mergeCell ref="J70:M72"/>
+    <mergeCell ref="K68:M68"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J19:M21"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J36:M38"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M55"/>
+    <mergeCell ref="K51:M51"/>
     <mergeCell ref="J74:M74"/>
     <mergeCell ref="K85:M85"/>
     <mergeCell ref="J86:M86"/>
@@ -10641,22 +10657,6 @@
     <mergeCell ref="P17:R17"/>
     <mergeCell ref="K34:M34"/>
     <mergeCell ref="P34:R34"/>
-    <mergeCell ref="J57:M57"/>
-    <mergeCell ref="J69:M69"/>
-    <mergeCell ref="J70:M72"/>
-    <mergeCell ref="K68:M68"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="J19:M21"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J36:M38"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M55"/>
-    <mergeCell ref="K51:M51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10681,13 +10681,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -10695,15 +10695,15 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="F4" s="88" t="s">
+      <c r="B4" s="85"/>
+      <c r="F4" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -10723,18 +10723,18 @@
       <c r="H6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="82" t="s">
+      <c r="J6" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="M6" s="82"/>
-      <c r="O6" s="82" t="s">
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="O6" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
@@ -11137,10 +11137,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="88"/>
+      <c r="B16" s="85"/>
       <c r="J16" s="56" t="s">
         <v>46</v>
       </c>
@@ -11175,31 +11175,31 @@
       <c r="J17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K17" s="79" t="s">
+      <c r="K17" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="L17" s="80"/>
-      <c r="M17" s="81"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="73"/>
       <c r="O17" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="P17" s="79"/>
-      <c r="Q17" s="80"/>
-      <c r="R17" s="81"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="73"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J18" s="83" t="s">
+      <c r="J18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="O18" s="83" t="s">
+      <c r="K18" s="74"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="74"/>
+      <c r="O18" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="83"/>
-      <c r="Q18" s="83"/>
-      <c r="R18" s="83"/>
+      <c r="P18" s="74"/>
+      <c r="Q18" s="74"/>
+      <c r="R18" s="74"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
@@ -11211,13 +11211,13 @@
       <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="J19" s="87" t="s">
+      <c r="J19" s="84" t="s">
         <v>75</v>
       </c>
       <c r="K19" s="89"/>
       <c r="L19" s="89"/>
       <c r="M19" s="90"/>
-      <c r="O19" s="87" t="s">
+      <c r="O19" s="84" t="s">
         <v>99</v>
       </c>
       <c r="P19" s="89"/>
@@ -11287,12 +11287,12 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="J23" s="82" t="s">
+      <c r="J23" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
+      <c r="K23" s="70"/>
+      <c r="L23" s="70"/>
+      <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
@@ -11478,22 +11478,22 @@
       <c r="J34" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K34" s="79" t="s">
+      <c r="K34" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="L34" s="80"/>
-      <c r="M34" s="81"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="73"/>
     </row>
     <row r="35" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J35" s="83" t="s">
+      <c r="J35" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="83"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="83"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="74"/>
     </row>
     <row r="36" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J36" s="87" t="s">
+      <c r="J36" s="84" t="s">
         <v>79</v>
       </c>
       <c r="K36" s="89"/>
@@ -11513,12 +11513,12 @@
       <c r="M38" s="96"/>
     </row>
     <row r="40" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J40" s="82" t="s">
+      <c r="J40" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="K40" s="82"/>
-      <c r="L40" s="82"/>
-      <c r="M40" s="82"/>
+      <c r="K40" s="70"/>
+      <c r="L40" s="70"/>
+      <c r="M40" s="70"/>
     </row>
     <row r="41" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J41" s="54" t="s">
@@ -11664,22 +11664,22 @@
       <c r="J51" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K51" s="79" t="s">
+      <c r="K51" s="71" t="s">
         <v>140</v>
       </c>
-      <c r="L51" s="80"/>
-      <c r="M51" s="81"/>
+      <c r="L51" s="72"/>
+      <c r="M51" s="73"/>
     </row>
     <row r="52" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J52" s="83" t="s">
+      <c r="J52" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="83"/>
-      <c r="L52" s="83"/>
-      <c r="M52" s="83"/>
+      <c r="K52" s="74"/>
+      <c r="L52" s="74"/>
+      <c r="M52" s="74"/>
     </row>
     <row r="53" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J53" s="87" t="s">
+      <c r="J53" s="84" t="s">
         <v>86</v>
       </c>
       <c r="K53" s="89"/>
@@ -11699,12 +11699,12 @@
       <c r="M55" s="96"/>
     </row>
     <row r="57" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J57" s="82" t="s">
+      <c r="J57" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="K57" s="82"/>
-      <c r="L57" s="82"/>
-      <c r="M57" s="82"/>
+      <c r="K57" s="70"/>
+      <c r="L57" s="70"/>
+      <c r="M57" s="70"/>
     </row>
     <row r="58" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J58" s="54" t="s">
@@ -11850,22 +11850,22 @@
       <c r="J68" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K68" s="79" t="s">
+      <c r="K68" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="L68" s="80"/>
-      <c r="M68" s="81"/>
+      <c r="L68" s="72"/>
+      <c r="M68" s="73"/>
     </row>
     <row r="69" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J69" s="83" t="s">
+      <c r="J69" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K69" s="83"/>
-      <c r="L69" s="83"/>
-      <c r="M69" s="83"/>
+      <c r="K69" s="74"/>
+      <c r="L69" s="74"/>
+      <c r="M69" s="74"/>
     </row>
     <row r="70" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J70" s="87" t="s">
+      <c r="J70" s="84" t="s">
         <v>101</v>
       </c>
       <c r="K70" s="89"/>
@@ -11885,12 +11885,12 @@
       <c r="M72" s="96"/>
     </row>
     <row r="74" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J74" s="82" t="s">
+      <c r="J74" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="K74" s="82"/>
-      <c r="L74" s="82"/>
-      <c r="M74" s="82"/>
+      <c r="K74" s="70"/>
+      <c r="L74" s="70"/>
+      <c r="M74" s="70"/>
     </row>
     <row r="75" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J75" s="54" t="s">
@@ -12036,22 +12036,22 @@
       <c r="J85" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K85" s="79" t="s">
+      <c r="K85" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="L85" s="80"/>
-      <c r="M85" s="81"/>
+      <c r="L85" s="72"/>
+      <c r="M85" s="73"/>
     </row>
     <row r="86" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J86" s="83" t="s">
+      <c r="J86" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K86" s="83"/>
-      <c r="L86" s="83"/>
-      <c r="M86" s="83"/>
+      <c r="K86" s="74"/>
+      <c r="L86" s="74"/>
+      <c r="M86" s="74"/>
     </row>
     <row r="87" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J87" s="87" t="s">
+      <c r="J87" s="84" t="s">
         <v>108</v>
       </c>
       <c r="K87" s="89"/>
@@ -12071,12 +12071,12 @@
       <c r="M89" s="96"/>
     </row>
     <row r="91" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J91" s="82" t="s">
-        <v>149</v>
-      </c>
-      <c r="K91" s="82"/>
-      <c r="L91" s="82"/>
-      <c r="M91" s="82"/>
+      <c r="J91" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="K91" s="70"/>
+      <c r="L91" s="70"/>
+      <c r="M91" s="70"/>
     </row>
     <row r="92" spans="10:13" x14ac:dyDescent="0.25">
       <c r="J92" s="54" t="s">
@@ -12222,23 +12222,23 @@
       <c r="J102" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="K102" s="79" t="s">
+      <c r="K102" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="L102" s="80"/>
-      <c r="M102" s="81"/>
+      <c r="L102" s="72"/>
+      <c r="M102" s="73"/>
     </row>
     <row r="103" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J103" s="83" t="s">
+      <c r="J103" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="K103" s="83"/>
-      <c r="L103" s="83"/>
-      <c r="M103" s="83"/>
+      <c r="K103" s="74"/>
+      <c r="L103" s="74"/>
+      <c r="M103" s="74"/>
     </row>
     <row r="104" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J104" s="87" t="s">
-        <v>150</v>
+      <c r="J104" s="84" t="s">
+        <v>149</v>
       </c>
       <c r="K104" s="89"/>
       <c r="L104" s="89"/>
@@ -12258,15 +12258,12 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="J91:M91"/>
-    <mergeCell ref="K102:M102"/>
-    <mergeCell ref="J103:M103"/>
-    <mergeCell ref="J104:M106"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="K85:M85"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M55"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K68:M68"/>
     <mergeCell ref="O6:R6"/>
     <mergeCell ref="O18:R18"/>
     <mergeCell ref="J19:M21"/>
@@ -12277,6 +12274,15 @@
     <mergeCell ref="K17:M17"/>
     <mergeCell ref="P17:R17"/>
     <mergeCell ref="K34:M34"/>
+    <mergeCell ref="J91:M91"/>
+    <mergeCell ref="K102:M102"/>
+    <mergeCell ref="J103:M103"/>
+    <mergeCell ref="J104:M106"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="J6:M6"/>
     <mergeCell ref="J36:M38"/>
     <mergeCell ref="J74:M74"/>
     <mergeCell ref="J86:M86"/>
@@ -12284,12 +12290,6 @@
     <mergeCell ref="J57:M57"/>
     <mergeCell ref="J69:M69"/>
     <mergeCell ref="J70:M72"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M55"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="K68:M68"/>
-    <mergeCell ref="K85:M85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>